<commit_message>
Soften borders on forms to light gray.
</commit_message>
<xml_diff>
--- a/post_season_inputs.xlsx
+++ b/post_season_inputs.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17030"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>VISITOR</t>
   </si>
@@ -52,16 +52,7 @@
     <t>Points:</t>
   </si>
   <si>
-    <t>at</t>
-  </si>
-  <si>
-    <t>Panthers</t>
-  </si>
-  <si>
-    <t>Broncos</t>
-  </si>
-  <si>
-    <t>Post Season Week 4 Input Form</t>
+    <t>Post Season Week 1 Input Form</t>
   </si>
 </sst>
 </file>
@@ -249,180 +240,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="hair">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color indexed="64"/>
-      </left>
-      <right style="hair">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="hair">
-        <color indexed="64"/>
-      </top>
-      <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="hair">
-        <color indexed="64"/>
-      </right>
-      <top style="hair">
-        <color indexed="64"/>
-      </top>
-      <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color indexed="64"/>
-      </left>
-      <right style="hair">
-        <color indexed="64"/>
-      </right>
-      <top style="hair">
-        <color indexed="64"/>
-      </top>
-      <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="hair">
-        <color indexed="64"/>
-      </top>
-      <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="hair">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="hair">
-        <color indexed="64"/>
-      </right>
-      <top style="hair">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color indexed="64"/>
-      </left>
-      <right style="hair">
-        <color indexed="64"/>
-      </right>
-      <top style="hair">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="hair">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top/>
       <bottom style="medium">
@@ -451,11 +268,195 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="hair">
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFD3D3D3"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFD3D3D3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFD3D3D3"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFD3D3D3"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFD3D3D3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFD3D3D3"/>
+      </left>
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFD3D3D3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFD3D3D3"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFD3D3D3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFD3D3D3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFD3D3D3"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFD3D3D3"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFD3D3D3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFD3D3D3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFD3D3D3"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFD3D3D3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFD3D3D3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFD3D3D3"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFD3D3D3"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFD3D3D3"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFD3D3D3"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFD3D3D3"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFD3D3D3"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFD3D3D3"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFD3D3D3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFD3D3D3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFD3D3D3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFD3D3D3"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFD3D3D3"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -562,18 +563,43 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -582,55 +608,30 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -705,6 +706,9 @@
       <rgbColor rgb="00333399"/>
       <rgbColor rgb="00333333"/>
     </indexedColors>
+    <mruColors>
+      <color rgb="FFD3D3D3"/>
+    </mruColors>
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1067,15 +1071,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:51" s="4" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="53" t="s">
-        <v>12</v>
+      <c r="B1" s="33" t="s">
+        <v>9</v>
       </c>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
       <c r="I1" s="1"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -1156,11 +1160,11 @@
       <c r="I3" s="5"/>
       <c r="AA3" s="1">
         <f ca="1">MIN(AA4:AA7)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AB3" s="1">
         <f ca="1">MIN(AB4:AB7)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AC3" s="1">
         <f ca="1">MIN(AC4:AC7)</f>
@@ -1168,37 +1172,31 @@
       </c>
     </row>
     <row r="4" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="30">
+      <c r="B4" s="49" t="str">
         <f ca="1">IF(ISTEXT($C4),ROW($B4)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B4)-ROW($B$4),0)),"")</f>
-        <v>1</v>
+        <v/>
       </c>
-      <c r="C4" s="31" t="s">
-        <v>10</v>
+      <c r="C4" s="43"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="35" t="str">
+        <f ca="1">IF(B4="","","by")</f>
+        <v/>
       </c>
-      <c r="D4" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="34"/>
-      <c r="G4" s="32" t="str">
-        <f ca="1">IF(B4="","","by")</f>
-        <v>by</v>
-      </c>
-      <c r="H4" s="35"/>
+      <c r="H4" s="36"/>
       <c r="I4" s="5"/>
       <c r="J4" s="6" t="str">
         <f>IF(ISNUMBER(SEARCH("Please assign a weight",$I$3)),$C$36,IF(ISNUMBER(SEARCH("You have assigned a weight of",$I$3)),"Each weight must be unique.  Please re-evaluate your assigned weights.",""))</f>
         <v/>
       </c>
-      <c r="AA4" s="1">
+      <c r="AA4" s="1" t="str">
         <f ca="1">IF($B4="","",IF(AND($F4&lt;&gt;"H",$F4&lt;&gt;"V"),ROW(),""))</f>
-        <v>4</v>
+        <v/>
       </c>
-      <c r="AB4" s="1">
+      <c r="AB4" s="1" t="str">
         <f ca="1">IF($B4="","",IF($H4&lt;1,ROW(),""))</f>
-        <v>4</v>
+        <v/>
       </c>
       <c r="AC4" s="1">
         <f>IF($AD4&lt;&gt;"",ROW(),"")</f>
@@ -1210,19 +1208,19 @@
       </c>
     </row>
     <row r="5" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="36" t="str">
+      <c r="B5" s="50" t="str">
         <f ca="1">IF(ISTEXT($C5),ROW($B5)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B5)-ROW($B$4),0)),"")</f>
         <v/>
       </c>
-      <c r="C5" s="37"/>
+      <c r="C5" s="45"/>
       <c r="D5" s="38"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="40"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="37"/>
       <c r="G5" s="38" t="str">
         <f ca="1">IF(B5="","","by")</f>
         <v/>
       </c>
-      <c r="H5" s="41"/>
+      <c r="H5" s="39"/>
       <c r="I5" s="5"/>
       <c r="J5" s="7" t="str">
         <f>IF(ISNUMBER(SEARCH("Each weight must be unique",$I$4)),$C$36,"")</f>
@@ -1236,29 +1234,29 @@
         <f ca="1">IF($B5="","",IF($H5&lt;1,ROW(),""))</f>
         <v/>
       </c>
-      <c r="AC5" s="1">
+      <c r="AC5" s="1" t="str">
         <f t="shared" ref="AC5:AC13" ca="1" si="0">IF($AD5&lt;&gt;"",ROW(),"")</f>
-        <v>5</v>
+        <v/>
       </c>
       <c r="AD5" s="3" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Please pick a winner (V or H) for the ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Please pick a winner (V or H) for the Panthers at Broncos (Game 1).</v>
+        <v/>
       </c>
     </row>
     <row r="6" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="36" t="str">
+      <c r="B6" s="50" t="str">
         <f ca="1">IF(ISTEXT($C6),ROW($B6)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B6)-ROW($B$4),0)),"")</f>
         <v/>
       </c>
-      <c r="C6" s="37"/>
+      <c r="C6" s="45"/>
       <c r="D6" s="38"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="40"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="37"/>
       <c r="G6" s="38" t="str">
         <f ca="1">IF(B6="","","by")</f>
         <v/>
       </c>
-      <c r="H6" s="41"/>
+      <c r="H6" s="39"/>
       <c r="I6" s="8"/>
       <c r="J6" s="9"/>
       <c r="AA6" s="1" t="str">
@@ -1269,29 +1267,29 @@
         <f ca="1">IF($B6="","",IF($H6&lt;1,ROW(),""))</f>
         <v/>
       </c>
-      <c r="AC6" s="1">
+      <c r="AC6" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v/>
       </c>
       <c r="AD6" s="3" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE("Please enter the predicted margin of victory for the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Please enter the predicted margin of victory for the Broncos (Game 1).</v>
+        <v/>
       </c>
     </row>
     <row r="7" spans="2:51" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="42" t="str">
+      <c r="B7" s="51" t="str">
         <f ca="1">IF(ISTEXT($C7),ROW($B7)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B7)-ROW($B$4),0)),"")</f>
         <v/>
       </c>
-      <c r="C7" s="43"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="44" t="str">
+      <c r="C7" s="47"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="41" t="str">
         <f ca="1">IF(B7="","","by")</f>
         <v/>
       </c>
-      <c r="H7" s="47"/>
+      <c r="H7" s="42"/>
       <c r="I7" s="8"/>
       <c r="J7" s="9"/>
       <c r="AA7" s="1" t="str">
@@ -1308,22 +1306,22 @@
       </c>
       <c r="AD7" s="3" t="str">
         <f ca="1">IF($H$8="",CONCATENATE("Please enter your Total Points Prediction for ",OFFSET($C$4,MAX($B4:$B7)-1,0)," at ",OFFSET($E$4,MAX($B4:$B7)-1,0)," (Game ",OFFSET($B$4,MAX($B4:$B7)-1,0),") in cell H8"),"")</f>
-        <v>Please enter your Total Points Prediction for Panthers at Broncos (Game 1) in cell H8</v>
+        <v>Please enter your Total Points Prediction for VISITOR at HOME (Game GAME) in cell H8</v>
       </c>
     </row>
     <row r="8" spans="2:51" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="48"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="50" t="str">
+      <c r="B8" s="30"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="32" t="str">
         <f ca="1">CONCATENATE("                   Game ",MAX(B4:B7)," Total")</f>
-        <v xml:space="preserve">                   Game 1 Total</v>
+        <v xml:space="preserve">                   Game 0 Total</v>
       </c>
-      <c r="F8" s="49"/>
-      <c r="G8" s="51" t="s">
+      <c r="F8" s="31"/>
+      <c r="G8" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="52"/>
+      <c r="H8" s="53"/>
       <c r="I8" s="8"/>
       <c r="J8" s="9"/>
     </row>
@@ -8725,7 +8723,6 @@
       <c r="AY181" s="14"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <sheetProtection sheet="1"/>
   <mergeCells count="1">
     <mergeCell ref="B1:H1"/>

</xml_diff>

<commit_message>
Soften borders on tables.
</commit_message>
<xml_diff>
--- a/post_season_inputs.xlsx
+++ b/post_season_inputs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="9420" windowHeight="4500" tabRatio="375"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="9420" windowHeight="4500" tabRatio="314"/>
   </bookViews>
   <sheets>
     <sheet name="Post Season Input Form" sheetId="1" r:id="rId1"/>
@@ -563,9 +563,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -632,6 +629,9 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1071,15 +1071,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:51" s="4" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
       <c r="I1" s="1"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -1172,19 +1172,19 @@
       </c>
     </row>
     <row r="4" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="49" t="str">
+      <c r="B4" s="48" t="str">
         <f ca="1">IF(ISTEXT($C4),ROW($B4)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B4)-ROW($B$4),0)),"")</f>
         <v/>
       </c>
-      <c r="C4" s="43"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="35" t="str">
+      <c r="C4" s="42"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="34" t="str">
         <f ca="1">IF(B4="","","by")</f>
         <v/>
       </c>
-      <c r="H4" s="36"/>
+      <c r="H4" s="35"/>
       <c r="I4" s="5"/>
       <c r="J4" s="6" t="str">
         <f>IF(ISNUMBER(SEARCH("Please assign a weight",$I$3)),$C$36,IF(ISNUMBER(SEARCH("You have assigned a weight of",$I$3)),"Each weight must be unique.  Please re-evaluate your assigned weights.",""))</f>
@@ -1208,19 +1208,19 @@
       </c>
     </row>
     <row r="5" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="50" t="str">
+      <c r="B5" s="49" t="str">
         <f ca="1">IF(ISTEXT($C5),ROW($B5)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B5)-ROW($B$4),0)),"")</f>
         <v/>
       </c>
-      <c r="C5" s="45"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="38" t="str">
+      <c r="C5" s="44"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="37" t="str">
         <f ca="1">IF(B5="","","by")</f>
         <v/>
       </c>
-      <c r="H5" s="39"/>
+      <c r="H5" s="38"/>
       <c r="I5" s="5"/>
       <c r="J5" s="7" t="str">
         <f>IF(ISNUMBER(SEARCH("Each weight must be unique",$I$4)),$C$36,"")</f>
@@ -1244,19 +1244,19 @@
       </c>
     </row>
     <row r="6" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="50" t="str">
+      <c r="B6" s="49" t="str">
         <f ca="1">IF(ISTEXT($C6),ROW($B6)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B6)-ROW($B$4),0)),"")</f>
         <v/>
       </c>
-      <c r="C6" s="45"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="38" t="str">
+      <c r="C6" s="44"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="37" t="str">
         <f ca="1">IF(B6="","","by")</f>
         <v/>
       </c>
-      <c r="H6" s="39"/>
+      <c r="H6" s="38"/>
       <c r="I6" s="8"/>
       <c r="J6" s="9"/>
       <c r="AA6" s="1" t="str">
@@ -1277,19 +1277,19 @@
       </c>
     </row>
     <row r="7" spans="2:51" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="51" t="str">
+      <c r="B7" s="50" t="str">
         <f ca="1">IF(ISTEXT($C7),ROW($B7)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B7)-ROW($B$4),0)),"")</f>
         <v/>
       </c>
-      <c r="C7" s="47"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="48"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="41" t="str">
+      <c r="C7" s="46"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="40" t="str">
         <f ca="1">IF(B7="","","by")</f>
         <v/>
       </c>
-      <c r="H7" s="42"/>
+      <c r="H7" s="41"/>
       <c r="I7" s="8"/>
       <c r="J7" s="9"/>
       <c r="AA7" s="1" t="str">
@@ -1318,10 +1318,10 @@
         <v xml:space="preserve">                   Game 0 Total</v>
       </c>
       <c r="F8" s="31"/>
-      <c r="G8" s="52" t="s">
+      <c r="G8" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="53"/>
+      <c r="H8" s="52"/>
       <c r="I8" s="8"/>
       <c r="J8" s="9"/>
     </row>

</xml_diff>

<commit_message>
2016 Week 17 Final update.
</commit_message>
<xml_diff>
--- a/post_season_inputs.xlsx
+++ b/post_season_inputs.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jerry\Desktop\2016 Football Pool Page\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2016 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>VISITOR</t>
   </si>
@@ -53,6 +53,33 @@
   </si>
   <si>
     <t>Post Season Week 1 Input Form</t>
+  </si>
+  <si>
+    <t>Raiders</t>
+  </si>
+  <si>
+    <t>at</t>
+  </si>
+  <si>
+    <t>Texans</t>
+  </si>
+  <si>
+    <t>Lions</t>
+  </si>
+  <si>
+    <t>Seahawks</t>
+  </si>
+  <si>
+    <t>Dolphins</t>
+  </si>
+  <si>
+    <t>Steelers</t>
+  </si>
+  <si>
+    <t>Giants</t>
+  </si>
+  <si>
+    <t>Packers</t>
   </si>
 </sst>
 </file>
@@ -625,9 +652,6 @@
     <xf numFmtId="1" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -635,6 +659,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1074,59 +1101,59 @@
     <col min="53" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:51" s="54" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="51" t="s">
+    <row r="1" spans="2:51" s="53" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="52"/>
-      <c r="M1" s="52"/>
-      <c r="N1" s="52"/>
-      <c r="O1" s="52"/>
-      <c r="P1" s="52"/>
-      <c r="Q1" s="52"/>
-      <c r="R1" s="52"/>
-      <c r="S1" s="52"/>
-      <c r="T1" s="52"/>
-      <c r="U1" s="52"/>
-      <c r="V1" s="52"/>
-      <c r="W1" s="52"/>
-      <c r="X1" s="52"/>
-      <c r="Y1" s="52"/>
-      <c r="Z1" s="52"/>
-      <c r="AA1" s="52"/>
-      <c r="AB1" s="52"/>
-      <c r="AC1" s="52"/>
-      <c r="AD1" s="53"/>
-      <c r="AE1" s="52"/>
-      <c r="AF1" s="52"/>
-      <c r="AG1" s="52"/>
-      <c r="AH1" s="52"/>
-      <c r="AI1" s="52"/>
-      <c r="AJ1" s="52"/>
-      <c r="AK1" s="52"/>
-      <c r="AL1" s="52"/>
-      <c r="AM1" s="52"/>
-      <c r="AN1" s="52"/>
-      <c r="AO1" s="53"/>
-      <c r="AP1" s="52"/>
-      <c r="AQ1" s="52"/>
-      <c r="AR1" s="52"/>
-      <c r="AS1" s="52"/>
-      <c r="AT1" s="52"/>
-      <c r="AU1" s="52"/>
-      <c r="AV1" s="52"/>
-      <c r="AW1" s="52"/>
-      <c r="AX1" s="52"/>
-      <c r="AY1" s="52"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="51"/>
+      <c r="L1" s="51"/>
+      <c r="M1" s="51"/>
+      <c r="N1" s="51"/>
+      <c r="O1" s="51"/>
+      <c r="P1" s="51"/>
+      <c r="Q1" s="51"/>
+      <c r="R1" s="51"/>
+      <c r="S1" s="51"/>
+      <c r="T1" s="51"/>
+      <c r="U1" s="51"/>
+      <c r="V1" s="51"/>
+      <c r="W1" s="51"/>
+      <c r="X1" s="51"/>
+      <c r="Y1" s="51"/>
+      <c r="Z1" s="51"/>
+      <c r="AA1" s="51"/>
+      <c r="AB1" s="51"/>
+      <c r="AC1" s="51"/>
+      <c r="AD1" s="52"/>
+      <c r="AE1" s="51"/>
+      <c r="AF1" s="51"/>
+      <c r="AG1" s="51"/>
+      <c r="AH1" s="51"/>
+      <c r="AI1" s="51"/>
+      <c r="AJ1" s="51"/>
+      <c r="AK1" s="51"/>
+      <c r="AL1" s="51"/>
+      <c r="AM1" s="51"/>
+      <c r="AN1" s="51"/>
+      <c r="AO1" s="52"/>
+      <c r="AP1" s="51"/>
+      <c r="AQ1" s="51"/>
+      <c r="AR1" s="51"/>
+      <c r="AS1" s="51"/>
+      <c r="AT1" s="51"/>
+      <c r="AU1" s="51"/>
+      <c r="AV1" s="51"/>
+      <c r="AW1" s="51"/>
+      <c r="AX1" s="51"/>
+      <c r="AY1" s="51"/>
     </row>
     <row r="2" spans="2:51" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="39"/>
@@ -1164,11 +1191,11 @@
       <c r="I3" s="3"/>
       <c r="AA3" s="1">
         <f ca="1">MIN(AA4:AA7)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AB3" s="1">
         <f ca="1">MIN(AB4:AB7)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AC3" s="1">
         <f ca="1">MIN(AC4:AC7)</f>
@@ -1176,17 +1203,23 @@
       </c>
     </row>
     <row r="4" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="34" t="str">
+      <c r="B4" s="34">
         <f ca="1">IF(ISTEXT($C4),ROW($B4)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B4)-ROW($B$4),0)),"")</f>
-        <v/>
-      </c>
-      <c r="C4" s="28"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="29"/>
+        <v>1</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="29" t="s">
+        <v>12</v>
+      </c>
       <c r="F4" s="19"/>
       <c r="G4" s="20" t="str">
         <f ca="1">IF(B4="","","by")</f>
-        <v/>
+        <v>by</v>
       </c>
       <c r="H4" s="21"/>
       <c r="I4" s="3"/>
@@ -1194,13 +1227,13 @@
         <f>IF(ISNUMBER(SEARCH("Please assign a weight",$I$3)),$C$36,IF(ISNUMBER(SEARCH("You have assigned a weight of",$I$3)),"Each weight must be unique.  Please re-evaluate your assigned weights.",""))</f>
         <v/>
       </c>
-      <c r="AA4" s="1" t="str">
+      <c r="AA4" s="1">
         <f ca="1">IF($B4="","",IF(AND($F4&lt;&gt;"H",$F4&lt;&gt;"V"),ROW(),""))</f>
-        <v/>
-      </c>
-      <c r="AB4" s="1" t="str">
+        <v>4</v>
+      </c>
+      <c r="AB4" s="1">
         <f ca="1">IF($B4="","",IF($H4&lt;1,ROW(),""))</f>
-        <v/>
+        <v>4</v>
       </c>
       <c r="AC4" s="1">
         <f>IF($AD4&lt;&gt;"",ROW(),"")</f>
@@ -1212,17 +1245,23 @@
       </c>
     </row>
     <row r="5" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="35" t="str">
+      <c r="B5" s="35">
         <f ca="1">IF(ISTEXT($C5),ROW($B5)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B5)-ROW($B$4),0)),"")</f>
-        <v/>
-      </c>
-      <c r="C5" s="30"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="31"/>
+        <v>2</v>
+      </c>
+      <c r="C5" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="31" t="s">
+        <v>14</v>
+      </c>
       <c r="F5" s="22"/>
       <c r="G5" s="23" t="str">
         <f ca="1">IF(B5="","","by")</f>
-        <v/>
+        <v>by</v>
       </c>
       <c r="H5" s="24"/>
       <c r="I5" s="3"/>
@@ -1230,79 +1269,91 @@
         <f>IF(ISNUMBER(SEARCH("Each weight must be unique",$I$4)),$C$36,"")</f>
         <v/>
       </c>
-      <c r="AA5" s="1" t="str">
+      <c r="AA5" s="1">
         <f ca="1">IF($B5="","",IF(AND($F5&lt;&gt;"H",$F5&lt;&gt;"V"),ROW(),""))</f>
-        <v/>
-      </c>
-      <c r="AB5" s="1" t="str">
+        <v>5</v>
+      </c>
+      <c r="AB5" s="1">
         <f ca="1">IF($B5="","",IF($H5&lt;1,ROW(),""))</f>
-        <v/>
-      </c>
-      <c r="AC5" s="1" t="str">
+        <v>5</v>
+      </c>
+      <c r="AC5" s="1">
         <f t="shared" ref="AC5:AC13" ca="1" si="0">IF($AD5&lt;&gt;"",ROW(),"")</f>
-        <v/>
+        <v>5</v>
       </c>
       <c r="AD5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Please pick a winner (V or H) for the ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v/>
+        <v>Please pick a winner (V or H) for the Raiders at Texans (Game 1).</v>
       </c>
     </row>
     <row r="6" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="35" t="str">
+      <c r="B6" s="35">
         <f ca="1">IF(ISTEXT($C6),ROW($B6)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B6)-ROW($B$4),0)),"")</f>
-        <v/>
-      </c>
-      <c r="C6" s="30"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="31"/>
+        <v>3</v>
+      </c>
+      <c r="C6" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="31" t="s">
+        <v>16</v>
+      </c>
       <c r="F6" s="22"/>
       <c r="G6" s="23" t="str">
         <f ca="1">IF(B6="","","by")</f>
-        <v/>
+        <v>by</v>
       </c>
       <c r="H6" s="24"/>
       <c r="I6" s="6"/>
       <c r="J6" s="7"/>
-      <c r="AA6" s="1" t="str">
+      <c r="AA6" s="1">
         <f ca="1">IF($B6="","",IF(AND($F6&lt;&gt;"H",$F6&lt;&gt;"V"),ROW(),""))</f>
-        <v/>
-      </c>
-      <c r="AB6" s="1" t="str">
+        <v>6</v>
+      </c>
+      <c r="AB6" s="1">
         <f ca="1">IF($B6="","",IF($H6&lt;1,ROW(),""))</f>
-        <v/>
-      </c>
-      <c r="AC6" s="1" t="str">
+        <v>6</v>
+      </c>
+      <c r="AC6" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v>6</v>
       </c>
       <c r="AD6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE("Please enter the predicted margin of victory for the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v/>
+        <v>Please enter the predicted margin of victory for the Texans (Game 1).</v>
       </c>
     </row>
     <row r="7" spans="2:51" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="36" t="str">
+      <c r="B7" s="36">
         <f ca="1">IF(ISTEXT($C7),ROW($B7)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B7)-ROW($B$4),0)),"")</f>
-        <v/>
-      </c>
-      <c r="C7" s="32"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="33"/>
+        <v>4</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="33" t="s">
+        <v>18</v>
+      </c>
       <c r="F7" s="25"/>
       <c r="G7" s="26" t="str">
         <f ca="1">IF(B7="","","by")</f>
-        <v/>
+        <v>by</v>
       </c>
       <c r="H7" s="27"/>
       <c r="I7" s="6"/>
       <c r="J7" s="7"/>
-      <c r="AA7" s="1" t="str">
+      <c r="AA7" s="1">
         <f ca="1">IF($B7="","",IF(AND($F7&lt;&gt;"H",$F7&lt;&gt;"V"),ROW(),""))</f>
-        <v/>
-      </c>
-      <c r="AB7" s="1" t="str">
+        <v>7</v>
+      </c>
+      <c r="AB7" s="1">
         <f ca="1">IF($B7="","",IF($H7&lt;1,ROW(),""))</f>
-        <v/>
+        <v>7</v>
       </c>
       <c r="AC7" s="1">
         <f ca="1">IF($AD7&lt;&gt;"",ROW(),"")</f>
@@ -1310,7 +1361,7 @@
       </c>
       <c r="AD7" s="2" t="str">
         <f ca="1">IF($H$8="",CONCATENATE("Please enter your Total Points Prediction for ",OFFSET($C$4,MAX($B4:$B7)-1,0)," at ",OFFSET($E$4,MAX($B4:$B7)-1,0)," (Game ",OFFSET($B$4,MAX($B4:$B7)-1,0),") in cell H8"),"")</f>
-        <v>Please enter your Total Points Prediction for VISITOR at HOME (Game GAME) in cell H8</v>
+        <v>Please enter your Total Points Prediction for Giants at Packers (Game 4) in cell H8</v>
       </c>
     </row>
     <row r="8" spans="2:51" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1319,7 +1370,7 @@
       <c r="D8" s="17"/>
       <c r="E8" s="18" t="str">
         <f ca="1">CONCATENATE("                   Game ",MAX(B4:B7)," Total")</f>
-        <v xml:space="preserve">                   Game 0 Total</v>
+        <v xml:space="preserve">                   Game 4 Total</v>
       </c>
       <c r="F8" s="17"/>
       <c r="G8" s="37" t="s">

</xml_diff>

<commit_message>
2016 Week 18 Final update.
</commit_message>
<xml_diff>
--- a/post_season_inputs.xlsx
+++ b/post_season_inputs.xlsx
@@ -52,34 +52,34 @@
     <t>Points:</t>
   </si>
   <si>
-    <t>Post Season Week 1 Input Form</t>
-  </si>
-  <si>
-    <t>Raiders</t>
-  </si>
-  <si>
     <t>at</t>
   </si>
   <si>
     <t>Texans</t>
   </si>
   <si>
-    <t>Lions</t>
-  </si>
-  <si>
     <t>Seahawks</t>
-  </si>
-  <si>
-    <t>Dolphins</t>
   </si>
   <si>
     <t>Steelers</t>
   </si>
   <si>
-    <t>Giants</t>
+    <t>Packers</t>
   </si>
   <si>
-    <t>Packers</t>
+    <t>Falcons</t>
+  </si>
+  <si>
+    <t>Patriots</t>
+  </si>
+  <si>
+    <t>Chiefs</t>
+  </si>
+  <si>
+    <t>Cowboys</t>
+  </si>
+  <si>
+    <t>Post Season Week 2 Input Form</t>
   </si>
 </sst>
 </file>
@@ -1103,7 +1103,7 @@
   <sheetData>
     <row r="1" spans="2:51" s="53" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="54" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C1" s="54"/>
       <c r="D1" s="54"/>
@@ -1208,13 +1208,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F4" s="19"/>
       <c r="G4" s="20" t="str">
@@ -1250,13 +1250,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E5" s="31" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F5" s="22"/>
       <c r="G5" s="23" t="str">
@@ -1283,7 +1283,7 @@
       </c>
       <c r="AD5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Please pick a winner (V or H) for the ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Please pick a winner (V or H) for the Raiders at Texans (Game 1).</v>
+        <v>Please pick a winner (V or H) for the Seahawks at Falcons (Game 1).</v>
       </c>
     </row>
     <row r="6" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -1292,10 +1292,10 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E6" s="31" t="s">
         <v>16</v>
@@ -1322,7 +1322,7 @@
       </c>
       <c r="AD6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE("Please enter the predicted margin of victory for the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Please enter the predicted margin of victory for the Texans (Game 1).</v>
+        <v>Please enter the predicted margin of victory for the Falcons (Game 1).</v>
       </c>
     </row>
     <row r="7" spans="2:51" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1331,13 +1331,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="33" t="s">
         <v>17</v>
-      </c>
-      <c r="D7" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="33" t="s">
-        <v>18</v>
       </c>
       <c r="F7" s="25"/>
       <c r="G7" s="26" t="str">
@@ -1361,7 +1361,7 @@
       </c>
       <c r="AD7" s="2" t="str">
         <f ca="1">IF($H$8="",CONCATENATE("Please enter your Total Points Prediction for ",OFFSET($C$4,MAX($B4:$B7)-1,0)," at ",OFFSET($E$4,MAX($B4:$B7)-1,0)," (Game ",OFFSET($B$4,MAX($B4:$B7)-1,0),") in cell H8"),"")</f>
-        <v>Please enter your Total Points Prediction for Giants at Packers (Game 4) in cell H8</v>
+        <v>Please enter your Total Points Prediction for Packers at Cowboys (Game 4) in cell H8</v>
       </c>
     </row>
     <row r="8" spans="2:51" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
2016 Week 19 Final update.
</commit_message>
<xml_diff>
--- a/post_season_inputs.xlsx
+++ b/post_season_inputs.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>VISITOR</t>
   </si>
@@ -55,12 +55,6 @@
     <t>at</t>
   </si>
   <si>
-    <t>Texans</t>
-  </si>
-  <si>
-    <t>Seahawks</t>
-  </si>
-  <si>
     <t>Steelers</t>
   </si>
   <si>
@@ -73,13 +67,7 @@
     <t>Patriots</t>
   </si>
   <si>
-    <t>Chiefs</t>
-  </si>
-  <si>
-    <t>Cowboys</t>
-  </si>
-  <si>
-    <t>Post Season Week 2 Input Form</t>
+    <t>Post Season Week 3 Input Form</t>
   </si>
 </sst>
 </file>
@@ -1103,7 +1091,7 @@
   <sheetData>
     <row r="1" spans="2:51" s="53" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="54" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C1" s="54"/>
       <c r="D1" s="54"/>
@@ -1214,7 +1202,7 @@
         <v>9</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F4" s="19"/>
       <c r="G4" s="20" t="str">
@@ -1256,7 +1244,7 @@
         <v>9</v>
       </c>
       <c r="E5" s="31" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F5" s="22"/>
       <c r="G5" s="23" t="str">
@@ -1283,38 +1271,32 @@
       </c>
       <c r="AD5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Please pick a winner (V or H) for the ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Please pick a winner (V or H) for the Seahawks at Falcons (Game 1).</v>
+        <v>Please pick a winner (V or H) for the Packers at Falcons (Game 1).</v>
       </c>
     </row>
     <row r="6" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="35">
+      <c r="B6" s="35" t="str">
         <f ca="1">IF(ISTEXT($C6),ROW($B6)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B6)-ROW($B$4),0)),"")</f>
-        <v>3</v>
-      </c>
-      <c r="C6" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="31" t="s">
-        <v>16</v>
-      </c>
+        <v/>
+      </c>
+      <c r="C6" s="30"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="31"/>
       <c r="F6" s="22"/>
       <c r="G6" s="23" t="str">
         <f ca="1">IF(B6="","","by")</f>
-        <v>by</v>
+        <v/>
       </c>
       <c r="H6" s="24"/>
       <c r="I6" s="6"/>
       <c r="J6" s="7"/>
-      <c r="AA6" s="1">
+      <c r="AA6" s="1" t="str">
         <f ca="1">IF($B6="","",IF(AND($F6&lt;&gt;"H",$F6&lt;&gt;"V"),ROW(),""))</f>
-        <v>6</v>
-      </c>
-      <c r="AB6" s="1">
+        <v/>
+      </c>
+      <c r="AB6" s="1" t="str">
         <f ca="1">IF($B6="","",IF($H6&lt;1,ROW(),""))</f>
-        <v>6</v>
+        <v/>
       </c>
       <c r="AC6" s="1">
         <f t="shared" ca="1" si="0"/>
@@ -1326,34 +1308,28 @@
       </c>
     </row>
     <row r="7" spans="2:51" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="36">
+      <c r="B7" s="36" t="str">
         <f ca="1">IF(ISTEXT($C7),ROW($B7)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B7)-ROW($B$4),0)),"")</f>
-        <v>4</v>
-      </c>
-      <c r="C7" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="33" t="s">
-        <v>17</v>
-      </c>
+        <v/>
+      </c>
+      <c r="C7" s="32"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="33"/>
       <c r="F7" s="25"/>
       <c r="G7" s="26" t="str">
         <f ca="1">IF(B7="","","by")</f>
-        <v>by</v>
+        <v/>
       </c>
       <c r="H7" s="27"/>
       <c r="I7" s="6"/>
       <c r="J7" s="7"/>
-      <c r="AA7" s="1">
+      <c r="AA7" s="1" t="str">
         <f ca="1">IF($B7="","",IF(AND($F7&lt;&gt;"H",$F7&lt;&gt;"V"),ROW(),""))</f>
-        <v>7</v>
-      </c>
-      <c r="AB7" s="1">
+        <v/>
+      </c>
+      <c r="AB7" s="1" t="str">
         <f ca="1">IF($B7="","",IF($H7&lt;1,ROW(),""))</f>
-        <v>7</v>
+        <v/>
       </c>
       <c r="AC7" s="1">
         <f ca="1">IF($AD7&lt;&gt;"",ROW(),"")</f>
@@ -1361,7 +1337,7 @@
       </c>
       <c r="AD7" s="2" t="str">
         <f ca="1">IF($H$8="",CONCATENATE("Please enter your Total Points Prediction for ",OFFSET($C$4,MAX($B4:$B7)-1,0)," at ",OFFSET($E$4,MAX($B4:$B7)-1,0)," (Game ",OFFSET($B$4,MAX($B4:$B7)-1,0),") in cell H8"),"")</f>
-        <v>Please enter your Total Points Prediction for Packers at Cowboys (Game 4) in cell H8</v>
+        <v>Please enter your Total Points Prediction for Steelers at Patriots (Game 2) in cell H8</v>
       </c>
     </row>
     <row r="8" spans="2:51" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1370,7 +1346,7 @@
       <c r="D8" s="17"/>
       <c r="E8" s="18" t="str">
         <f ca="1">CONCATENATE("                   Game ",MAX(B4:B7)," Total")</f>
-        <v xml:space="preserve">                   Game 4 Total</v>
+        <v xml:space="preserve">                   Game 2 Total</v>
       </c>
       <c r="F8" s="17"/>
       <c r="G8" s="37" t="s">

</xml_diff>

<commit_message>
2016 Week 20 Final update.
</commit_message>
<xml_diff>
--- a/post_season_inputs.xlsx
+++ b/post_season_inputs.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>VISITOR</t>
   </si>
@@ -55,19 +55,13 @@
     <t>at</t>
   </si>
   <si>
-    <t>Steelers</t>
-  </si>
-  <si>
-    <t>Packers</t>
-  </si>
-  <si>
     <t>Falcons</t>
   </si>
   <si>
     <t>Patriots</t>
   </si>
   <si>
-    <t>Post Season Week 3 Input Form</t>
+    <t>Post Season Week 4 Input Form</t>
   </si>
 </sst>
 </file>
@@ -1091,7 +1085,7 @@
   <sheetData>
     <row r="1" spans="2:51" s="53" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="54" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C1" s="54"/>
       <c r="D1" s="54"/>
@@ -1202,7 +1196,7 @@
         <v>9</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F4" s="19"/>
       <c r="G4" s="20" t="str">
@@ -1233,23 +1227,17 @@
       </c>
     </row>
     <row r="5" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="35">
+      <c r="B5" s="35" t="str">
         <f ca="1">IF(ISTEXT($C5),ROW($B5)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B5)-ROW($B$4),0)),"")</f>
-        <v>2</v>
+        <v/>
       </c>
-      <c r="C5" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="31" t="s">
-        <v>13</v>
-      </c>
+      <c r="C5" s="30"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="31"/>
       <c r="F5" s="22"/>
       <c r="G5" s="23" t="str">
         <f ca="1">IF(B5="","","by")</f>
-        <v>by</v>
+        <v/>
       </c>
       <c r="H5" s="24"/>
       <c r="I5" s="3"/>
@@ -1257,13 +1245,13 @@
         <f>IF(ISNUMBER(SEARCH("Each weight must be unique",$I$4)),$C$36,"")</f>
         <v/>
       </c>
-      <c r="AA5" s="1">
+      <c r="AA5" s="1" t="str">
         <f ca="1">IF($B5="","",IF(AND($F5&lt;&gt;"H",$F5&lt;&gt;"V"),ROW(),""))</f>
-        <v>5</v>
+        <v/>
       </c>
-      <c r="AB5" s="1">
+      <c r="AB5" s="1" t="str">
         <f ca="1">IF($B5="","",IF($H5&lt;1,ROW(),""))</f>
-        <v>5</v>
+        <v/>
       </c>
       <c r="AC5" s="1">
         <f t="shared" ref="AC5:AC13" ca="1" si="0">IF($AD5&lt;&gt;"",ROW(),"")</f>
@@ -1271,7 +1259,7 @@
       </c>
       <c r="AD5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Please pick a winner (V or H) for the ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Please pick a winner (V or H) for the Packers at Falcons (Game 1).</v>
+        <v>Please pick a winner (V or H) for the Patriots at Falcons (Game 1).</v>
       </c>
     </row>
     <row r="6" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -1337,7 +1325,7 @@
       </c>
       <c r="AD7" s="2" t="str">
         <f ca="1">IF($H$8="",CONCATENATE("Please enter your Total Points Prediction for ",OFFSET($C$4,MAX($B4:$B7)-1,0)," at ",OFFSET($E$4,MAX($B4:$B7)-1,0)," (Game ",OFFSET($B$4,MAX($B4:$B7)-1,0),") in cell H8"),"")</f>
-        <v>Please enter your Total Points Prediction for Steelers at Patriots (Game 2) in cell H8</v>
+        <v>Please enter your Total Points Prediction for Patriots at Falcons (Game 1) in cell H8</v>
       </c>
     </row>
     <row r="8" spans="2:51" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1346,7 +1334,7 @@
       <c r="D8" s="17"/>
       <c r="E8" s="18" t="str">
         <f ca="1">CONCATENATE("                   Game ",MAX(B4:B7)," Total")</f>
-        <v xml:space="preserve">                   Game 2 Total</v>
+        <v xml:space="preserve">                   Game 1 Total</v>
       </c>
       <c r="F8" s="17"/>
       <c r="G8" s="37" t="s">

</xml_diff>

<commit_message>
2017 Week 12 Final update.
</commit_message>
<xml_diff>
--- a/post_season_inputs.xlsx
+++ b/post_season_inputs.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jerry\Desktop\Test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Spreadsheets\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>H</t>
   </si>
@@ -35,9 +35,6 @@
   </si>
   <si>
     <t>Points:</t>
-  </si>
-  <si>
-    <t>at</t>
   </si>
   <si>
     <t>Raiders</t>
@@ -1088,7 +1085,7 @@
   <sheetData>
     <row r="1" spans="2:51" s="52" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="53" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C1" s="53"/>
       <c r="D1" s="53"/>
@@ -1143,7 +1140,7 @@
     <row r="2" spans="2:51" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="39"/>
       <c r="C2" s="40" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2" s="41"/>
       <c r="E2" s="42"/>
@@ -1159,20 +1156,20 @@
     </row>
     <row r="3" spans="2:51" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="45" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="46" t="s">
+      <c r="D3" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="47" t="s">
+      <c r="E3" s="48" t="s">
         <v>16</v>
-      </c>
-      <c r="E3" s="48" t="s">
-        <v>17</v>
       </c>
       <c r="F3" s="46"/>
       <c r="G3" s="47" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H3" s="49"/>
       <c r="I3" s="3"/>
@@ -1195,13 +1192,14 @@
         <v>1</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="20" t="s">
         <v>4</v>
       </c>
+      <c r="D4" s="20" t="str">
+        <f ca="1">IF(B4="","","at")</f>
+        <v>at</v>
+      </c>
       <c r="E4" s="29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F4" s="19"/>
       <c r="G4" s="20" t="str">
@@ -1234,13 +1232,14 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
-      <c r="D5" s="23" t="s">
-        <v>4</v>
+      <c r="D5" s="23" t="str">
+        <f t="shared" ref="D5:D7" ca="1" si="0">IF(B5="","","at")</f>
+        <v>at</v>
       </c>
       <c r="E5" s="31" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F5" s="22"/>
       <c r="G5" s="23" t="str">
@@ -1259,7 +1258,7 @@
         <v>5</v>
       </c>
       <c r="AC5" s="1">
-        <f t="shared" ref="AC5:AC13" ca="1" si="0">IF($AD5&lt;&gt;"",ROW(),"")</f>
+        <f t="shared" ref="AC5:AC13" ca="1" si="1">IF($AD5&lt;&gt;"",ROW(),"")</f>
         <v>5</v>
       </c>
       <c r="AD5" s="2" t="str">
@@ -1273,13 +1272,14 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
-      <c r="D6" s="23" t="s">
-        <v>4</v>
+      <c r="D6" s="23" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>at</v>
       </c>
       <c r="E6" s="31" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F6" s="22"/>
       <c r="G6" s="23" t="str">
@@ -1298,7 +1298,7 @@
         <v>6</v>
       </c>
       <c r="AC6" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>6</v>
       </c>
       <c r="AD6" s="2" t="str">
@@ -1312,13 +1312,14 @@
         <v>4</v>
       </c>
       <c r="C7" s="32" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
-      <c r="D7" s="26" t="s">
-        <v>4</v>
+      <c r="D7" s="26" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>at</v>
       </c>
       <c r="E7" s="33" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" s="25"/>
       <c r="G7" s="26" t="str">
@@ -1384,7 +1385,7 @@
       <c r="AA9" s="1"/>
       <c r="AB9" s="1"/>
       <c r="AC9" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="AD9" s="2"/>
@@ -1439,7 +1440,7 @@
       <c r="AA10" s="1"/>
       <c r="AB10" s="1"/>
       <c r="AC10" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="AD10" s="2"/>
@@ -1491,7 +1492,7 @@
       <c r="AA11" s="1"/>
       <c r="AB11" s="1"/>
       <c r="AC11" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="AD11" s="2"/>
@@ -1539,7 +1540,7 @@
       <c r="AA12" s="1"/>
       <c r="AB12" s="1"/>
       <c r="AC12" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="AD12" s="2"/>
@@ -1587,7 +1588,7 @@
       <c r="AA13" s="1"/>
       <c r="AB13" s="1"/>
       <c r="AC13" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="AD13" s="2"/>

</xml_diff>

<commit_message>
2017 Week 17 Final update.
</commit_message>
<xml_diff>
--- a/post_season_inputs.xlsx
+++ b/post_season_inputs.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Spreadsheets\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2017 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -37,31 +37,7 @@
     <t>Points:</t>
   </si>
   <si>
-    <t>Raiders</t>
-  </si>
-  <si>
     <t>Post Season Week 1 Input Form</t>
-  </si>
-  <si>
-    <t>Texans</t>
-  </si>
-  <si>
-    <t>Seahawks</t>
-  </si>
-  <si>
-    <t>Steelers</t>
-  </si>
-  <si>
-    <t>Packers</t>
-  </si>
-  <si>
-    <t>Lions</t>
-  </si>
-  <si>
-    <t>Dolphins</t>
-  </si>
-  <si>
-    <t>Giants</t>
   </si>
   <si>
     <t>Game</t>
@@ -80,6 +56,30 @@
   </si>
   <si>
     <t xml:space="preserve">Name:  </t>
+  </si>
+  <si>
+    <t>Titans</t>
+  </si>
+  <si>
+    <t>Falcons</t>
+  </si>
+  <si>
+    <t>Bills</t>
+  </si>
+  <si>
+    <t>Panthers</t>
+  </si>
+  <si>
+    <t>Chiefs</t>
+  </si>
+  <si>
+    <t>Rams</t>
+  </si>
+  <si>
+    <t>Jaguars</t>
+  </si>
+  <si>
+    <t>Saints</t>
   </si>
 </sst>
 </file>
@@ -1058,7 +1058,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:AZ166"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -1085,7 +1085,7 @@
   <sheetData>
     <row r="1" spans="2:51" s="52" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="53" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C1" s="53"/>
       <c r="D1" s="53"/>
@@ -1140,7 +1140,7 @@
     <row r="2" spans="2:51" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="39"/>
       <c r="C2" s="40" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D2" s="41"/>
       <c r="E2" s="42"/>
@@ -1156,20 +1156,20 @@
     </row>
     <row r="3" spans="2:51" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="45" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C3" s="46" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D3" s="47" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E3" s="48" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="F3" s="46"/>
       <c r="G3" s="47" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="H3" s="49"/>
       <c r="I3" s="3"/>
@@ -1192,14 +1192,14 @@
         <v>1</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="D4" s="20" t="str">
         <f ca="1">IF(B4="","","at")</f>
         <v>at</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="F4" s="19"/>
       <c r="G4" s="20" t="str">
@@ -1232,14 +1232,14 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D5" s="23" t="str">
         <f t="shared" ref="D5:D7" ca="1" si="0">IF(B5="","","at")</f>
         <v>at</v>
       </c>
       <c r="E5" s="31" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="F5" s="22"/>
       <c r="G5" s="23" t="str">
@@ -1263,7 +1263,7 @@
       </c>
       <c r="AD5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for the ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for the Raiders at Texans (Game 1).</v>
+        <v>Pick a winner (V or H) for the Titans at Chiefs (Game 1).</v>
       </c>
     </row>
     <row r="6" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -1272,14 +1272,14 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D6" s="23" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>at</v>
       </c>
       <c r="E6" s="31" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F6" s="22"/>
       <c r="G6" s="23" t="str">
@@ -1303,7 +1303,7 @@
       </c>
       <c r="AD6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE("Enter the predicted margin of victory for the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Enter the predicted margin of victory for the Texans (Game 1).</v>
+        <v>Enter the predicted margin of victory for the Chiefs (Game 1).</v>
       </c>
     </row>
     <row r="7" spans="2:51" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1312,14 +1312,14 @@
         <v>4</v>
       </c>
       <c r="C7" s="32" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D7" s="26" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>at</v>
       </c>
       <c r="E7" s="33" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="F7" s="25"/>
       <c r="G7" s="26" t="str">
@@ -1343,7 +1343,7 @@
       </c>
       <c r="AD7" s="2" t="str">
         <f ca="1">IF($H$8="",CONCATENATE("Enter your Total Points Prediction for ",OFFSET($C$4,MAX($B4:$B7)-1,0)," at ",OFFSET($E$4,MAX($B4:$B7)-1,0)," (Game ",OFFSET($B$4,MAX($B4:$B7)-1,0),") in cell H8"),"")</f>
-        <v>Enter your Total Points Prediction for Giants at Packers (Game 4) in cell H8</v>
+        <v>Enter your Total Points Prediction for Panthers at Saints (Game 4) in cell H8</v>
       </c>
     </row>
     <row r="8" spans="2:51" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
2017 Post Season Week 1 Final update.
</commit_message>
<xml_diff>
--- a/post_season_inputs.xlsx
+++ b/post_season_inputs.xlsx
@@ -37,9 +37,6 @@
     <t>Points:</t>
   </si>
   <si>
-    <t>Post Season Week 1 Input Form</t>
-  </si>
-  <si>
     <t>Game</t>
   </si>
   <si>
@@ -64,22 +61,25 @@
     <t>Falcons</t>
   </si>
   <si>
-    <t>Bills</t>
-  </si>
-  <si>
-    <t>Panthers</t>
-  </si>
-  <si>
-    <t>Chiefs</t>
-  </si>
-  <si>
-    <t>Rams</t>
-  </si>
-  <si>
     <t>Jaguars</t>
   </si>
   <si>
     <t>Saints</t>
+  </si>
+  <si>
+    <t>Eagles</t>
+  </si>
+  <si>
+    <t>Patriots</t>
+  </si>
+  <si>
+    <t>Steelers</t>
+  </si>
+  <si>
+    <t>Vikings</t>
+  </si>
+  <si>
+    <t>Post Season Week 2 Input Form</t>
   </si>
 </sst>
 </file>
@@ -1085,7 +1085,7 @@
   <sheetData>
     <row r="1" spans="2:51" s="52" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="53" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="C1" s="53"/>
       <c r="D1" s="53"/>
@@ -1140,7 +1140,7 @@
     <row r="2" spans="2:51" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="39"/>
       <c r="C2" s="40" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" s="41"/>
       <c r="E2" s="42"/>
@@ -1156,20 +1156,20 @@
     </row>
     <row r="3" spans="2:51" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="46" t="s">
+      <c r="D3" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="47" t="s">
+      <c r="E3" s="48" t="s">
         <v>7</v>
-      </c>
-      <c r="E3" s="48" t="s">
-        <v>8</v>
       </c>
       <c r="F3" s="46"/>
       <c r="G3" s="47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H3" s="49"/>
       <c r="I3" s="3"/>
@@ -1199,7 +1199,7 @@
         <v>at</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F4" s="19"/>
       <c r="G4" s="20" t="str">
@@ -1232,14 +1232,14 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D5" s="23" t="str">
         <f t="shared" ref="D5:D7" ca="1" si="0">IF(B5="","","at")</f>
         <v>at</v>
       </c>
       <c r="E5" s="31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F5" s="22"/>
       <c r="G5" s="23" t="str">
@@ -1263,7 +1263,7 @@
       </c>
       <c r="AD5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for the ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for the Titans at Chiefs (Game 1).</v>
+        <v>Pick a winner (V or H) for the Falcons at Eagles (Game 1).</v>
       </c>
     </row>
     <row r="6" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -1272,14 +1272,14 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" s="23" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>at</v>
       </c>
       <c r="E6" s="31" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F6" s="22"/>
       <c r="G6" s="23" t="str">
@@ -1303,7 +1303,7 @@
       </c>
       <c r="AD6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE("Enter the predicted margin of victory for the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Enter the predicted margin of victory for the Chiefs (Game 1).</v>
+        <v>Enter the predicted margin of victory for the Eagles (Game 1).</v>
       </c>
     </row>
     <row r="7" spans="2:51" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1312,14 +1312,14 @@
         <v>4</v>
       </c>
       <c r="C7" s="32" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D7" s="26" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>at</v>
       </c>
       <c r="E7" s="33" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F7" s="25"/>
       <c r="G7" s="26" t="str">
@@ -1343,7 +1343,7 @@
       </c>
       <c r="AD7" s="2" t="str">
         <f ca="1">IF($H$8="",CONCATENATE("Enter your Total Points Prediction for ",OFFSET($C$4,MAX($B4:$B7)-1,0)," at ",OFFSET($E$4,MAX($B4:$B7)-1,0)," (Game ",OFFSET($B$4,MAX($B4:$B7)-1,0),") in cell H8"),"")</f>
-        <v>Enter your Total Points Prediction for Panthers at Saints (Game 4) in cell H8</v>
+        <v>Enter your Total Points Prediction for Saints at Vikings (Game 4) in cell H8</v>
       </c>
     </row>
     <row r="8" spans="2:51" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
2017 Post Season Week 2 Final update.
</commit_message>
<xml_diff>
--- a/post_season_inputs.xlsx
+++ b/post_season_inputs.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>H</t>
   </si>
@@ -55,16 +55,7 @@
     <t xml:space="preserve">Name:  </t>
   </si>
   <si>
-    <t>Titans</t>
-  </si>
-  <si>
-    <t>Falcons</t>
-  </si>
-  <si>
     <t>Jaguars</t>
-  </si>
-  <si>
-    <t>Saints</t>
   </si>
   <si>
     <t>Eagles</t>
@@ -73,13 +64,10 @@
     <t>Patriots</t>
   </si>
   <si>
-    <t>Steelers</t>
-  </si>
-  <si>
     <t>Vikings</t>
   </si>
   <si>
-    <t>Post Season Week 2 Input Form</t>
+    <t>Post Season Week 3 Input Form</t>
   </si>
 </sst>
 </file>
@@ -1085,7 +1073,7 @@
   <sheetData>
     <row r="1" spans="2:51" s="52" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="53" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C1" s="53"/>
       <c r="D1" s="53"/>
@@ -1192,14 +1180,14 @@
         <v>1</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" s="20" t="str">
         <f ca="1">IF(B4="","","at")</f>
         <v>at</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F4" s="19"/>
       <c r="G4" s="20" t="str">
@@ -1232,14 +1220,14 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D5" s="23" t="str">
         <f t="shared" ref="D5:D7" ca="1" si="0">IF(B5="","","at")</f>
         <v>at</v>
       </c>
       <c r="E5" s="31" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F5" s="22"/>
       <c r="G5" s="23" t="str">
@@ -1263,39 +1251,35 @@
       </c>
       <c r="AD5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for the ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for the Falcons at Eagles (Game 1).</v>
+        <v>Pick a winner (V or H) for the Jaguars at Patriots (Game 1).</v>
       </c>
     </row>
     <row r="6" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="35">
+      <c r="B6" s="35" t="str">
         <f ca="1">IF(ISTEXT($C6),ROW($B6)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B6)-ROW($B$4),0)),"")</f>
-        <v>3</v>
+        <v/>
       </c>
-      <c r="C6" s="30" t="s">
-        <v>12</v>
-      </c>
+      <c r="C6" s="30"/>
       <c r="D6" s="23" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>at</v>
+        <v/>
       </c>
-      <c r="E6" s="31" t="s">
-        <v>16</v>
-      </c>
+      <c r="E6" s="31"/>
       <c r="F6" s="22"/>
       <c r="G6" s="23" t="str">
         <f ca="1">IF(B6="","","by")</f>
-        <v>by</v>
+        <v/>
       </c>
       <c r="H6" s="24"/>
       <c r="I6" s="6"/>
       <c r="J6" s="7"/>
-      <c r="AA6" s="1">
+      <c r="AA6" s="1" t="str">
         <f ca="1">IF($B6="","",IF(AND($F6&lt;&gt;"H",$F6&lt;&gt;"V"),ROW(),""))</f>
-        <v>6</v>
+        <v/>
       </c>
-      <c r="AB6" s="1">
+      <c r="AB6" s="1" t="str">
         <f ca="1">IF($B6="","",IF($H6&lt;1,ROW(),""))</f>
-        <v>6</v>
+        <v/>
       </c>
       <c r="AC6" s="1">
         <f t="shared" ca="1" si="1"/>
@@ -1303,39 +1287,35 @@
       </c>
       <c r="AD6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE("Enter the predicted margin of victory for the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Enter the predicted margin of victory for the Eagles (Game 1).</v>
+        <v>Enter the predicted margin of victory for the Patriots (Game 1).</v>
       </c>
     </row>
     <row r="7" spans="2:51" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="36">
+      <c r="B7" s="36" t="str">
         <f ca="1">IF(ISTEXT($C7),ROW($B7)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B7)-ROW($B$4),0)),"")</f>
-        <v>4</v>
+        <v/>
       </c>
-      <c r="C7" s="32" t="s">
-        <v>13</v>
-      </c>
+      <c r="C7" s="32"/>
       <c r="D7" s="26" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>at</v>
+        <v/>
       </c>
-      <c r="E7" s="33" t="s">
-        <v>17</v>
-      </c>
+      <c r="E7" s="33"/>
       <c r="F7" s="25"/>
       <c r="G7" s="26" t="str">
         <f ca="1">IF(B7="","","by")</f>
-        <v>by</v>
+        <v/>
       </c>
       <c r="H7" s="27"/>
       <c r="I7" s="6"/>
       <c r="J7" s="7"/>
-      <c r="AA7" s="1">
+      <c r="AA7" s="1" t="str">
         <f ca="1">IF($B7="","",IF(AND($F7&lt;&gt;"H",$F7&lt;&gt;"V"),ROW(),""))</f>
-        <v>7</v>
+        <v/>
       </c>
-      <c r="AB7" s="1">
+      <c r="AB7" s="1" t="str">
         <f ca="1">IF($B7="","",IF($H7&lt;1,ROW(),""))</f>
-        <v>7</v>
+        <v/>
       </c>
       <c r="AC7" s="1">
         <f ca="1">IF($AD7&lt;&gt;"",ROW(),"")</f>
@@ -1343,7 +1323,7 @@
       </c>
       <c r="AD7" s="2" t="str">
         <f ca="1">IF($H$8="",CONCATENATE("Enter your Total Points Prediction for ",OFFSET($C$4,MAX($B4:$B7)-1,0)," at ",OFFSET($E$4,MAX($B4:$B7)-1,0)," (Game ",OFFSET($B$4,MAX($B4:$B7)-1,0),") in cell H8"),"")</f>
-        <v>Enter your Total Points Prediction for Saints at Vikings (Game 4) in cell H8</v>
+        <v>Enter your Total Points Prediction for Vikings at Eagles (Game 2) in cell H8</v>
       </c>
     </row>
     <row r="8" spans="2:51" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1352,7 +1332,7 @@
       <c r="D8" s="17"/>
       <c r="E8" s="18" t="str">
         <f ca="1">CONCATENATE("                   Game ",MAX(B4:B7)," Total")</f>
-        <v xml:space="preserve">                   Game 4 Total</v>
+        <v xml:space="preserve">                   Game 2 Total</v>
       </c>
       <c r="F8" s="17"/>
       <c r="G8" s="37" t="s">

</xml_diff>

<commit_message>
2017 Post Season Week 3 Final update.
</commit_message>
<xml_diff>
--- a/post_season_inputs.xlsx
+++ b/post_season_inputs.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>H</t>
   </si>
@@ -55,19 +55,13 @@
     <t xml:space="preserve">Name:  </t>
   </si>
   <si>
-    <t>Jaguars</t>
-  </si>
-  <si>
     <t>Eagles</t>
   </si>
   <si>
     <t>Patriots</t>
   </si>
   <si>
-    <t>Vikings</t>
-  </si>
-  <si>
-    <t>Post Season Week 3 Input Form</t>
+    <t>Post Season Week 4 Input Form</t>
   </si>
 </sst>
 </file>
@@ -1073,7 +1067,7 @@
   <sheetData>
     <row r="1" spans="2:51" s="52" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="53" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C1" s="53"/>
       <c r="D1" s="53"/>
@@ -1187,7 +1181,7 @@
         <v>at</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4" s="19"/>
       <c r="G4" s="20" t="str">
@@ -1215,35 +1209,31 @@
       </c>
     </row>
     <row r="5" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="35">
+      <c r="B5" s="35" t="str">
         <f ca="1">IF(ISTEXT($C5),ROW($B5)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B5)-ROW($B$4),0)),"")</f>
-        <v>2</v>
+        <v/>
       </c>
-      <c r="C5" s="30" t="s">
-        <v>13</v>
-      </c>
+      <c r="C5" s="30"/>
       <c r="D5" s="23" t="str">
         <f t="shared" ref="D5:D7" ca="1" si="0">IF(B5="","","at")</f>
-        <v>at</v>
+        <v/>
       </c>
-      <c r="E5" s="31" t="s">
-        <v>11</v>
-      </c>
+      <c r="E5" s="31"/>
       <c r="F5" s="22"/>
       <c r="G5" s="23" t="str">
         <f ca="1">IF(B5="","","by")</f>
-        <v>by</v>
+        <v/>
       </c>
       <c r="H5" s="24"/>
       <c r="I5" s="3"/>
       <c r="J5" s="5"/>
-      <c r="AA5" s="1">
+      <c r="AA5" s="1" t="str">
         <f ca="1">IF($B5="","",IF(AND($F5&lt;&gt;"H",$F5&lt;&gt;"V"),ROW(),""))</f>
-        <v>5</v>
+        <v/>
       </c>
-      <c r="AB5" s="1">
+      <c r="AB5" s="1" t="str">
         <f ca="1">IF($B5="","",IF($H5&lt;1,ROW(),""))</f>
-        <v>5</v>
+        <v/>
       </c>
       <c r="AC5" s="1">
         <f t="shared" ref="AC5:AC13" ca="1" si="1">IF($AD5&lt;&gt;"",ROW(),"")</f>
@@ -1251,7 +1241,7 @@
       </c>
       <c r="AD5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for the ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for the Jaguars at Patriots (Game 1).</v>
+        <v>Pick a winner (V or H) for the Eagles at Patriots (Game 1).</v>
       </c>
     </row>
     <row r="6" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -1323,7 +1313,7 @@
       </c>
       <c r="AD7" s="2" t="str">
         <f ca="1">IF($H$8="",CONCATENATE("Enter your Total Points Prediction for ",OFFSET($C$4,MAX($B4:$B7)-1,0)," at ",OFFSET($E$4,MAX($B4:$B7)-1,0)," (Game ",OFFSET($B$4,MAX($B4:$B7)-1,0),") in cell H8"),"")</f>
-        <v>Enter your Total Points Prediction for Vikings at Eagles (Game 2) in cell H8</v>
+        <v>Enter your Total Points Prediction for Eagles at Patriots (Game 1) in cell H8</v>
       </c>
     </row>
     <row r="8" spans="2:51" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1332,7 +1322,7 @@
       <c r="D8" s="17"/>
       <c r="E8" s="18" t="str">
         <f ca="1">CONCATENATE("                   Game ",MAX(B4:B7)," Total")</f>
-        <v xml:space="preserve">                   Game 2 Total</v>
+        <v xml:space="preserve">                   Game 1 Total</v>
       </c>
       <c r="F8" s="17"/>
       <c r="G8" s="37" t="s">

</xml_diff>

<commit_message>
2018 Week 17 Final update.
</commit_message>
<xml_diff>
--- a/post_season_inputs.xlsx
+++ b/post_season_inputs.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2017 Football Pool Page\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2018 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C511EE06-9A61-42E7-8254-1DEF7773DEB5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="9420" windowHeight="4500" tabRatio="267"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="9420" windowHeight="4500" tabRatio="267" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Post Season Input Form" sheetId="1" r:id="rId1"/>
@@ -18,12 +19,12 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Post Season Input Form'!$B$1:$H$7</definedName>
     <definedName name="Season_total_points">'Post Season Input Form'!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>H</t>
   </si>
@@ -58,16 +59,34 @@
     <t>Eagles</t>
   </si>
   <si>
-    <t>Patriots</t>
+    <t>Colts</t>
   </si>
   <si>
-    <t>Post Season Week 4 Input Form</t>
+    <t>Seahawks</t>
+  </si>
+  <si>
+    <t>Chargers</t>
+  </si>
+  <si>
+    <t>Texans</t>
+  </si>
+  <si>
+    <t>Cowboys</t>
+  </si>
+  <si>
+    <t>Ravens</t>
+  </si>
+  <si>
+    <t>Bears</t>
+  </si>
+  <si>
+    <t>Post Season Week 1 Input Form</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1036,7 +1055,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:AZ166"/>
   <sheetViews>
@@ -1067,7 +1086,7 @@
   <sheetData>
     <row r="1" spans="2:51" s="52" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="53" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C1" s="53"/>
       <c r="D1" s="53"/>
@@ -1174,14 +1193,14 @@
         <v>1</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D4" s="20" t="str">
         <f ca="1">IF(B4="","","at")</f>
         <v>at</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F4" s="19"/>
       <c r="G4" s="20" t="str">
@@ -1209,31 +1228,35 @@
       </c>
     </row>
     <row r="5" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="35" t="str">
+      <c r="B5" s="35">
         <f ca="1">IF(ISTEXT($C5),ROW($B5)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B5)-ROW($B$4),0)),"")</f>
-        <v/>
+        <v>2</v>
       </c>
-      <c r="C5" s="30"/>
+      <c r="C5" s="30" t="s">
+        <v>12</v>
+      </c>
       <c r="D5" s="23" t="str">
         <f t="shared" ref="D5:D7" ca="1" si="0">IF(B5="","","at")</f>
-        <v/>
+        <v>at</v>
       </c>
-      <c r="E5" s="31"/>
+      <c r="E5" s="31" t="s">
+        <v>15</v>
+      </c>
       <c r="F5" s="22"/>
       <c r="G5" s="23" t="str">
         <f ca="1">IF(B5="","","by")</f>
-        <v/>
+        <v>by</v>
       </c>
       <c r="H5" s="24"/>
       <c r="I5" s="3"/>
       <c r="J5" s="5"/>
-      <c r="AA5" s="1" t="str">
+      <c r="AA5" s="1">
         <f ca="1">IF($B5="","",IF(AND($F5&lt;&gt;"H",$F5&lt;&gt;"V"),ROW(),""))</f>
-        <v/>
+        <v>5</v>
       </c>
-      <c r="AB5" s="1" t="str">
+      <c r="AB5" s="1">
         <f ca="1">IF($B5="","",IF($H5&lt;1,ROW(),""))</f>
-        <v/>
+        <v>5</v>
       </c>
       <c r="AC5" s="1">
         <f t="shared" ref="AC5:AC13" ca="1" si="1">IF($AD5&lt;&gt;"",ROW(),"")</f>
@@ -1241,35 +1264,39 @@
       </c>
       <c r="AD5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for the ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for the Eagles at Patriots (Game 1).</v>
+        <v>Pick a winner (V or H) for the Colts at Texans (Game 1).</v>
       </c>
     </row>
     <row r="6" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="35" t="str">
+      <c r="B6" s="35">
         <f ca="1">IF(ISTEXT($C6),ROW($B6)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B6)-ROW($B$4),0)),"")</f>
-        <v/>
+        <v>3</v>
       </c>
-      <c r="C6" s="30"/>
+      <c r="C6" s="30" t="s">
+        <v>13</v>
+      </c>
       <c r="D6" s="23" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v>at</v>
       </c>
-      <c r="E6" s="31"/>
+      <c r="E6" s="31" t="s">
+        <v>16</v>
+      </c>
       <c r="F6" s="22"/>
       <c r="G6" s="23" t="str">
         <f ca="1">IF(B6="","","by")</f>
-        <v/>
+        <v>by</v>
       </c>
       <c r="H6" s="24"/>
       <c r="I6" s="6"/>
       <c r="J6" s="7"/>
-      <c r="AA6" s="1" t="str">
+      <c r="AA6" s="1">
         <f ca="1">IF($B6="","",IF(AND($F6&lt;&gt;"H",$F6&lt;&gt;"V"),ROW(),""))</f>
-        <v/>
+        <v>6</v>
       </c>
-      <c r="AB6" s="1" t="str">
+      <c r="AB6" s="1">
         <f ca="1">IF($B6="","",IF($H6&lt;1,ROW(),""))</f>
-        <v/>
+        <v>6</v>
       </c>
       <c r="AC6" s="1">
         <f t="shared" ca="1" si="1"/>
@@ -1277,35 +1304,39 @@
       </c>
       <c r="AD6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE("Enter the predicted margin of victory for the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Enter the predicted margin of victory for the Patriots (Game 1).</v>
+        <v>Enter the predicted margin of victory for the Texans (Game 1).</v>
       </c>
     </row>
     <row r="7" spans="2:51" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="36" t="str">
+      <c r="B7" s="36">
         <f ca="1">IF(ISTEXT($C7),ROW($B7)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B7)-ROW($B$4),0)),"")</f>
-        <v/>
+        <v>4</v>
       </c>
-      <c r="C7" s="32"/>
+      <c r="C7" s="32" t="s">
+        <v>10</v>
+      </c>
       <c r="D7" s="26" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v>at</v>
       </c>
-      <c r="E7" s="33"/>
+      <c r="E7" s="33" t="s">
+        <v>17</v>
+      </c>
       <c r="F7" s="25"/>
       <c r="G7" s="26" t="str">
         <f ca="1">IF(B7="","","by")</f>
-        <v/>
+        <v>by</v>
       </c>
       <c r="H7" s="27"/>
       <c r="I7" s="6"/>
       <c r="J7" s="7"/>
-      <c r="AA7" s="1" t="str">
+      <c r="AA7" s="1">
         <f ca="1">IF($B7="","",IF(AND($F7&lt;&gt;"H",$F7&lt;&gt;"V"),ROW(),""))</f>
-        <v/>
+        <v>7</v>
       </c>
-      <c r="AB7" s="1" t="str">
+      <c r="AB7" s="1">
         <f ca="1">IF($B7="","",IF($H7&lt;1,ROW(),""))</f>
-        <v/>
+        <v>7</v>
       </c>
       <c r="AC7" s="1">
         <f ca="1">IF($AD7&lt;&gt;"",ROW(),"")</f>
@@ -1313,7 +1344,7 @@
       </c>
       <c r="AD7" s="2" t="str">
         <f ca="1">IF($H$8="",CONCATENATE("Enter your Total Points Prediction for ",OFFSET($C$4,MAX($B4:$B7)-1,0)," at ",OFFSET($E$4,MAX($B4:$B7)-1,0)," (Game ",OFFSET($B$4,MAX($B4:$B7)-1,0),") in cell H8"),"")</f>
-        <v>Enter your Total Points Prediction for Eagles at Patriots (Game 1) in cell H8</v>
+        <v>Enter your Total Points Prediction for Eagles at Bears (Game 4) in cell H8</v>
       </c>
     </row>
     <row r="8" spans="2:51" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1322,7 +1353,7 @@
       <c r="D8" s="17"/>
       <c r="E8" s="18" t="str">
         <f ca="1">CONCATENATE("                   Game ",MAX(B4:B7)," Total")</f>
-        <v xml:space="preserve">                   Game 1 Total</v>
+        <v xml:space="preserve">                   Game 4 Total</v>
       </c>
       <c r="F8" s="17"/>
       <c r="G8" s="37" t="s">
@@ -8343,18 +8374,18 @@
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations count="4">
-    <dataValidation type="whole" allowBlank="1" showErrorMessage="1" errorTitle="PREDICTION" error="Enter a number between 1 and 99 for the predicted margin of victory._x000a__x000a_If there are no teams listed in this row, then your only choice is to leave this cell blank._x000a_" sqref="H4:H7">
+    <dataValidation type="whole" allowBlank="1" showErrorMessage="1" errorTitle="PREDICTION" error="Enter a number between 1 and 99 for the predicted margin of victory._x000a__x000a_If there are no teams listed in this row, then your only choice is to leave this cell blank._x000a_" sqref="H4:H7" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>IF(B4="","",1)</formula1>
       <formula2>IF(B4="","",99)</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showErrorMessage="1" errorTitle="Total Points Prediction" error="Enter a number between 1 and 99 for your Total Points Prediction._x000a_" sqref="H8">
+    <dataValidation type="whole" allowBlank="1" showErrorMessage="1" errorTitle="Total Points Prediction" error="Enter a number between 1 and 99 for your Total Points Prediction._x000a_" sqref="H8" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>IF(B4="","",1)</formula1>
       <formula2>IF(B4="","",99)</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="PREDICTION" error="Pick a winner._x000a__x000a_Enter &quot;H&quot; for the home team or &quot;V&quot; for the visiting team._x000a__x000a_If there are no teams listed in this row, then your only choice is to leave this cell blank._x000a_" sqref="F4:F7">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="PREDICTION" error="Pick a winner._x000a__x000a_Enter &quot;H&quot; for the home team or &quot;V&quot; for the visiting team._x000a__x000a_If there are no teams listed in this row, then your only choice is to leave this cell blank._x000a_" sqref="F4:F7" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>IF($B4="",$AC$2:$AC$2,$AA$2:$AB$2)</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showErrorMessage="1" errorTitle="NAME:" error="Your name must include at least 2 non-blank characters." sqref="D2">
+    <dataValidation type="custom" allowBlank="1" showErrorMessage="1" errorTitle="NAME:" error="Your name must include at least 2 non-blank characters." sqref="D2" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>OR($D$2="",LEN(SUBSTITUTE($D$2," ",""))&gt;1)</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
2018 Post Season Week 1 Final update.
</commit_message>
<xml_diff>
--- a/post_season_inputs.xlsx
+++ b/post_season_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2018 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A93ABD68-77AC-452A-81D0-C28286080084}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E626D4B-BA59-4A3B-BB31-F75397A3A9CC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="135" windowWidth="9420" windowHeight="4500" tabRatio="267" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,25 +62,25 @@
     <t>Colts</t>
   </si>
   <si>
-    <t>Seahawks</t>
-  </si>
-  <si>
     <t>Chargers</t>
-  </si>
-  <si>
-    <t>Texans</t>
   </si>
   <si>
     <t>Cowboys</t>
   </si>
   <si>
-    <t>Ravens</t>
+    <t>Chiefs</t>
   </si>
   <si>
-    <t>Bears</t>
+    <t>Rams</t>
   </si>
   <si>
-    <t>Post Season Week 1 Input Form</t>
+    <t>Patriots</t>
+  </si>
+  <si>
+    <t>Saints</t>
+  </si>
+  <si>
+    <t>Post Season Week 2 Input Form</t>
   </si>
 </sst>
 </file>
@@ -1233,7 +1233,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D5" s="23" t="str">
         <f t="shared" ref="D5:D7" ca="1" si="0">IF(B5="","","at")</f>
@@ -1264,7 +1264,7 @@
       </c>
       <c r="AD5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for the ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for the Colts at Texans (Game 1).</v>
+        <v>Pick a winner (V or H) for the Colts at Chiefs (Game 1).</v>
       </c>
     </row>
     <row r="6" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -1273,7 +1273,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" s="23" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -1304,7 +1304,7 @@
       </c>
       <c r="AD6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE("Enter the predicted margin of victory for the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Enter the predicted margin of victory for the Texans (Game 1).</v>
+        <v>Enter the predicted margin of victory for the Chiefs (Game 1).</v>
       </c>
     </row>
     <row r="7" spans="2:51" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1344,7 +1344,7 @@
       </c>
       <c r="AD7" s="2" t="str">
         <f ca="1">IF($H$8="",CONCATENATE("Enter your Total Points Prediction for ",OFFSET($C$4,MAX($B4:$B7)-1,0)," at ",OFFSET($E$4,MAX($B4:$B7)-1,0)," (Game ",OFFSET($B$4,MAX($B4:$B7)-1,0),") in cell H8"),"")</f>
-        <v>Enter your Total Points Prediction for Eagles at Bears (Game 4) in cell H8</v>
+        <v>Enter your Total Points Prediction for Eagles at Saints (Game 4) in cell H8</v>
       </c>
     </row>
     <row r="8" spans="2:51" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
2018 Post Season Week 2 Final update.
</commit_message>
<xml_diff>
--- a/post_season_inputs.xlsx
+++ b/post_season_inputs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2018 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E626D4B-BA59-4A3B-BB31-F75397A3A9CC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46012F07-680F-4A55-8847-E42610FA4727}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="135" windowWidth="9420" windowHeight="4500" tabRatio="267" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>H</t>
   </si>
@@ -56,18 +56,6 @@
     <t xml:space="preserve">Name:  </t>
   </si>
   <si>
-    <t>Eagles</t>
-  </si>
-  <si>
-    <t>Colts</t>
-  </si>
-  <si>
-    <t>Chargers</t>
-  </si>
-  <si>
-    <t>Cowboys</t>
-  </si>
-  <si>
     <t>Chiefs</t>
   </si>
   <si>
@@ -80,7 +68,7 @@
     <t>Saints</t>
   </si>
   <si>
-    <t>Post Season Week 2 Input Form</t>
+    <t>Post Season Week 3 Input Form</t>
   </si>
 </sst>
 </file>
@@ -1086,7 +1074,7 @@
   <sheetData>
     <row r="1" spans="2:51" s="52" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="53" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C1" s="53"/>
       <c r="D1" s="53"/>
@@ -1200,7 +1188,7 @@
         <v>at</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F4" s="19"/>
       <c r="G4" s="20" t="str">
@@ -1233,14 +1221,14 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" s="23" t="str">
         <f t="shared" ref="D5:D7" ca="1" si="0">IF(B5="","","at")</f>
         <v>at</v>
       </c>
       <c r="E5" s="31" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F5" s="22"/>
       <c r="G5" s="23" t="str">
@@ -1264,39 +1252,35 @@
       </c>
       <c r="AD5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for the ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for the Colts at Chiefs (Game 1).</v>
+        <v>Pick a winner (V or H) for the Rams at Saints (Game 1).</v>
       </c>
     </row>
     <row r="6" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="35">
+      <c r="B6" s="35" t="str">
         <f ca="1">IF(ISTEXT($C6),ROW($B6)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B6)-ROW($B$4),0)),"")</f>
-        <v>3</v>
+        <v/>
       </c>
-      <c r="C6" s="30" t="s">
-        <v>12</v>
-      </c>
+      <c r="C6" s="30"/>
       <c r="D6" s="23" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>at</v>
+        <v/>
       </c>
-      <c r="E6" s="31" t="s">
-        <v>16</v>
-      </c>
+      <c r="E6" s="31"/>
       <c r="F6" s="22"/>
       <c r="G6" s="23" t="str">
         <f ca="1">IF(B6="","","by")</f>
-        <v>by</v>
+        <v/>
       </c>
       <c r="H6" s="24"/>
       <c r="I6" s="6"/>
       <c r="J6" s="7"/>
-      <c r="AA6" s="1">
+      <c r="AA6" s="1" t="str">
         <f ca="1">IF($B6="","",IF(AND($F6&lt;&gt;"H",$F6&lt;&gt;"V"),ROW(),""))</f>
-        <v>6</v>
+        <v/>
       </c>
-      <c r="AB6" s="1">
+      <c r="AB6" s="1" t="str">
         <f ca="1">IF($B6="","",IF($H6&lt;1,ROW(),""))</f>
-        <v>6</v>
+        <v/>
       </c>
       <c r="AC6" s="1">
         <f t="shared" ca="1" si="1"/>
@@ -1304,39 +1288,35 @@
       </c>
       <c r="AD6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE("Enter the predicted margin of victory for the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Enter the predicted margin of victory for the Chiefs (Game 1).</v>
+        <v>Enter the predicted margin of victory for the Saints (Game 1).</v>
       </c>
     </row>
     <row r="7" spans="2:51" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="36">
+      <c r="B7" s="36" t="str">
         <f ca="1">IF(ISTEXT($C7),ROW($B7)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B7)-ROW($B$4),0)),"")</f>
-        <v>4</v>
+        <v/>
       </c>
-      <c r="C7" s="32" t="s">
-        <v>10</v>
-      </c>
+      <c r="C7" s="32"/>
       <c r="D7" s="26" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>at</v>
+        <v/>
       </c>
-      <c r="E7" s="33" t="s">
-        <v>17</v>
-      </c>
+      <c r="E7" s="33"/>
       <c r="F7" s="25"/>
       <c r="G7" s="26" t="str">
         <f ca="1">IF(B7="","","by")</f>
-        <v>by</v>
+        <v/>
       </c>
       <c r="H7" s="27"/>
       <c r="I7" s="6"/>
       <c r="J7" s="7"/>
-      <c r="AA7" s="1">
+      <c r="AA7" s="1" t="str">
         <f ca="1">IF($B7="","",IF(AND($F7&lt;&gt;"H",$F7&lt;&gt;"V"),ROW(),""))</f>
-        <v>7</v>
+        <v/>
       </c>
-      <c r="AB7" s="1">
+      <c r="AB7" s="1" t="str">
         <f ca="1">IF($B7="","",IF($H7&lt;1,ROW(),""))</f>
-        <v>7</v>
+        <v/>
       </c>
       <c r="AC7" s="1">
         <f ca="1">IF($AD7&lt;&gt;"",ROW(),"")</f>
@@ -1344,7 +1324,7 @@
       </c>
       <c r="AD7" s="2" t="str">
         <f ca="1">IF($H$8="",CONCATENATE("Enter your Total Points Prediction for ",OFFSET($C$4,MAX($B4:$B7)-1,0)," at ",OFFSET($E$4,MAX($B4:$B7)-1,0)," (Game ",OFFSET($B$4,MAX($B4:$B7)-1,0),") in cell H8"),"")</f>
-        <v>Enter your Total Points Prediction for Eagles at Saints (Game 4) in cell H8</v>
+        <v>Enter your Total Points Prediction for Patriots at Chiefs (Game 2) in cell H8</v>
       </c>
     </row>
     <row r="8" spans="2:51" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1353,7 +1333,7 @@
       <c r="D8" s="17"/>
       <c r="E8" s="18" t="str">
         <f ca="1">CONCATENATE("                   Game ",MAX(B4:B7)," Total")</f>
-        <v xml:space="preserve">                   Game 4 Total</v>
+        <v xml:space="preserve">                   Game 2 Total</v>
       </c>
       <c r="F8" s="17"/>
       <c r="G8" s="37" t="s">

</xml_diff>

<commit_message>
2018 Post Season Week 3 Final update.
</commit_message>
<xml_diff>
--- a/post_season_inputs.xlsx
+++ b/post_season_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2018 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46012F07-680F-4A55-8847-E42610FA4727}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DCAAC0F-88C4-414B-B373-2D810046D14D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="135" windowWidth="9420" windowHeight="4500" tabRatio="267" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>H</t>
   </si>
@@ -56,19 +56,13 @@
     <t xml:space="preserve">Name:  </t>
   </si>
   <si>
-    <t>Chiefs</t>
-  </si>
-  <si>
     <t>Rams</t>
   </si>
   <si>
     <t>Patriots</t>
   </si>
   <si>
-    <t>Saints</t>
-  </si>
-  <si>
-    <t>Post Season Week 3 Input Form</t>
+    <t>Post Season Week 4 Input Form</t>
   </si>
 </sst>
 </file>
@@ -1074,7 +1068,7 @@
   <sheetData>
     <row r="1" spans="2:51" s="52" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="53" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C1" s="53"/>
       <c r="D1" s="53"/>
@@ -1188,7 +1182,7 @@
         <v>at</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F4" s="19"/>
       <c r="G4" s="20" t="str">
@@ -1216,35 +1210,31 @@
       </c>
     </row>
     <row r="5" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="35">
+      <c r="B5" s="35" t="str">
         <f ca="1">IF(ISTEXT($C5),ROW($B5)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B5)-ROW($B$4),0)),"")</f>
-        <v>2</v>
+        <v/>
       </c>
-      <c r="C5" s="30" t="s">
-        <v>12</v>
-      </c>
+      <c r="C5" s="30"/>
       <c r="D5" s="23" t="str">
         <f t="shared" ref="D5:D7" ca="1" si="0">IF(B5="","","at")</f>
-        <v>at</v>
+        <v/>
       </c>
-      <c r="E5" s="31" t="s">
-        <v>10</v>
-      </c>
+      <c r="E5" s="31"/>
       <c r="F5" s="22"/>
       <c r="G5" s="23" t="str">
         <f ca="1">IF(B5="","","by")</f>
-        <v>by</v>
+        <v/>
       </c>
       <c r="H5" s="24"/>
       <c r="I5" s="3"/>
       <c r="J5" s="5"/>
-      <c r="AA5" s="1">
+      <c r="AA5" s="1" t="str">
         <f ca="1">IF($B5="","",IF(AND($F5&lt;&gt;"H",$F5&lt;&gt;"V"),ROW(),""))</f>
-        <v>5</v>
+        <v/>
       </c>
-      <c r="AB5" s="1">
+      <c r="AB5" s="1" t="str">
         <f ca="1">IF($B5="","",IF($H5&lt;1,ROW(),""))</f>
-        <v>5</v>
+        <v/>
       </c>
       <c r="AC5" s="1">
         <f t="shared" ref="AC5:AC13" ca="1" si="1">IF($AD5&lt;&gt;"",ROW(),"")</f>
@@ -1252,7 +1242,7 @@
       </c>
       <c r="AD5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for the ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for the Rams at Saints (Game 1).</v>
+        <v>Pick a winner (V or H) for the Patriots at Rams (Game 1).</v>
       </c>
     </row>
     <row r="6" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -1288,7 +1278,7 @@
       </c>
       <c r="AD6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE("Enter the predicted margin of victory for the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Enter the predicted margin of victory for the Saints (Game 1).</v>
+        <v>Enter the predicted margin of victory for the Rams (Game 1).</v>
       </c>
     </row>
     <row r="7" spans="2:51" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1324,7 +1314,7 @@
       </c>
       <c r="AD7" s="2" t="str">
         <f ca="1">IF($H$8="",CONCATENATE("Enter your Total Points Prediction for ",OFFSET($C$4,MAX($B4:$B7)-1,0)," at ",OFFSET($E$4,MAX($B4:$B7)-1,0)," (Game ",OFFSET($B$4,MAX($B4:$B7)-1,0),") in cell H8"),"")</f>
-        <v>Enter your Total Points Prediction for Patriots at Chiefs (Game 2) in cell H8</v>
+        <v>Enter your Total Points Prediction for Patriots at Rams (Game 1) in cell H8</v>
       </c>
     </row>
     <row r="8" spans="2:51" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1333,7 +1323,7 @@
       <c r="D8" s="17"/>
       <c r="E8" s="18" t="str">
         <f ca="1">CONCATENATE("                   Game ",MAX(B4:B7)," Total")</f>
-        <v xml:space="preserve">                   Game 2 Total</v>
+        <v xml:space="preserve">                   Game 1 Total</v>
       </c>
       <c r="F8" s="17"/>
       <c r="G8" s="37" t="s">

</xml_diff>

<commit_message>
2019 Post Season Week 1 Final update.
</commit_message>
<xml_diff>
--- a/post_season_inputs.xlsx
+++ b/post_season_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2019 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5045789-CB8B-4C09-B3FA-7847F8B6641F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F31CDC3A-BF54-41EB-B0D7-CC3385209E2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="267" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,12 +64,6 @@
     <t xml:space="preserve">Name:  </t>
   </si>
   <si>
-    <t>Patriots</t>
-  </si>
-  <si>
-    <t>Bills</t>
-  </si>
-  <si>
     <t>Titans</t>
   </si>
   <si>
@@ -82,13 +76,19 @@
     <t>Texans</t>
   </si>
   <si>
-    <t>Saints</t>
+    <t>49ers</t>
   </si>
   <si>
-    <t>Eagles</t>
+    <t>Ravens</t>
   </si>
   <si>
-    <t>Post Season Week 1 Input Form</t>
+    <t>Chiefs</t>
+  </si>
+  <si>
+    <t>Packers</t>
+  </si>
+  <si>
+    <t>Post Season Week 2 Input Form</t>
   </si>
 </sst>
 </file>
@@ -1208,7 +1208,7 @@
         <v>at</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F4" s="19"/>
       <c r="G4" s="20" t="str">
@@ -1241,14 +1241,14 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D5" s="23" t="str">
         <f t="shared" ref="D5:D7" ca="1" si="0">IF(B5="","","at")</f>
         <v>at</v>
       </c>
       <c r="E5" s="31" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F5" s="22"/>
       <c r="G5" s="23" t="str">
@@ -1272,7 +1272,7 @@
       </c>
       <c r="AD5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for the ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for the Bills at Texans (Game 1).</v>
+        <v>Pick a winner (V or H) for the Vikings at 49ers (Game 1).</v>
       </c>
     </row>
     <row r="6" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -1312,7 +1312,7 @@
       </c>
       <c r="AD6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE("Enter the predicted margin of victory for the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Enter the predicted margin of victory for the Texans (Game 1).</v>
+        <v>Enter the predicted margin of victory for the 49ers (Game 1).</v>
       </c>
     </row>
     <row r="7" spans="2:51" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1321,7 +1321,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="32" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D7" s="26" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -1352,7 +1352,7 @@
       </c>
       <c r="AD7" s="2" t="str">
         <f ca="1">IF($H$8="",CONCATENATE("Enter your Total Points Prediction for ",OFFSET($C$4,MAX($B4:$B7)-1,0)," at ",OFFSET($E$4,MAX($B4:$B7)-1,0)," (Game ",OFFSET($B$4,MAX($B4:$B7)-1,0),") in cell H8"),"")</f>
-        <v>Enter your Total Points Prediction for Seahawks at Eagles (Game 4) in cell H8</v>
+        <v>Enter your Total Points Prediction for Seahawks at Packers (Game 4) in cell H8</v>
       </c>
     </row>
     <row r="8" spans="2:51" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
2019 Post Season Week 2 Final update.
</commit_message>
<xml_diff>
--- a/post_season_inputs.xlsx
+++ b/post_season_inputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2019 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F31CDC3A-BF54-41EB-B0D7-CC3385209E2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BF8B3F2-E347-446C-81E5-08D1C793F138}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="267" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" tabRatio="267" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Post Season Input Form" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>H</t>
   </si>
@@ -67,19 +67,7 @@
     <t>Titans</t>
   </si>
   <si>
-    <t>Vikings</t>
-  </si>
-  <si>
-    <t>Seahawks</t>
-  </si>
-  <si>
-    <t>Texans</t>
-  </si>
-  <si>
     <t>49ers</t>
-  </si>
-  <si>
-    <t>Ravens</t>
   </si>
   <si>
     <t>Chiefs</t>
@@ -88,7 +76,7 @@
     <t>Packers</t>
   </si>
   <si>
-    <t>Post Season Week 2 Input Form</t>
+    <t>Post Season Week 3 Input Form</t>
   </si>
 </sst>
 </file>
@@ -1094,7 +1082,7 @@
   <sheetData>
     <row r="1" spans="2:51" s="52" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="53" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C1" s="53"/>
       <c r="D1" s="53"/>
@@ -1201,14 +1189,14 @@
         <v>1</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" s="20" t="str">
         <f ca="1">IF(B4="","","at")</f>
         <v>at</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F4" s="19"/>
       <c r="G4" s="20" t="str">
@@ -1241,14 +1229,14 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D5" s="23" t="str">
         <f t="shared" ref="D5:D7" ca="1" si="0">IF(B5="","","at")</f>
         <v>at</v>
       </c>
       <c r="E5" s="31" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F5" s="22"/>
       <c r="G5" s="23" t="str">
@@ -1272,39 +1260,35 @@
       </c>
       <c r="AD5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for the ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for the Vikings at 49ers (Game 1).</v>
+        <v>Pick a winner (V or H) for the Titans at Chiefs (Game 1).</v>
       </c>
     </row>
     <row r="6" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="35">
+      <c r="B6" s="35" t="str">
         <f ca="1">IF(ISTEXT($C6),ROW($B6)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B6)-ROW($B$4),0)),"")</f>
-        <v>3</v>
+        <v/>
       </c>
-      <c r="C6" s="30" t="s">
-        <v>13</v>
-      </c>
+      <c r="C6" s="30"/>
       <c r="D6" s="23" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>at</v>
+        <v/>
       </c>
-      <c r="E6" s="31" t="s">
-        <v>16</v>
-      </c>
+      <c r="E6" s="31"/>
       <c r="F6" s="22"/>
       <c r="G6" s="23" t="str">
         <f ca="1">IF(B6="","","by")</f>
-        <v>by</v>
+        <v/>
       </c>
       <c r="H6" s="24"/>
       <c r="I6" s="6"/>
       <c r="J6" s="7"/>
-      <c r="AA6" s="1">
+      <c r="AA6" s="1" t="str">
         <f ca="1">IF($B6="","",IF(AND($F6&lt;&gt;"H",$F6&lt;&gt;"V"),ROW(),""))</f>
-        <v>6</v>
+        <v/>
       </c>
-      <c r="AB6" s="1">
+      <c r="AB6" s="1" t="str">
         <f ca="1">IF($B6="","",IF($H6&lt;1,ROW(),""))</f>
-        <v>6</v>
+        <v/>
       </c>
       <c r="AC6" s="1">
         <f t="shared" ca="1" si="1"/>
@@ -1312,39 +1296,35 @@
       </c>
       <c r="AD6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE("Enter the predicted margin of victory for the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Enter the predicted margin of victory for the 49ers (Game 1).</v>
+        <v>Enter the predicted margin of victory for the Chiefs (Game 1).</v>
       </c>
     </row>
     <row r="7" spans="2:51" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="36">
+      <c r="B7" s="36" t="str">
         <f ca="1">IF(ISTEXT($C7),ROW($B7)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B7)-ROW($B$4),0)),"")</f>
-        <v>4</v>
+        <v/>
       </c>
-      <c r="C7" s="32" t="s">
-        <v>12</v>
-      </c>
+      <c r="C7" s="32"/>
       <c r="D7" s="26" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>at</v>
+        <v/>
       </c>
-      <c r="E7" s="33" t="s">
-        <v>17</v>
-      </c>
+      <c r="E7" s="33"/>
       <c r="F7" s="25"/>
       <c r="G7" s="26" t="str">
         <f ca="1">IF(B7="","","by")</f>
-        <v>by</v>
+        <v/>
       </c>
       <c r="H7" s="27"/>
       <c r="I7" s="6"/>
       <c r="J7" s="7"/>
-      <c r="AA7" s="1">
+      <c r="AA7" s="1" t="str">
         <f ca="1">IF($B7="","",IF(AND($F7&lt;&gt;"H",$F7&lt;&gt;"V"),ROW(),""))</f>
-        <v>7</v>
+        <v/>
       </c>
-      <c r="AB7" s="1">
+      <c r="AB7" s="1" t="str">
         <f ca="1">IF($B7="","",IF($H7&lt;1,ROW(),""))</f>
-        <v>7</v>
+        <v/>
       </c>
       <c r="AC7" s="1">
         <f ca="1">IF($AD7&lt;&gt;"",ROW(),"")</f>
@@ -1352,7 +1332,7 @@
       </c>
       <c r="AD7" s="2" t="str">
         <f ca="1">IF($H$8="",CONCATENATE("Enter your Total Points Prediction for ",OFFSET($C$4,MAX($B4:$B7)-1,0)," at ",OFFSET($E$4,MAX($B4:$B7)-1,0)," (Game ",OFFSET($B$4,MAX($B4:$B7)-1,0),") in cell H8"),"")</f>
-        <v>Enter your Total Points Prediction for Seahawks at Packers (Game 4) in cell H8</v>
+        <v>Enter your Total Points Prediction for Packers at 49ers (Game 2) in cell H8</v>
       </c>
     </row>
     <row r="8" spans="2:51" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1361,7 +1341,7 @@
       <c r="D8" s="17"/>
       <c r="E8" s="18" t="str">
         <f ca="1">CONCATENATE("                   Game ",MAX(B4:B7)," Total")</f>
-        <v xml:space="preserve">                   Game 4 Total</v>
+        <v xml:space="preserve">                   Game 2 Total</v>
       </c>
       <c r="F8" s="17"/>
       <c r="G8" s="37" t="s">

</xml_diff>

<commit_message>
2019 Post Season Week 3 Final update.
</commit_message>
<xml_diff>
--- a/post_season_inputs.xlsx
+++ b/post_season_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2019 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BF8B3F2-E347-446C-81E5-08D1C793F138}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5DD3993-6295-4106-8693-36EB57E570A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" tabRatio="267" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="267" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Post Season Input Form" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>H</t>
   </si>
@@ -64,19 +64,13 @@
     <t xml:space="preserve">Name:  </t>
   </si>
   <si>
-    <t>Titans</t>
-  </si>
-  <si>
     <t>49ers</t>
   </si>
   <si>
     <t>Chiefs</t>
   </si>
   <si>
-    <t>Packers</t>
-  </si>
-  <si>
-    <t>Post Season Week 3 Input Form</t>
+    <t>Post Season Week 4 Input Form</t>
   </si>
 </sst>
 </file>
@@ -1082,7 +1076,7 @@
   <sheetData>
     <row r="1" spans="2:51" s="52" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="53" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C1" s="53"/>
       <c r="D1" s="53"/>
@@ -1196,7 +1190,7 @@
         <v>at</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4" s="19"/>
       <c r="G4" s="20" t="str">
@@ -1224,35 +1218,31 @@
       </c>
     </row>
     <row r="5" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="35">
+      <c r="B5" s="35" t="str">
         <f ca="1">IF(ISTEXT($C5),ROW($B5)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B5)-ROW($B$4),0)),"")</f>
-        <v>2</v>
+        <v/>
       </c>
-      <c r="C5" s="30" t="s">
-        <v>13</v>
-      </c>
+      <c r="C5" s="30"/>
       <c r="D5" s="23" t="str">
         <f t="shared" ref="D5:D7" ca="1" si="0">IF(B5="","","at")</f>
-        <v>at</v>
+        <v/>
       </c>
-      <c r="E5" s="31" t="s">
-        <v>11</v>
-      </c>
+      <c r="E5" s="31"/>
       <c r="F5" s="22"/>
       <c r="G5" s="23" t="str">
         <f ca="1">IF(B5="","","by")</f>
-        <v>by</v>
+        <v/>
       </c>
       <c r="H5" s="24"/>
       <c r="I5" s="3"/>
       <c r="J5" s="5"/>
-      <c r="AA5" s="1">
+      <c r="AA5" s="1" t="str">
         <f ca="1">IF($B5="","",IF(AND($F5&lt;&gt;"H",$F5&lt;&gt;"V"),ROW(),""))</f>
-        <v>5</v>
+        <v/>
       </c>
-      <c r="AB5" s="1">
+      <c r="AB5" s="1" t="str">
         <f ca="1">IF($B5="","",IF($H5&lt;1,ROW(),""))</f>
-        <v>5</v>
+        <v/>
       </c>
       <c r="AC5" s="1">
         <f t="shared" ref="AC5:AC13" ca="1" si="1">IF($AD5&lt;&gt;"",ROW(),"")</f>
@@ -1260,7 +1250,7 @@
       </c>
       <c r="AD5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for the ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for the Titans at Chiefs (Game 1).</v>
+        <v>Pick a winner (V or H) for the 49ers at Chiefs (Game 1).</v>
       </c>
     </row>
     <row r="6" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -1332,7 +1322,7 @@
       </c>
       <c r="AD7" s="2" t="str">
         <f ca="1">IF($H$8="",CONCATENATE("Enter your Total Points Prediction for ",OFFSET($C$4,MAX($B4:$B7)-1,0)," at ",OFFSET($E$4,MAX($B4:$B7)-1,0)," (Game ",OFFSET($B$4,MAX($B4:$B7)-1,0),") in cell H8"),"")</f>
-        <v>Enter your Total Points Prediction for Packers at 49ers (Game 2) in cell H8</v>
+        <v>Enter your Total Points Prediction for 49ers at Chiefs (Game 1) in cell H8</v>
       </c>
     </row>
     <row r="8" spans="2:51" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1341,7 +1331,7 @@
       <c r="D8" s="17"/>
       <c r="E8" s="18" t="str">
         <f ca="1">CONCATENATE("                   Game ",MAX(B4:B7)," Total")</f>
-        <v xml:space="preserve">                   Game 2 Total</v>
+        <v xml:space="preserve">                   Game 1 Total</v>
       </c>
       <c r="F8" s="17"/>
       <c r="G8" s="37" t="s">

</xml_diff>

<commit_message>
Updates for new 2020 NFL Playoff format.
</commit_message>
<xml_diff>
--- a/post_season_inputs.xlsx
+++ b/post_season_inputs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2019 Football Pool Page\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jerry\Desktop\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5DD3993-6295-4106-8693-36EB57E570A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03A80740-620F-4ED8-A862-4DA408C595F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="267" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,13 @@
     <sheet name="Post Season Input Form" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Post Season Input Form'!$B$1:$H$7</definedName>
+    <definedName name="home_teams_column">'Post Season Input Form'!$E$4</definedName>
+    <definedName name="input_form">'Post Season Input Form'!$B$1,'Post Season Input Form'!$D$2,'Post Season Input Form'!$C$4:$C$9,'Post Season Input Form'!$E$4:$E$9,'Post Season Input Form'!$F$4:$F$9,'Post Season Input Form'!$H$4:$H$9,'Post Season Input Form'!$H$10</definedName>
+    <definedName name="name">'Post Season Input Form'!$D$2</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Post Season Input Form'!$B$1:$H$9</definedName>
     <definedName name="Season_total_points">'Post Season Input Form'!#REF!</definedName>
+    <definedName name="title">'Post Season Input Form'!$B$1</definedName>
+    <definedName name="visiting_teams_column">'Post Season Input Form'!$C$4</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>H</t>
   </si>
@@ -64,13 +69,7 @@
     <t xml:space="preserve">Name:  </t>
   </si>
   <si>
-    <t>49ers</t>
-  </si>
-  <si>
-    <t>Chiefs</t>
-  </si>
-  <si>
-    <t>Post Season Week 4 Input Form</t>
+    <t>Post Season Week 1 Input Form</t>
   </si>
 </sst>
 </file>
@@ -1047,7 +1046,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B1:AZ166"/>
+  <dimension ref="B1:AZ168"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -1076,7 +1075,7 @@
   <sheetData>
     <row r="1" spans="2:51" s="52" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="53" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C1" s="53"/>
       <c r="D1" s="53"/>
@@ -1165,48 +1164,44 @@
       <c r="H3" s="49"/>
       <c r="I3" s="3"/>
       <c r="AA3" s="1">
-        <f ca="1">MIN(AA4:AA7)</f>
+        <f ca="1">MIN(AA4:AA9)</f>
+        <v>0</v>
+      </c>
+      <c r="AB3" s="1">
+        <f ca="1">MIN(AB4:AB9)</f>
+        <v>0</v>
+      </c>
+      <c r="AC3" s="1">
+        <f ca="1">MIN(AC4:AC9)</f>
         <v>4</v>
       </c>
-      <c r="AB3" s="1">
-        <f ca="1">MIN(AB4:AB7)</f>
-        <v>4</v>
+    </row>
+    <row r="4" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="34" t="str">
+        <f ca="1">IF(ISTEXT($C4),ROW($B4)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B4)-ROW($B$4),0)),"")</f>
+        <v/>
       </c>
-      <c r="AC3" s="1">
-        <f ca="1">MIN(AC4:AC7)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="34">
-        <f ca="1">IF(ISTEXT($C4),ROW($B4)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B4)-ROW($B$4),0)),"")</f>
-        <v>1</v>
-      </c>
-      <c r="C4" s="28" t="s">
-        <v>10</v>
-      </c>
+      <c r="C4" s="28"/>
       <c r="D4" s="20" t="str">
         <f ca="1">IF(B4="","","at")</f>
-        <v>at</v>
+        <v/>
       </c>
-      <c r="E4" s="29" t="s">
-        <v>11</v>
-      </c>
+      <c r="E4" s="29"/>
       <c r="F4" s="19"/>
       <c r="G4" s="20" t="str">
-        <f ca="1">IF(B4="","","by")</f>
-        <v>by</v>
+        <f t="shared" ref="G4:G9" ca="1" si="0">IF(B4="","","by")</f>
+        <v/>
       </c>
       <c r="H4" s="21"/>
       <c r="I4" s="3"/>
       <c r="J4" s="4"/>
-      <c r="AA4" s="1">
-        <f ca="1">IF($B4="","",IF(AND($F4&lt;&gt;"H",$F4&lt;&gt;"V"),ROW(),""))</f>
-        <v>4</v>
+      <c r="AA4" s="1" t="str">
+        <f t="shared" ref="AA4:AA9" ca="1" si="1">IF($B4="","",IF(AND($F4&lt;&gt;"H",$F4&lt;&gt;"V"),ROW(),""))</f>
+        <v/>
       </c>
-      <c r="AB4" s="1">
-        <f ca="1">IF($B4="","",IF($H4&lt;1,ROW(),""))</f>
-        <v>4</v>
+      <c r="AB4" s="1" t="str">
+        <f t="shared" ref="AB4:AB9" ca="1" si="2">IF($B4="","",IF($H4&lt;1,ROW(),""))</f>
+        <v/>
       </c>
       <c r="AC4" s="1">
         <f>IF($AD4&lt;&gt;"",ROW(),"")</f>
@@ -1224,33 +1219,33 @@
       </c>
       <c r="C5" s="30"/>
       <c r="D5" s="23" t="str">
-        <f t="shared" ref="D5:D7" ca="1" si="0">IF(B5="","","at")</f>
+        <f t="shared" ref="D5" ca="1" si="3">IF(B5="","","at")</f>
         <v/>
       </c>
       <c r="E5" s="31"/>
       <c r="F5" s="22"/>
       <c r="G5" s="23" t="str">
-        <f ca="1">IF(B5="","","by")</f>
+        <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
       <c r="H5" s="24"/>
       <c r="I5" s="3"/>
       <c r="J5" s="5"/>
       <c r="AA5" s="1" t="str">
-        <f ca="1">IF($B5="","",IF(AND($F5&lt;&gt;"H",$F5&lt;&gt;"V"),ROW(),""))</f>
+        <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
       <c r="AB5" s="1" t="str">
-        <f ca="1">IF($B5="","",IF($H5&lt;1,ROW(),""))</f>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
-      <c r="AC5" s="1">
-        <f t="shared" ref="AC5:AC13" ca="1" si="1">IF($AD5&lt;&gt;"",ROW(),"")</f>
-        <v>5</v>
+      <c r="AC5" s="1" t="str">
+        <f t="shared" ref="AC5:AC15" ca="1" si="4">IF($AD5&lt;&gt;"",ROW(),"")</f>
+        <v/>
       </c>
       <c r="AD5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for the ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for the 49ers at Chiefs (Game 1).</v>
+        <v/>
       </c>
     </row>
     <row r="6" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -1260,198 +1255,163 @@
       </c>
       <c r="C6" s="30"/>
       <c r="D6" s="23" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ref="D6" ca="1" si="5">IF(B6="","","at")</f>
         <v/>
       </c>
       <c r="E6" s="31"/>
       <c r="F6" s="22"/>
       <c r="G6" s="23" t="str">
-        <f ca="1">IF(B6="","","by")</f>
+        <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
       <c r="H6" s="24"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="7"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="5"/>
       <c r="AA6" s="1" t="str">
-        <f ca="1">IF($B6="","",IF(AND($F6&lt;&gt;"H",$F6&lt;&gt;"V"),ROW(),""))</f>
+        <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
       <c r="AB6" s="1" t="str">
-        <f ca="1">IF($B6="","",IF($H6&lt;1,ROW(),""))</f>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
-      <c r="AC6" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+      <c r="AC6" s="1" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v/>
       </c>
       <c r="AD6" s="2" t="str">
-        <f ca="1">IF($AB$3&gt;0,CONCATENATE("Enter the predicted margin of victory for the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Enter the predicted margin of victory for the Chiefs (Game 1).</v>
+        <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for the ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
+        <v/>
       </c>
     </row>
-    <row r="7" spans="2:51" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="36" t="str">
+    <row r="7" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="35" t="str">
         <f ca="1">IF(ISTEXT($C7),ROW($B7)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B7)-ROW($B$4),0)),"")</f>
         <v/>
       </c>
-      <c r="C7" s="32"/>
-      <c r="D7" s="26" t="str">
+      <c r="C7" s="30"/>
+      <c r="D7" s="23" t="str">
+        <f t="shared" ref="D7:D9" ca="1" si="6">IF(B7="","","at")</f>
+        <v/>
+      </c>
+      <c r="E7" s="31"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="23" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
-      <c r="E7" s="33"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="26" t="str">
-        <f ca="1">IF(B7="","","by")</f>
-        <v/>
-      </c>
-      <c r="H7" s="27"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="7"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="5"/>
       <c r="AA7" s="1" t="str">
-        <f ca="1">IF($B7="","",IF(AND($F7&lt;&gt;"H",$F7&lt;&gt;"V"),ROW(),""))</f>
+        <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
       <c r="AB7" s="1" t="str">
-        <f ca="1">IF($B7="","",IF($H7&lt;1,ROW(),""))</f>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
-      <c r="AC7" s="1">
-        <f ca="1">IF($AD7&lt;&gt;"",ROW(),"")</f>
-        <v>7</v>
+      <c r="AC7" s="1" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v/>
       </c>
       <c r="AD7" s="2" t="str">
-        <f ca="1">IF($H$8="",CONCATENATE("Enter your Total Points Prediction for ",OFFSET($C$4,MAX($B4:$B7)-1,0)," at ",OFFSET($E$4,MAX($B4:$B7)-1,0)," (Game ",OFFSET($B$4,MAX($B4:$B7)-1,0),") in cell H8"),"")</f>
-        <v>Enter your Total Points Prediction for 49ers at Chiefs (Game 1) in cell H8</v>
+        <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for the ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
+        <v/>
       </c>
     </row>
-    <row r="8" spans="2:51" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="16"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="18" t="str">
-        <f ca="1">CONCATENATE("                   Game ",MAX(B4:B7)," Total")</f>
-        <v xml:space="preserve">                   Game 1 Total</v>
+    <row r="8" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="35" t="str">
+        <f ca="1">IF(ISTEXT($C8),ROW($B8)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B8)-ROW($B$4),0)),"")</f>
+        <v/>
       </c>
-      <c r="F8" s="17"/>
-      <c r="G8" s="37" t="s">
+      <c r="C8" s="30"/>
+      <c r="D8" s="23" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v/>
+      </c>
+      <c r="E8" s="31"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="23" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="H8" s="24"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="7"/>
+      <c r="AA8" s="1" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="AB8" s="1" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+      <c r="AC8" s="1" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v/>
+      </c>
+      <c r="AD8" s="2" t="str">
+        <f ca="1">IF($AB$3&gt;0,CONCATENATE("Enter the predicted margin of victory for the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="2:51" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="36" t="str">
+        <f ca="1">IF(ISTEXT($C9),ROW($B9)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B9)-ROW($B$4),0)),"")</f>
+        <v/>
+      </c>
+      <c r="C9" s="32"/>
+      <c r="D9" s="26" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v/>
+      </c>
+      <c r="E9" s="33"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="26" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="H9" s="27"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="7"/>
+      <c r="AA9" s="1" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="AB9" s="1" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+      <c r="AC9" s="1">
+        <f ca="1">IF($AD9&lt;&gt;"",ROW(),"")</f>
+        <v>9</v>
+      </c>
+      <c r="AD9" s="2" t="str">
+        <f ca="1">IF($H$10="",CONCATENATE("Enter your Total Points Prediction for ",OFFSET($C$4,MAX($B4:$B9)-1,0)," at ",OFFSET($E$4,MAX($B4:$B9)-1,0)," (Game ",OFFSET($B$4,MAX($B4:$B9)-1,0),") in cell H10"),"")</f>
+        <v>Enter your Total Points Prediction for Visitor at Home (Game Game) in cell H10</v>
+      </c>
+    </row>
+    <row r="10" spans="2:51" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="16"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="18" t="str">
+        <f ca="1">CONCATENATE("                   Game ",MAX(B4:B9)," Total")</f>
+        <v xml:space="preserve">                   Game 0 Total</v>
+      </c>
+      <c r="F10" s="17"/>
+      <c r="G10" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="H8" s="38"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="7"/>
-    </row>
-    <row r="9" spans="2:51" s="8" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G9" s="9"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="1"/>
-      <c r="S9" s="1"/>
-      <c r="T9" s="1"/>
-      <c r="U9" s="1"/>
-      <c r="V9" s="1"/>
-      <c r="W9" s="1"/>
-      <c r="X9" s="1"/>
-      <c r="Y9" s="1"/>
-      <c r="Z9" s="1"/>
-      <c r="AA9" s="1"/>
-      <c r="AB9" s="1"/>
-      <c r="AC9" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AD9" s="2"/>
-      <c r="AE9" s="1" t="str">
-        <f ca="1">IF($AB$3&gt;0,(IF($AN$4&lt;&gt;"",IF($AN$4:$AN$4="",$AN$4,CONCATENATE(" and ",$AN$4)),"")),"")</f>
-        <v/>
-      </c>
-      <c r="AF9" s="1"/>
-      <c r="AG9" s="1"/>
-      <c r="AH9" s="1"/>
-      <c r="AI9" s="1"/>
-      <c r="AJ9" s="1"/>
-      <c r="AK9" s="1"/>
-      <c r="AL9" s="1"/>
-      <c r="AM9" s="1"/>
-      <c r="AN9" s="1"/>
-      <c r="AO9" s="2"/>
-      <c r="AP9" s="1"/>
-      <c r="AQ9" s="1"/>
-      <c r="AR9" s="1"/>
-      <c r="AS9" s="1"/>
-      <c r="AT9" s="1"/>
-      <c r="AU9" s="1"/>
-      <c r="AV9" s="1"/>
-      <c r="AW9" s="1"/>
-      <c r="AX9" s="1"/>
-      <c r="AY9" s="1"/>
-    </row>
-    <row r="10" spans="2:51" s="8" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="14" t="str">
-        <f ca="1">IF(COUNTIF($AA$3:$AC$3,"&gt;0"),"Input Form Error:","")</f>
-        <v>Input Form Error:</v>
-      </c>
-      <c r="I10" s="3"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="6"/>
       <c r="J10" s="7"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
-      <c r="S10" s="1"/>
-      <c r="T10" s="1"/>
-      <c r="U10" s="1"/>
-      <c r="V10" s="1"/>
-      <c r="W10" s="1"/>
-      <c r="X10" s="1"/>
-      <c r="Y10" s="1"/>
-      <c r="Z10" s="1"/>
-      <c r="AA10" s="1"/>
-      <c r="AB10" s="1"/>
-      <c r="AC10" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AD10" s="2"/>
-      <c r="AE10" s="1"/>
-      <c r="AF10" s="1"/>
-      <c r="AG10" s="1"/>
-      <c r="AH10" s="1"/>
-      <c r="AI10" s="1"/>
-      <c r="AJ10" s="1"/>
-      <c r="AK10" s="1"/>
-      <c r="AL10" s="1"/>
-      <c r="AM10" s="1"/>
-      <c r="AN10" s="1"/>
-      <c r="AO10" s="2"/>
-      <c r="AP10" s="1"/>
-      <c r="AQ10" s="1"/>
-      <c r="AR10" s="1"/>
-      <c r="AS10" s="1"/>
-      <c r="AT10" s="1"/>
-      <c r="AU10" s="1"/>
-      <c r="AV10" s="1"/>
-      <c r="AW10" s="1"/>
-      <c r="AX10" s="1"/>
-      <c r="AY10" s="1"/>
     </row>
     <row r="11" spans="2:51" s="8" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="15" t="str">
-        <f ca="1">IF($AC$3&gt;0,OFFSET($AD$4,$AC$3-ROW($B$4),0),"")</f>
-        <v>Enter your name in cell D2.</v>
-      </c>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
+      <c r="G11" s="9"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="7"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
@@ -1471,11 +1431,14 @@
       <c r="AA11" s="1"/>
       <c r="AB11" s="1"/>
       <c r="AC11" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="AD11" s="2"/>
-      <c r="AE11" s="1"/>
+      <c r="AE11" s="1" t="str">
+        <f ca="1">IF($AB$3&gt;0,(IF($AN$4&lt;&gt;"",IF($AN$4:$AN$4="",$AN$4,CONCATENATE(" and ",$AN$4)),"")),"")</f>
+        <v/>
+      </c>
       <c r="AF11" s="1"/>
       <c r="AG11" s="1"/>
       <c r="AH11" s="1"/>
@@ -1498,8 +1461,12 @@
       <c r="AY11" s="1"/>
     </row>
     <row r="12" spans="2:51" s="8" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
+      <c r="B12" s="14" t="str">
+        <f ca="1">IF(COUNTIF($AA$3:$AC$3,"&gt;0"),"Input Form Error:","")</f>
+        <v>Input Form Error:</v>
+      </c>
+      <c r="I12" s="3"/>
+      <c r="J12" s="7"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
@@ -1519,7 +1486,7 @@
       <c r="AA12" s="1"/>
       <c r="AB12" s="1"/>
       <c r="AC12" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="AD12" s="2"/>
@@ -1546,6 +1513,10 @@
       <c r="AY12" s="1"/>
     </row>
     <row r="13" spans="2:51" s="8" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="15" t="str">
+        <f ca="1">IF($AC$3&gt;0,OFFSET($AD$4,$AC$3-ROW($B$4),0),"")</f>
+        <v>Enter your name in cell D2.</v>
+      </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
@@ -1567,7 +1538,7 @@
       <c r="AA13" s="1"/>
       <c r="AB13" s="1"/>
       <c r="AC13" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="AD13" s="2"/>
@@ -1615,7 +1586,7 @@
       <c r="AA14" s="1"/>
       <c r="AB14" s="1"/>
       <c r="AC14" s="1" t="str">
-        <f>IF($AD14&lt;&gt;"",ROW(),"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="AD14" s="2"/>
@@ -1663,7 +1634,7 @@
       <c r="AA15" s="1"/>
       <c r="AB15" s="1"/>
       <c r="AC15" s="1" t="str">
-        <f>IF($AD15&lt;&gt;"",ROW(),"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="AD15" s="2"/>
@@ -1692,9 +1663,7 @@
     <row r="16" spans="2:51" s="8" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
-      <c r="K16" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
@@ -1790,7 +1759,9 @@
     <row r="18" spans="2:51" s="8" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
+      <c r="K18" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
@@ -1856,7 +1827,10 @@
       <c r="Z19" s="1"/>
       <c r="AA19" s="1"/>
       <c r="AB19" s="1"/>
-      <c r="AC19" s="1"/>
+      <c r="AC19" s="1" t="str">
+        <f>IF($AD19&lt;&gt;"",ROW(),"")</f>
+        <v/>
+      </c>
       <c r="AD19" s="2"/>
       <c r="AE19" s="1"/>
       <c r="AF19" s="1"/>
@@ -1901,7 +1875,10 @@
       <c r="Z20" s="1"/>
       <c r="AA20" s="1"/>
       <c r="AB20" s="1"/>
-      <c r="AC20" s="1"/>
+      <c r="AC20" s="1" t="str">
+        <f>IF($AD20&lt;&gt;"",ROW(),"")</f>
+        <v/>
+      </c>
       <c r="AD20" s="2"/>
       <c r="AE20" s="1"/>
       <c r="AF20" s="1"/>
@@ -1925,102 +1902,100 @@
       <c r="AX20" s="1"/>
       <c r="AY20" s="1"/>
     </row>
-    <row r="21" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="8"/>
-      <c r="AC21" s="11"/>
-      <c r="AD21" s="11"/>
-    </row>
-    <row r="22" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="11"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="11"/>
-      <c r="L22" s="11"/>
-      <c r="M22" s="11"/>
-      <c r="N22" s="11"/>
-      <c r="O22" s="11"/>
-      <c r="P22" s="11"/>
-      <c r="Q22" s="11"/>
-      <c r="R22" s="11"/>
-      <c r="S22" s="11"/>
-      <c r="T22" s="11"/>
-      <c r="U22" s="11"/>
-      <c r="V22" s="11"/>
-      <c r="W22" s="11"/>
-      <c r="X22" s="11"/>
-      <c r="Y22" s="11"/>
-      <c r="Z22" s="11"/>
-      <c r="AA22" s="11"/>
-      <c r="AB22" s="11"/>
-      <c r="AC22" s="11"/>
-      <c r="AD22" s="11"/>
-      <c r="AE22" s="11"/>
-      <c r="AF22" s="11"/>
-      <c r="AG22" s="11"/>
-      <c r="AH22" s="11"/>
-      <c r="AI22" s="11"/>
-      <c r="AJ22" s="11"/>
-      <c r="AK22" s="11"/>
-      <c r="AL22" s="11"/>
-      <c r="AM22" s="11"/>
-      <c r="AN22" s="11"/>
-      <c r="AO22" s="11"/>
-      <c r="AP22" s="11"/>
-      <c r="AQ22" s="11"/>
-      <c r="AR22" s="11"/>
-      <c r="AS22" s="11"/>
-      <c r="AT22" s="11"/>
-      <c r="AU22" s="11"/>
-      <c r="AV22" s="11"/>
-      <c r="AW22" s="11"/>
-      <c r="AX22" s="11"/>
-      <c r="AY22" s="11"/>
+    <row r="21" spans="2:51" s="8" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
+      <c r="T21" s="1"/>
+      <c r="U21" s="1"/>
+      <c r="V21" s="1"/>
+      <c r="W21" s="1"/>
+      <c r="X21" s="1"/>
+      <c r="Y21" s="1"/>
+      <c r="Z21" s="1"/>
+      <c r="AA21" s="1"/>
+      <c r="AB21" s="1"/>
+      <c r="AC21" s="1"/>
+      <c r="AD21" s="2"/>
+      <c r="AE21" s="1"/>
+      <c r="AF21" s="1"/>
+      <c r="AG21" s="1"/>
+      <c r="AH21" s="1"/>
+      <c r="AI21" s="1"/>
+      <c r="AJ21" s="1"/>
+      <c r="AK21" s="1"/>
+      <c r="AL21" s="1"/>
+      <c r="AM21" s="1"/>
+      <c r="AN21" s="1"/>
+      <c r="AO21" s="2"/>
+      <c r="AP21" s="1"/>
+      <c r="AQ21" s="1"/>
+      <c r="AR21" s="1"/>
+      <c r="AS21" s="1"/>
+      <c r="AT21" s="1"/>
+      <c r="AU21" s="1"/>
+      <c r="AV21" s="1"/>
+      <c r="AW21" s="1"/>
+      <c r="AX21" s="1"/>
+      <c r="AY21" s="1"/>
+    </row>
+    <row r="22" spans="2:51" s="8" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
+      <c r="S22" s="1"/>
+      <c r="T22" s="1"/>
+      <c r="U22" s="1"/>
+      <c r="V22" s="1"/>
+      <c r="W22" s="1"/>
+      <c r="X22" s="1"/>
+      <c r="Y22" s="1"/>
+      <c r="Z22" s="1"/>
+      <c r="AA22" s="1"/>
+      <c r="AB22" s="1"/>
+      <c r="AC22" s="1"/>
+      <c r="AD22" s="2"/>
+      <c r="AE22" s="1"/>
+      <c r="AF22" s="1"/>
+      <c r="AG22" s="1"/>
+      <c r="AH22" s="1"/>
+      <c r="AI22" s="1"/>
+      <c r="AJ22" s="1"/>
+      <c r="AK22" s="1"/>
+      <c r="AL22" s="1"/>
+      <c r="AM22" s="1"/>
+      <c r="AN22" s="1"/>
+      <c r="AO22" s="2"/>
+      <c r="AP22" s="1"/>
+      <c r="AQ22" s="1"/>
+      <c r="AR22" s="1"/>
+      <c r="AS22" s="1"/>
+      <c r="AT22" s="1"/>
+      <c r="AU22" s="1"/>
+      <c r="AV22" s="1"/>
+      <c r="AW22" s="1"/>
+      <c r="AX22" s="1"/>
+      <c r="AY22" s="1"/>
     </row>
     <row r="23" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="11"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="11"/>
-      <c r="K23" s="11"/>
-      <c r="L23" s="11"/>
-      <c r="M23" s="11"/>
-      <c r="N23" s="11"/>
-      <c r="O23" s="11"/>
-      <c r="P23" s="11"/>
-      <c r="Q23" s="11"/>
-      <c r="R23" s="11"/>
-      <c r="S23" s="11"/>
-      <c r="T23" s="11"/>
-      <c r="U23" s="11"/>
-      <c r="V23" s="11"/>
-      <c r="W23" s="11"/>
-      <c r="X23" s="11"/>
-      <c r="Y23" s="11"/>
-      <c r="Z23" s="11"/>
-      <c r="AA23" s="11"/>
-      <c r="AB23" s="11"/>
+      <c r="B23" s="8"/>
       <c r="AC23" s="11"/>
       <c r="AD23" s="11"/>
-      <c r="AE23" s="11"/>
-      <c r="AF23" s="11"/>
-      <c r="AG23" s="11"/>
-      <c r="AH23" s="11"/>
-      <c r="AI23" s="11"/>
-      <c r="AJ23" s="11"/>
-      <c r="AK23" s="11"/>
-      <c r="AL23" s="11"/>
-      <c r="AM23" s="11"/>
-      <c r="AN23" s="11"/>
-      <c r="AO23" s="11"/>
-      <c r="AP23" s="11"/>
-      <c r="AQ23" s="11"/>
-      <c r="AR23" s="11"/>
-      <c r="AS23" s="11"/>
-      <c r="AT23" s="11"/>
-      <c r="AU23" s="11"/>
-      <c r="AV23" s="11"/>
-      <c r="AW23" s="11"/>
-      <c r="AX23" s="11"/>
-      <c r="AY23" s="11"/>
     </row>
     <row r="24" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="11"/>
@@ -2044,7 +2019,8 @@
       <c r="Z24" s="11"/>
       <c r="AA24" s="11"/>
       <c r="AB24" s="11"/>
-      <c r="AD24" s="1"/>
+      <c r="AC24" s="11"/>
+      <c r="AD24" s="11"/>
       <c r="AE24" s="11"/>
       <c r="AF24" s="11"/>
       <c r="AG24" s="11"/>
@@ -2068,12 +2044,95 @@
       <c r="AY24" s="11"/>
     </row>
     <row r="25" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AD25" s="1"/>
-      <c r="AO25" s="1"/>
+      <c r="B25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="11"/>
+      <c r="N25" s="11"/>
+      <c r="O25" s="11"/>
+      <c r="P25" s="11"/>
+      <c r="Q25" s="11"/>
+      <c r="R25" s="11"/>
+      <c r="S25" s="11"/>
+      <c r="T25" s="11"/>
+      <c r="U25" s="11"/>
+      <c r="V25" s="11"/>
+      <c r="W25" s="11"/>
+      <c r="X25" s="11"/>
+      <c r="Y25" s="11"/>
+      <c r="Z25" s="11"/>
+      <c r="AA25" s="11"/>
+      <c r="AB25" s="11"/>
+      <c r="AC25" s="11"/>
+      <c r="AD25" s="11"/>
+      <c r="AE25" s="11"/>
+      <c r="AF25" s="11"/>
+      <c r="AG25" s="11"/>
+      <c r="AH25" s="11"/>
+      <c r="AI25" s="11"/>
+      <c r="AJ25" s="11"/>
+      <c r="AK25" s="11"/>
+      <c r="AL25" s="11"/>
+      <c r="AM25" s="11"/>
+      <c r="AN25" s="11"/>
+      <c r="AO25" s="11"/>
+      <c r="AP25" s="11"/>
+      <c r="AQ25" s="11"/>
+      <c r="AR25" s="11"/>
+      <c r="AS25" s="11"/>
+      <c r="AT25" s="11"/>
+      <c r="AU25" s="11"/>
+      <c r="AV25" s="11"/>
+      <c r="AW25" s="11"/>
+      <c r="AX25" s="11"/>
+      <c r="AY25" s="11"/>
     </row>
     <row r="26" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="11"/>
+      <c r="M26" s="11"/>
+      <c r="N26" s="11"/>
+      <c r="O26" s="11"/>
+      <c r="P26" s="11"/>
+      <c r="Q26" s="11"/>
+      <c r="R26" s="11"/>
+      <c r="S26" s="11"/>
+      <c r="T26" s="11"/>
+      <c r="U26" s="11"/>
+      <c r="V26" s="11"/>
+      <c r="W26" s="11"/>
+      <c r="X26" s="11"/>
+      <c r="Y26" s="11"/>
+      <c r="Z26" s="11"/>
+      <c r="AA26" s="11"/>
+      <c r="AB26" s="11"/>
       <c r="AD26" s="1"/>
-      <c r="AO26" s="1"/>
+      <c r="AE26" s="11"/>
+      <c r="AF26" s="11"/>
+      <c r="AG26" s="11"/>
+      <c r="AH26" s="11"/>
+      <c r="AI26" s="11"/>
+      <c r="AJ26" s="11"/>
+      <c r="AK26" s="11"/>
+      <c r="AL26" s="11"/>
+      <c r="AM26" s="11"/>
+      <c r="AN26" s="11"/>
+      <c r="AO26" s="11"/>
+      <c r="AP26" s="11"/>
+      <c r="AQ26" s="11"/>
+      <c r="AR26" s="11"/>
+      <c r="AS26" s="11"/>
+      <c r="AT26" s="11"/>
+      <c r="AU26" s="11"/>
+      <c r="AV26" s="11"/>
+      <c r="AW26" s="11"/>
+      <c r="AX26" s="11"/>
+      <c r="AY26" s="11"/>
     </row>
     <row r="27" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AD27" s="1"/>
@@ -2092,96 +2151,12 @@
       <c r="AO30" s="1"/>
     </row>
     <row r="31" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="12"/>
-      <c r="I31" s="12"/>
-      <c r="J31" s="12"/>
-      <c r="K31" s="12"/>
-      <c r="L31" s="12"/>
-      <c r="M31" s="12"/>
-      <c r="N31" s="12"/>
-      <c r="O31" s="12"/>
-      <c r="P31" s="12"/>
-      <c r="Q31" s="12"/>
-      <c r="R31" s="12"/>
-      <c r="S31" s="12"/>
-      <c r="T31" s="12"/>
-      <c r="U31" s="12"/>
-      <c r="V31" s="12"/>
-      <c r="W31" s="12"/>
-      <c r="X31" s="12"/>
-      <c r="Y31" s="12"/>
-      <c r="Z31" s="12"/>
-      <c r="AA31" s="12"/>
-      <c r="AB31" s="12"/>
-      <c r="AC31" s="12"/>
-      <c r="AD31" s="12"/>
-      <c r="AE31" s="12"/>
-      <c r="AF31" s="12"/>
-      <c r="AG31" s="12"/>
-      <c r="AH31" s="12"/>
-      <c r="AI31" s="12"/>
-      <c r="AJ31" s="12"/>
-      <c r="AK31" s="12"/>
-      <c r="AL31" s="12"/>
-      <c r="AM31" s="12"/>
-      <c r="AN31" s="12"/>
-      <c r="AO31" s="12"/>
-      <c r="AP31" s="12"/>
-      <c r="AQ31" s="12"/>
-      <c r="AR31" s="12"/>
-      <c r="AS31" s="12"/>
-      <c r="AT31" s="12"/>
-      <c r="AU31" s="12"/>
-      <c r="AV31" s="12"/>
-      <c r="AW31" s="12"/>
-      <c r="AX31" s="12"/>
-      <c r="AY31" s="12"/>
+      <c r="AD31" s="1"/>
+      <c r="AO31" s="1"/>
     </row>
     <row r="32" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="12"/>
-      <c r="I32" s="12"/>
-      <c r="J32" s="12"/>
-      <c r="K32" s="12"/>
-      <c r="L32" s="12"/>
-      <c r="M32" s="12"/>
-      <c r="N32" s="12"/>
-      <c r="O32" s="12"/>
-      <c r="P32" s="12"/>
-      <c r="Q32" s="12"/>
-      <c r="R32" s="12"/>
-      <c r="S32" s="12"/>
-      <c r="T32" s="12"/>
-      <c r="U32" s="12"/>
-      <c r="V32" s="12"/>
-      <c r="W32" s="12"/>
-      <c r="X32" s="12"/>
-      <c r="Y32" s="12"/>
-      <c r="Z32" s="12"/>
-      <c r="AA32" s="12"/>
-      <c r="AB32" s="12"/>
-      <c r="AC32" s="12"/>
-      <c r="AD32" s="12"/>
-      <c r="AE32" s="12"/>
-      <c r="AF32" s="12"/>
-      <c r="AG32" s="12"/>
-      <c r="AH32" s="12"/>
-      <c r="AI32" s="12"/>
-      <c r="AJ32" s="12"/>
-      <c r="AK32" s="12"/>
-      <c r="AL32" s="12"/>
-      <c r="AM32" s="12"/>
-      <c r="AN32" s="12"/>
-      <c r="AO32" s="12"/>
-      <c r="AP32" s="12"/>
-      <c r="AQ32" s="12"/>
-      <c r="AR32" s="12"/>
-      <c r="AS32" s="12"/>
-      <c r="AT32" s="12"/>
-      <c r="AU32" s="12"/>
-      <c r="AV32" s="12"/>
-      <c r="AW32" s="12"/>
-      <c r="AX32" s="12"/>
-      <c r="AY32" s="12"/>
+      <c r="AD32" s="1"/>
+      <c r="AO32" s="1"/>
     </row>
     <row r="33" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="12"/>
@@ -4552,7 +4527,7 @@
       <c r="AA84" s="12"/>
       <c r="AB84" s="12"/>
       <c r="AC84" s="12"/>
-      <c r="AD84" s="13"/>
+      <c r="AD84" s="12"/>
       <c r="AE84" s="12"/>
       <c r="AF84" s="12"/>
       <c r="AG84" s="12"/>
@@ -4576,7 +4551,7 @@
       <c r="AY84" s="12"/>
     </row>
     <row r="85" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B85" s="8"/>
+      <c r="B85" s="12"/>
       <c r="I85" s="12"/>
       <c r="J85" s="12"/>
       <c r="K85" s="12"/>
@@ -4598,7 +4573,7 @@
       <c r="AA85" s="12"/>
       <c r="AB85" s="12"/>
       <c r="AC85" s="12"/>
-      <c r="AD85" s="13"/>
+      <c r="AD85" s="12"/>
       <c r="AE85" s="12"/>
       <c r="AF85" s="12"/>
       <c r="AG85" s="12"/>
@@ -4609,7 +4584,7 @@
       <c r="AL85" s="12"/>
       <c r="AM85" s="12"/>
       <c r="AN85" s="12"/>
-      <c r="AO85" s="13"/>
+      <c r="AO85" s="12"/>
       <c r="AP85" s="12"/>
       <c r="AQ85" s="12"/>
       <c r="AR85" s="12"/>
@@ -4622,7 +4597,7 @@
       <c r="AY85" s="12"/>
     </row>
     <row r="86" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B86" s="8"/>
+      <c r="B86" s="12"/>
       <c r="I86" s="12"/>
       <c r="J86" s="12"/>
       <c r="K86" s="12"/>
@@ -4655,7 +4630,7 @@
       <c r="AL86" s="12"/>
       <c r="AM86" s="12"/>
       <c r="AN86" s="12"/>
-      <c r="AO86" s="13"/>
+      <c r="AO86" s="12"/>
       <c r="AP86" s="12"/>
       <c r="AQ86" s="12"/>
       <c r="AR86" s="12"/>
@@ -4667,7 +4642,7 @@
       <c r="AX86" s="12"/>
       <c r="AY86" s="12"/>
     </row>
-    <row r="87" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B87" s="8"/>
       <c r="I87" s="12"/>
       <c r="J87" s="12"/>
@@ -4713,7 +4688,7 @@
       <c r="AX87" s="12"/>
       <c r="AY87" s="12"/>
     </row>
-    <row r="88" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B88" s="8"/>
       <c r="I88" s="12"/>
       <c r="J88" s="12"/>
@@ -8323,6 +8298,8 @@
       <c r="Z166" s="12"/>
       <c r="AA166" s="12"/>
       <c r="AB166" s="12"/>
+      <c r="AC166" s="12"/>
+      <c r="AD166" s="13"/>
       <c r="AE166" s="12"/>
       <c r="AF166" s="12"/>
       <c r="AG166" s="12"/>
@@ -8345,6 +8322,96 @@
       <c r="AX166" s="12"/>
       <c r="AY166" s="12"/>
     </row>
+    <row r="167" spans="2:51" x14ac:dyDescent="0.2">
+      <c r="B167" s="8"/>
+      <c r="I167" s="12"/>
+      <c r="J167" s="12"/>
+      <c r="K167" s="12"/>
+      <c r="L167" s="12"/>
+      <c r="M167" s="12"/>
+      <c r="N167" s="12"/>
+      <c r="O167" s="12"/>
+      <c r="P167" s="12"/>
+      <c r="Q167" s="12"/>
+      <c r="R167" s="12"/>
+      <c r="S167" s="12"/>
+      <c r="T167" s="12"/>
+      <c r="U167" s="12"/>
+      <c r="V167" s="12"/>
+      <c r="W167" s="12"/>
+      <c r="X167" s="12"/>
+      <c r="Y167" s="12"/>
+      <c r="Z167" s="12"/>
+      <c r="AA167" s="12"/>
+      <c r="AB167" s="12"/>
+      <c r="AC167" s="12"/>
+      <c r="AD167" s="13"/>
+      <c r="AE167" s="12"/>
+      <c r="AF167" s="12"/>
+      <c r="AG167" s="12"/>
+      <c r="AH167" s="12"/>
+      <c r="AI167" s="12"/>
+      <c r="AJ167" s="12"/>
+      <c r="AK167" s="12"/>
+      <c r="AL167" s="12"/>
+      <c r="AM167" s="12"/>
+      <c r="AN167" s="12"/>
+      <c r="AO167" s="13"/>
+      <c r="AP167" s="12"/>
+      <c r="AQ167" s="12"/>
+      <c r="AR167" s="12"/>
+      <c r="AS167" s="12"/>
+      <c r="AT167" s="12"/>
+      <c r="AU167" s="12"/>
+      <c r="AV167" s="12"/>
+      <c r="AW167" s="12"/>
+      <c r="AX167" s="12"/>
+      <c r="AY167" s="12"/>
+    </row>
+    <row r="168" spans="2:51" x14ac:dyDescent="0.2">
+      <c r="B168" s="8"/>
+      <c r="I168" s="12"/>
+      <c r="J168" s="12"/>
+      <c r="K168" s="12"/>
+      <c r="L168" s="12"/>
+      <c r="M168" s="12"/>
+      <c r="N168" s="12"/>
+      <c r="O168" s="12"/>
+      <c r="P168" s="12"/>
+      <c r="Q168" s="12"/>
+      <c r="R168" s="12"/>
+      <c r="S168" s="12"/>
+      <c r="T168" s="12"/>
+      <c r="U168" s="12"/>
+      <c r="V168" s="12"/>
+      <c r="W168" s="12"/>
+      <c r="X168" s="12"/>
+      <c r="Y168" s="12"/>
+      <c r="Z168" s="12"/>
+      <c r="AA168" s="12"/>
+      <c r="AB168" s="12"/>
+      <c r="AE168" s="12"/>
+      <c r="AF168" s="12"/>
+      <c r="AG168" s="12"/>
+      <c r="AH168" s="12"/>
+      <c r="AI168" s="12"/>
+      <c r="AJ168" s="12"/>
+      <c r="AK168" s="12"/>
+      <c r="AL168" s="12"/>
+      <c r="AM168" s="12"/>
+      <c r="AN168" s="12"/>
+      <c r="AO168" s="13"/>
+      <c r="AP168" s="12"/>
+      <c r="AQ168" s="12"/>
+      <c r="AR168" s="12"/>
+      <c r="AS168" s="12"/>
+      <c r="AT168" s="12"/>
+      <c r="AU168" s="12"/>
+      <c r="AV168" s="12"/>
+      <c r="AW168" s="12"/>
+      <c r="AX168" s="12"/>
+      <c r="AY168" s="12"/>
+    </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
@@ -8352,15 +8419,15 @@
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations count="4">
-    <dataValidation type="whole" allowBlank="1" showErrorMessage="1" errorTitle="PREDICTION" error="Enter a number between 1 and 99 for the predicted margin of victory._x000a__x000a_If there are no teams listed in this row, then your only choice is to leave this cell blank._x000a_" sqref="H4:H7" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="whole" allowBlank="1" showErrorMessage="1" errorTitle="PREDICTION" error="Enter a number between 1 and 99 for the predicted margin of victory._x000a__x000a_If there are no teams listed in this row, then your only choice is to leave this cell blank._x000a_" sqref="H4:H9" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>IF(B4="","",1)</formula1>
       <formula2>IF(B4="","",99)</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showErrorMessage="1" errorTitle="Total Points Prediction" error="Enter a number between 1 and 99 for your Total Points Prediction._x000a_" sqref="H8" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="whole" allowBlank="1" showErrorMessage="1" errorTitle="Total Points Prediction" error="Enter a number between 1 and 99 for your Total Points Prediction._x000a_" sqref="H10" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>IF(B4="","",1)</formula1>
       <formula2>IF(B4="","",99)</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="PREDICTION" error="Pick a winner._x000a__x000a_Enter &quot;H&quot; for the home team or &quot;V&quot; for the visiting team._x000a__x000a_If there are no teams listed in this row, then your only choice is to leave this cell blank._x000a_" sqref="F4:F7" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="PREDICTION" error="Pick a winner._x000a__x000a_Enter &quot;H&quot; for the home team or &quot;V&quot; for the visiting team._x000a__x000a_If there are no teams listed in this row, then your only choice is to leave this cell blank._x000a_" sqref="F4:F9" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>IF($B4="",$AC$2:$AC$2,$AA$2:$AB$2)</formula1>
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" showErrorMessage="1" errorTitle="NAME:" error="Your name must include at least 2 non-blank characters." sqref="D2" xr:uid="{00000000-0002-0000-0000-000003000000}">

</xml_diff>

<commit_message>
2020 Week 17 Preliminary update.
</commit_message>
<xml_diff>
--- a/post_season_inputs.xlsx
+++ b/post_season_inputs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jerry\Desktop\Test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2020 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03A80740-620F-4ED8-A862-4DA408C595F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2581E1B2-86EC-4A68-AEC7-2D9B34088114}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="267" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,14 +25,6 @@
     <definedName name="visiting_teams_column">'Post Season Input Form'!$C$4</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -1052,13 +1044,13 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="4.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="6.7109375" style="1" customWidth="1"/>
     <col min="7" max="7" width="4.7109375" style="1" customWidth="1"/>
     <col min="8" max="8" width="6.7109375" style="10" customWidth="1"/>
@@ -1073,7 +1065,7 @@
     <col min="53" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:51" s="52" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:51" s="52" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="53" t="s">
         <v>10</v>
       </c>
@@ -1127,7 +1119,7 @@
       <c r="AX1" s="50"/>
       <c r="AY1" s="50"/>
     </row>
-    <row r="2" spans="2:51" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:51" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="39"/>
       <c r="C2" s="40" t="s">
         <v>9</v>
@@ -1137,6 +1129,10 @@
       <c r="F2" s="42"/>
       <c r="G2" s="43"/>
       <c r="H2" s="44"/>
+      <c r="J2" s="14" t="str">
+        <f ca="1">IF(COUNTIF($AA$3:$AC$3,"&gt;0"),"Input Form Error:","")</f>
+        <v>Input Form Error:</v>
+      </c>
       <c r="AA2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1144,7 +1140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:51" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:51" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="45" t="s">
         <v>4</v>
       </c>
@@ -1163,6 +1159,10 @@
       </c>
       <c r="H3" s="49"/>
       <c r="I3" s="3"/>
+      <c r="J3" s="15" t="str">
+        <f ca="1">IF($AC$3&gt;0,OFFSET($AD$4,$AC$3-ROW($B$4),0),"")</f>
+        <v>Enter your name in cell D2.</v>
+      </c>
       <c r="AA3" s="1">
         <f ca="1">MIN(AA4:AA9)</f>
         <v>0</v>
@@ -1392,7 +1392,7 @@
         <v>Enter your Total Points Prediction for Visitor at Home (Game Game) in cell H10</v>
       </c>
     </row>
-    <row r="10" spans="2:51" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:51" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="16"/>
       <c r="C10" s="17"/>
       <c r="D10" s="17"/>
@@ -1461,10 +1461,6 @@
       <c r="AY11" s="1"/>
     </row>
     <row r="12" spans="2:51" s="8" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="14" t="str">
-        <f ca="1">IF(COUNTIF($AA$3:$AC$3,"&gt;0"),"Input Form Error:","")</f>
-        <v>Input Form Error:</v>
-      </c>
       <c r="I12" s="3"/>
       <c r="J12" s="7"/>
       <c r="K12" s="1"/>
@@ -1513,10 +1509,6 @@
       <c r="AY12" s="1"/>
     </row>
     <row r="13" spans="2:51" s="8" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="15" t="str">
-        <f ca="1">IF($AC$3&gt;0,OFFSET($AD$4,$AC$3-ROW($B$4),0),"")</f>
-        <v>Enter your name in cell D2.</v>
-      </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
@@ -4734,7 +4726,7 @@
       <c r="AX88" s="12"/>
       <c r="AY88" s="12"/>
     </row>
-    <row r="89" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B89" s="8"/>
       <c r="I89" s="12"/>
       <c r="J89" s="12"/>
@@ -4780,7 +4772,7 @@
       <c r="AX89" s="12"/>
       <c r="AY89" s="12"/>
     </row>
-    <row r="90" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B90" s="8"/>
       <c r="I90" s="12"/>
       <c r="J90" s="12"/>
@@ -4826,7 +4818,7 @@
       <c r="AX90" s="12"/>
       <c r="AY90" s="12"/>
     </row>
-    <row r="91" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B91" s="8"/>
       <c r="I91" s="12"/>
       <c r="J91" s="12"/>
@@ -4872,7 +4864,7 @@
       <c r="AX91" s="12"/>
       <c r="AY91" s="12"/>
     </row>
-    <row r="92" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B92" s="8"/>
       <c r="I92" s="12"/>
       <c r="J92" s="12"/>
@@ -4918,7 +4910,7 @@
       <c r="AX92" s="12"/>
       <c r="AY92" s="12"/>
     </row>
-    <row r="93" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B93" s="8"/>
       <c r="I93" s="12"/>
       <c r="J93" s="12"/>
@@ -4964,7 +4956,7 @@
       <c r="AX93" s="12"/>
       <c r="AY93" s="12"/>
     </row>
-    <row r="94" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B94" s="8"/>
       <c r="I94" s="12"/>
       <c r="J94" s="12"/>
@@ -5010,7 +5002,7 @@
       <c r="AX94" s="12"/>
       <c r="AY94" s="12"/>
     </row>
-    <row r="95" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B95" s="8"/>
       <c r="I95" s="12"/>
       <c r="J95" s="12"/>
@@ -5056,7 +5048,7 @@
       <c r="AX95" s="12"/>
       <c r="AY95" s="12"/>
     </row>
-    <row r="96" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B96" s="8"/>
       <c r="I96" s="12"/>
       <c r="J96" s="12"/>
@@ -5102,7 +5094,7 @@
       <c r="AX96" s="12"/>
       <c r="AY96" s="12"/>
     </row>
-    <row r="97" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B97" s="8"/>
       <c r="I97" s="12"/>
       <c r="J97" s="12"/>
@@ -5148,7 +5140,7 @@
       <c r="AX97" s="12"/>
       <c r="AY97" s="12"/>
     </row>
-    <row r="98" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B98" s="8"/>
       <c r="I98" s="12"/>
       <c r="J98" s="12"/>
@@ -5194,7 +5186,7 @@
       <c r="AX98" s="12"/>
       <c r="AY98" s="12"/>
     </row>
-    <row r="99" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B99" s="8"/>
       <c r="I99" s="12"/>
       <c r="J99" s="12"/>
@@ -5240,7 +5232,7 @@
       <c r="AX99" s="12"/>
       <c r="AY99" s="12"/>
     </row>
-    <row r="100" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B100" s="8"/>
       <c r="I100" s="12"/>
       <c r="J100" s="12"/>
@@ -5286,7 +5278,7 @@
       <c r="AX100" s="12"/>
       <c r="AY100" s="12"/>
     </row>
-    <row r="101" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B101" s="8"/>
       <c r="I101" s="12"/>
       <c r="J101" s="12"/>
@@ -5332,7 +5324,7 @@
       <c r="AX101" s="12"/>
       <c r="AY101" s="12"/>
     </row>
-    <row r="102" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B102" s="8"/>
       <c r="I102" s="12"/>
       <c r="J102" s="12"/>
@@ -5378,7 +5370,7 @@
       <c r="AX102" s="12"/>
       <c r="AY102" s="12"/>
     </row>
-    <row r="103" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B103" s="8"/>
       <c r="I103" s="12"/>
       <c r="J103" s="12"/>
@@ -5424,7 +5416,7 @@
       <c r="AX103" s="12"/>
       <c r="AY103" s="12"/>
     </row>
-    <row r="104" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="104" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B104" s="8"/>
       <c r="I104" s="12"/>
       <c r="J104" s="12"/>
@@ -5470,7 +5462,7 @@
       <c r="AX104" s="12"/>
       <c r="AY104" s="12"/>
     </row>
-    <row r="105" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="105" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B105" s="8"/>
       <c r="I105" s="12"/>
       <c r="J105" s="12"/>
@@ -5516,7 +5508,7 @@
       <c r="AX105" s="12"/>
       <c r="AY105" s="12"/>
     </row>
-    <row r="106" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="106" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B106" s="8"/>
       <c r="I106" s="12"/>
       <c r="J106" s="12"/>
@@ -5562,7 +5554,7 @@
       <c r="AX106" s="12"/>
       <c r="AY106" s="12"/>
     </row>
-    <row r="107" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="107" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B107" s="8"/>
       <c r="I107" s="12"/>
       <c r="J107" s="12"/>
@@ -5608,7 +5600,7 @@
       <c r="AX107" s="12"/>
       <c r="AY107" s="12"/>
     </row>
-    <row r="108" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B108" s="8"/>
       <c r="I108" s="12"/>
       <c r="J108" s="12"/>
@@ -5654,7 +5646,7 @@
       <c r="AX108" s="12"/>
       <c r="AY108" s="12"/>
     </row>
-    <row r="109" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B109" s="8"/>
       <c r="I109" s="12"/>
       <c r="J109" s="12"/>
@@ -5700,7 +5692,7 @@
       <c r="AX109" s="12"/>
       <c r="AY109" s="12"/>
     </row>
-    <row r="110" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="110" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B110" s="8"/>
       <c r="I110" s="12"/>
       <c r="J110" s="12"/>
@@ -5746,7 +5738,7 @@
       <c r="AX110" s="12"/>
       <c r="AY110" s="12"/>
     </row>
-    <row r="111" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="111" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B111" s="8"/>
       <c r="I111" s="12"/>
       <c r="J111" s="12"/>
@@ -5792,7 +5784,7 @@
       <c r="AX111" s="12"/>
       <c r="AY111" s="12"/>
     </row>
-    <row r="112" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="112" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B112" s="8"/>
       <c r="I112" s="12"/>
       <c r="J112" s="12"/>
@@ -5838,7 +5830,7 @@
       <c r="AX112" s="12"/>
       <c r="AY112" s="12"/>
     </row>
-    <row r="113" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B113" s="8"/>
       <c r="I113" s="12"/>
       <c r="J113" s="12"/>
@@ -5884,7 +5876,7 @@
       <c r="AX113" s="12"/>
       <c r="AY113" s="12"/>
     </row>
-    <row r="114" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B114" s="8"/>
       <c r="I114" s="12"/>
       <c r="J114" s="12"/>
@@ -5930,7 +5922,7 @@
       <c r="AX114" s="12"/>
       <c r="AY114" s="12"/>
     </row>
-    <row r="115" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="115" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B115" s="8"/>
       <c r="I115" s="12"/>
       <c r="J115" s="12"/>
@@ -5976,7 +5968,7 @@
       <c r="AX115" s="12"/>
       <c r="AY115" s="12"/>
     </row>
-    <row r="116" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="116" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B116" s="8"/>
       <c r="I116" s="12"/>
       <c r="J116" s="12"/>
@@ -6022,7 +6014,7 @@
       <c r="AX116" s="12"/>
       <c r="AY116" s="12"/>
     </row>
-    <row r="117" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="117" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B117" s="8"/>
       <c r="I117" s="12"/>
       <c r="J117" s="12"/>
@@ -6068,7 +6060,7 @@
       <c r="AX117" s="12"/>
       <c r="AY117" s="12"/>
     </row>
-    <row r="118" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="118" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B118" s="8"/>
       <c r="I118" s="12"/>
       <c r="J118" s="12"/>
@@ -6114,7 +6106,7 @@
       <c r="AX118" s="12"/>
       <c r="AY118" s="12"/>
     </row>
-    <row r="119" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="119" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B119" s="8"/>
       <c r="I119" s="12"/>
       <c r="J119" s="12"/>
@@ -6160,7 +6152,7 @@
       <c r="AX119" s="12"/>
       <c r="AY119" s="12"/>
     </row>
-    <row r="120" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="120" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B120" s="8"/>
       <c r="I120" s="12"/>
       <c r="J120" s="12"/>
@@ -6206,7 +6198,7 @@
       <c r="AX120" s="12"/>
       <c r="AY120" s="12"/>
     </row>
-    <row r="121" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="121" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B121" s="8"/>
       <c r="I121" s="12"/>
       <c r="J121" s="12"/>
@@ -6252,7 +6244,7 @@
       <c r="AX121" s="12"/>
       <c r="AY121" s="12"/>
     </row>
-    <row r="122" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="122" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B122" s="8"/>
       <c r="I122" s="12"/>
       <c r="J122" s="12"/>
@@ -6298,7 +6290,7 @@
       <c r="AX122" s="12"/>
       <c r="AY122" s="12"/>
     </row>
-    <row r="123" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="123" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B123" s="8"/>
       <c r="I123" s="12"/>
       <c r="J123" s="12"/>
@@ -6344,7 +6336,7 @@
       <c r="AX123" s="12"/>
       <c r="AY123" s="12"/>
     </row>
-    <row r="124" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="124" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B124" s="8"/>
       <c r="I124" s="12"/>
       <c r="J124" s="12"/>
@@ -6390,7 +6382,7 @@
       <c r="AX124" s="12"/>
       <c r="AY124" s="12"/>
     </row>
-    <row r="125" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="125" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B125" s="8"/>
       <c r="I125" s="12"/>
       <c r="J125" s="12"/>
@@ -6436,7 +6428,7 @@
       <c r="AX125" s="12"/>
       <c r="AY125" s="12"/>
     </row>
-    <row r="126" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="126" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B126" s="8"/>
       <c r="I126" s="12"/>
       <c r="J126" s="12"/>
@@ -6482,7 +6474,7 @@
       <c r="AX126" s="12"/>
       <c r="AY126" s="12"/>
     </row>
-    <row r="127" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="127" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B127" s="8"/>
       <c r="I127" s="12"/>
       <c r="J127" s="12"/>
@@ -6528,7 +6520,7 @@
       <c r="AX127" s="12"/>
       <c r="AY127" s="12"/>
     </row>
-    <row r="128" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="128" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B128" s="8"/>
       <c r="I128" s="12"/>
       <c r="J128" s="12"/>
@@ -6574,7 +6566,7 @@
       <c r="AX128" s="12"/>
       <c r="AY128" s="12"/>
     </row>
-    <row r="129" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="129" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B129" s="8"/>
       <c r="I129" s="12"/>
       <c r="J129" s="12"/>
@@ -6620,7 +6612,7 @@
       <c r="AX129" s="12"/>
       <c r="AY129" s="12"/>
     </row>
-    <row r="130" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="130" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B130" s="8"/>
       <c r="I130" s="12"/>
       <c r="J130" s="12"/>
@@ -6666,7 +6658,7 @@
       <c r="AX130" s="12"/>
       <c r="AY130" s="12"/>
     </row>
-    <row r="131" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="131" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B131" s="8"/>
       <c r="I131" s="12"/>
       <c r="J131" s="12"/>
@@ -6712,7 +6704,7 @@
       <c r="AX131" s="12"/>
       <c r="AY131" s="12"/>
     </row>
-    <row r="132" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="132" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B132" s="8"/>
       <c r="I132" s="12"/>
       <c r="J132" s="12"/>
@@ -6758,7 +6750,7 @@
       <c r="AX132" s="12"/>
       <c r="AY132" s="12"/>
     </row>
-    <row r="133" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="133" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B133" s="8"/>
       <c r="I133" s="12"/>
       <c r="J133" s="12"/>
@@ -6804,7 +6796,7 @@
       <c r="AX133" s="12"/>
       <c r="AY133" s="12"/>
     </row>
-    <row r="134" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="134" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B134" s="8"/>
       <c r="I134" s="12"/>
       <c r="J134" s="12"/>
@@ -6850,7 +6842,7 @@
       <c r="AX134" s="12"/>
       <c r="AY134" s="12"/>
     </row>
-    <row r="135" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="135" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B135" s="8"/>
       <c r="I135" s="12"/>
       <c r="J135" s="12"/>
@@ -6896,7 +6888,7 @@
       <c r="AX135" s="12"/>
       <c r="AY135" s="12"/>
     </row>
-    <row r="136" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="136" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B136" s="8"/>
       <c r="I136" s="12"/>
       <c r="J136" s="12"/>
@@ -6942,7 +6934,7 @@
       <c r="AX136" s="12"/>
       <c r="AY136" s="12"/>
     </row>
-    <row r="137" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="137" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B137" s="8"/>
       <c r="I137" s="12"/>
       <c r="J137" s="12"/>
@@ -6988,7 +6980,7 @@
       <c r="AX137" s="12"/>
       <c r="AY137" s="12"/>
     </row>
-    <row r="138" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="138" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B138" s="8"/>
       <c r="I138" s="12"/>
       <c r="J138" s="12"/>
@@ -7034,7 +7026,7 @@
       <c r="AX138" s="12"/>
       <c r="AY138" s="12"/>
     </row>
-    <row r="139" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="139" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B139" s="8"/>
       <c r="I139" s="12"/>
       <c r="J139" s="12"/>
@@ -7080,7 +7072,7 @@
       <c r="AX139" s="12"/>
       <c r="AY139" s="12"/>
     </row>
-    <row r="140" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="140" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B140" s="8"/>
       <c r="I140" s="12"/>
       <c r="J140" s="12"/>
@@ -7126,7 +7118,7 @@
       <c r="AX140" s="12"/>
       <c r="AY140" s="12"/>
     </row>
-    <row r="141" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="141" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B141" s="8"/>
       <c r="I141" s="12"/>
       <c r="J141" s="12"/>
@@ -7172,7 +7164,7 @@
       <c r="AX141" s="12"/>
       <c r="AY141" s="12"/>
     </row>
-    <row r="142" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="142" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B142" s="8"/>
       <c r="I142" s="12"/>
       <c r="J142" s="12"/>
@@ -7218,7 +7210,7 @@
       <c r="AX142" s="12"/>
       <c r="AY142" s="12"/>
     </row>
-    <row r="143" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="143" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B143" s="8"/>
       <c r="I143" s="12"/>
       <c r="J143" s="12"/>
@@ -7264,7 +7256,7 @@
       <c r="AX143" s="12"/>
       <c r="AY143" s="12"/>
     </row>
-    <row r="144" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="144" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B144" s="8"/>
       <c r="I144" s="12"/>
       <c r="J144" s="12"/>
@@ -7310,7 +7302,7 @@
       <c r="AX144" s="12"/>
       <c r="AY144" s="12"/>
     </row>
-    <row r="145" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="145" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B145" s="8"/>
       <c r="I145" s="12"/>
       <c r="J145" s="12"/>
@@ -7356,7 +7348,7 @@
       <c r="AX145" s="12"/>
       <c r="AY145" s="12"/>
     </row>
-    <row r="146" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="146" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B146" s="8"/>
       <c r="I146" s="12"/>
       <c r="J146" s="12"/>
@@ -7402,7 +7394,7 @@
       <c r="AX146" s="12"/>
       <c r="AY146" s="12"/>
     </row>
-    <row r="147" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="147" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B147" s="8"/>
       <c r="I147" s="12"/>
       <c r="J147" s="12"/>
@@ -7448,7 +7440,7 @@
       <c r="AX147" s="12"/>
       <c r="AY147" s="12"/>
     </row>
-    <row r="148" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="148" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B148" s="8"/>
       <c r="I148" s="12"/>
       <c r="J148" s="12"/>
@@ -7494,7 +7486,7 @@
       <c r="AX148" s="12"/>
       <c r="AY148" s="12"/>
     </row>
-    <row r="149" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="149" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B149" s="8"/>
       <c r="I149" s="12"/>
       <c r="J149" s="12"/>
@@ -7540,7 +7532,7 @@
       <c r="AX149" s="12"/>
       <c r="AY149" s="12"/>
     </row>
-    <row r="150" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="150" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B150" s="8"/>
       <c r="I150" s="12"/>
       <c r="J150" s="12"/>
@@ -7586,7 +7578,7 @@
       <c r="AX150" s="12"/>
       <c r="AY150" s="12"/>
     </row>
-    <row r="151" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="151" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B151" s="8"/>
       <c r="I151" s="12"/>
       <c r="J151" s="12"/>
@@ -7632,7 +7624,7 @@
       <c r="AX151" s="12"/>
       <c r="AY151" s="12"/>
     </row>
-    <row r="152" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="152" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B152" s="8"/>
       <c r="I152" s="12"/>
       <c r="J152" s="12"/>
@@ -7678,7 +7670,7 @@
       <c r="AX152" s="12"/>
       <c r="AY152" s="12"/>
     </row>
-    <row r="153" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="153" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B153" s="8"/>
       <c r="I153" s="12"/>
       <c r="J153" s="12"/>
@@ -7724,7 +7716,7 @@
       <c r="AX153" s="12"/>
       <c r="AY153" s="12"/>
     </row>
-    <row r="154" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="154" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B154" s="8"/>
       <c r="I154" s="12"/>
       <c r="J154" s="12"/>
@@ -7770,7 +7762,7 @@
       <c r="AX154" s="12"/>
       <c r="AY154" s="12"/>
     </row>
-    <row r="155" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="155" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B155" s="8"/>
       <c r="I155" s="12"/>
       <c r="J155" s="12"/>
@@ -7816,7 +7808,7 @@
       <c r="AX155" s="12"/>
       <c r="AY155" s="12"/>
     </row>
-    <row r="156" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="156" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B156" s="8"/>
       <c r="I156" s="12"/>
       <c r="J156" s="12"/>
@@ -7862,7 +7854,7 @@
       <c r="AX156" s="12"/>
       <c r="AY156" s="12"/>
     </row>
-    <row r="157" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="157" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B157" s="8"/>
       <c r="I157" s="12"/>
       <c r="J157" s="12"/>
@@ -7908,7 +7900,7 @@
       <c r="AX157" s="12"/>
       <c r="AY157" s="12"/>
     </row>
-    <row r="158" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="158" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B158" s="8"/>
       <c r="I158" s="12"/>
       <c r="J158" s="12"/>
@@ -7954,7 +7946,7 @@
       <c r="AX158" s="12"/>
       <c r="AY158" s="12"/>
     </row>
-    <row r="159" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="159" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B159" s="8"/>
       <c r="I159" s="12"/>
       <c r="J159" s="12"/>
@@ -8000,7 +7992,7 @@
       <c r="AX159" s="12"/>
       <c r="AY159" s="12"/>
     </row>
-    <row r="160" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="160" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B160" s="8"/>
       <c r="I160" s="12"/>
       <c r="J160" s="12"/>
@@ -8046,7 +8038,7 @@
       <c r="AX160" s="12"/>
       <c r="AY160" s="12"/>
     </row>
-    <row r="161" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="161" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B161" s="8"/>
       <c r="I161" s="12"/>
       <c r="J161" s="12"/>
@@ -8092,7 +8084,7 @@
       <c r="AX161" s="12"/>
       <c r="AY161" s="12"/>
     </row>
-    <row r="162" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="162" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B162" s="8"/>
       <c r="I162" s="12"/>
       <c r="J162" s="12"/>
@@ -8138,7 +8130,7 @@
       <c r="AX162" s="12"/>
       <c r="AY162" s="12"/>
     </row>
-    <row r="163" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="163" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B163" s="8"/>
       <c r="I163" s="12"/>
       <c r="J163" s="12"/>
@@ -8184,7 +8176,7 @@
       <c r="AX163" s="12"/>
       <c r="AY163" s="12"/>
     </row>
-    <row r="164" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="164" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B164" s="8"/>
       <c r="I164" s="12"/>
       <c r="J164" s="12"/>
@@ -8230,7 +8222,7 @@
       <c r="AX164" s="12"/>
       <c r="AY164" s="12"/>
     </row>
-    <row r="165" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="165" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B165" s="8"/>
       <c r="I165" s="12"/>
       <c r="J165" s="12"/>
@@ -8276,7 +8268,7 @@
       <c r="AX165" s="12"/>
       <c r="AY165" s="12"/>
     </row>
-    <row r="166" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="166" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B166" s="8"/>
       <c r="I166" s="12"/>
       <c r="J166" s="12"/>
@@ -8322,7 +8314,7 @@
       <c r="AX166" s="12"/>
       <c r="AY166" s="12"/>
     </row>
-    <row r="167" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="167" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B167" s="8"/>
       <c r="I167" s="12"/>
       <c r="J167" s="12"/>
@@ -8368,7 +8360,7 @@
       <c r="AX167" s="12"/>
       <c r="AY167" s="12"/>
     </row>
-    <row r="168" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="168" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B168" s="8"/>
       <c r="I168" s="12"/>
       <c r="J168" s="12"/>
@@ -8427,11 +8419,11 @@
       <formula1>IF(B4="","",1)</formula1>
       <formula2>IF(B4="","",99)</formula2>
     </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showErrorMessage="1" errorTitle="NAME:" error="Your name must include at least 2 non-blank characters." sqref="D2" xr:uid="{00000000-0002-0000-0000-000003000000}">
+      <formula1>OR($D$2="",LEN(SUBSTITUTE($D$2," ",""))&gt;1)</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="PREDICTION" error="Pick a winner._x000a__x000a_Enter &quot;H&quot; for the home team or &quot;V&quot; for the visiting team._x000a__x000a_If there are no teams listed in this row, then your only choice is to leave this cell blank._x000a_" sqref="F4:F9" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>IF($B4="",$AC$2:$AC$2,$AA$2:$AB$2)</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showErrorMessage="1" errorTitle="NAME:" error="Your name must include at least 2 non-blank characters." sqref="D2" xr:uid="{00000000-0002-0000-0000-000003000000}">
-      <formula1>OR($D$2="",LEN(SUBSTITUTE($D$2," ",""))&gt;1)</formula1>
     </dataValidation>
   </dataValidations>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
2020 Week 17 Final update.
</commit_message>
<xml_diff>
--- a/post_season_inputs.xlsx
+++ b/post_season_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2020 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2581E1B2-86EC-4A68-AEC7-2D9B34088114}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88CFCDAD-B16F-4A7C-A47D-D633C97D1F78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="267" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>H</t>
   </si>
@@ -62,6 +62,42 @@
   </si>
   <si>
     <t>Post Season Week 1 Input Form</t>
+  </si>
+  <si>
+    <t>Colts</t>
+  </si>
+  <si>
+    <t>Rams</t>
+  </si>
+  <si>
+    <t>Buccaneers</t>
+  </si>
+  <si>
+    <t>Ravens</t>
+  </si>
+  <si>
+    <t>Bears</t>
+  </si>
+  <si>
+    <t>Browns</t>
+  </si>
+  <si>
+    <t>Bills</t>
+  </si>
+  <si>
+    <t>Seahawks</t>
+  </si>
+  <si>
+    <t>Football Team</t>
+  </si>
+  <si>
+    <t>Titans</t>
+  </si>
+  <si>
+    <t>Saints</t>
+  </si>
+  <si>
+    <t>Steelers</t>
   </si>
 </sst>
 </file>
@@ -1165,11 +1201,11 @@
       </c>
       <c r="AA3" s="1">
         <f ca="1">MIN(AA4:AA9)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AB3" s="1">
         <f ca="1">MIN(AB4:AB9)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AC3" s="1">
         <f ca="1">MIN(AC4:AC9)</f>
@@ -1177,31 +1213,35 @@
       </c>
     </row>
     <row r="4" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="34" t="str">
+      <c r="B4" s="34">
         <f ca="1">IF(ISTEXT($C4),ROW($B4)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B4)-ROW($B$4),0)),"")</f>
-        <v/>
+        <v>1</v>
       </c>
-      <c r="C4" s="28"/>
+      <c r="C4" s="28" t="s">
+        <v>11</v>
+      </c>
       <c r="D4" s="20" t="str">
         <f ca="1">IF(B4="","","at")</f>
-        <v/>
+        <v>at</v>
       </c>
-      <c r="E4" s="29"/>
+      <c r="E4" s="29" t="s">
+        <v>17</v>
+      </c>
       <c r="F4" s="19"/>
       <c r="G4" s="20" t="str">
         <f t="shared" ref="G4:G9" ca="1" si="0">IF(B4="","","by")</f>
-        <v/>
+        <v>by</v>
       </c>
       <c r="H4" s="21"/>
       <c r="I4" s="3"/>
       <c r="J4" s="4"/>
-      <c r="AA4" s="1" t="str">
+      <c r="AA4" s="1">
         <f t="shared" ref="AA4:AA9" ca="1" si="1">IF($B4="","",IF(AND($F4&lt;&gt;"H",$F4&lt;&gt;"V"),ROW(),""))</f>
-        <v/>
+        <v>4</v>
       </c>
-      <c r="AB4" s="1" t="str">
+      <c r="AB4" s="1">
         <f t="shared" ref="AB4:AB9" ca="1" si="2">IF($B4="","",IF($H4&lt;1,ROW(),""))</f>
-        <v/>
+        <v>4</v>
       </c>
       <c r="AC4" s="1">
         <f>IF($AD4&lt;&gt;"",ROW(),"")</f>
@@ -1213,175 +1253,195 @@
       </c>
     </row>
     <row r="5" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="35" t="str">
+      <c r="B5" s="35">
         <f ca="1">IF(ISTEXT($C5),ROW($B5)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B5)-ROW($B$4),0)),"")</f>
-        <v/>
+        <v>2</v>
       </c>
-      <c r="C5" s="30"/>
+      <c r="C5" s="30" t="s">
+        <v>12</v>
+      </c>
       <c r="D5" s="23" t="str">
         <f t="shared" ref="D5" ca="1" si="3">IF(B5="","","at")</f>
-        <v/>
+        <v>at</v>
       </c>
-      <c r="E5" s="31"/>
+      <c r="E5" s="31" t="s">
+        <v>18</v>
+      </c>
       <c r="F5" s="22"/>
       <c r="G5" s="23" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v>by</v>
       </c>
       <c r="H5" s="24"/>
       <c r="I5" s="3"/>
       <c r="J5" s="5"/>
-      <c r="AA5" s="1" t="str">
+      <c r="AA5" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>5</v>
       </c>
-      <c r="AB5" s="1" t="str">
+      <c r="AB5" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>5</v>
       </c>
-      <c r="AC5" s="1" t="str">
+      <c r="AC5" s="1">
         <f t="shared" ref="AC5:AC15" ca="1" si="4">IF($AD5&lt;&gt;"",ROW(),"")</f>
-        <v/>
+        <v>5</v>
       </c>
       <c r="AD5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for the ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v/>
+        <v>Pick a winner (V or H) for the Colts at Bills (Game 1).</v>
       </c>
     </row>
     <row r="6" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="35" t="str">
+      <c r="B6" s="35">
         <f ca="1">IF(ISTEXT($C6),ROW($B6)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B6)-ROW($B$4),0)),"")</f>
-        <v/>
+        <v>3</v>
       </c>
-      <c r="C6" s="30"/>
+      <c r="C6" s="30" t="s">
+        <v>13</v>
+      </c>
       <c r="D6" s="23" t="str">
         <f t="shared" ref="D6" ca="1" si="5">IF(B6="","","at")</f>
-        <v/>
+        <v>at</v>
       </c>
-      <c r="E6" s="31"/>
+      <c r="E6" s="31" t="s">
+        <v>19</v>
+      </c>
       <c r="F6" s="22"/>
       <c r="G6" s="23" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v>by</v>
       </c>
       <c r="H6" s="24"/>
       <c r="I6" s="3"/>
       <c r="J6" s="5"/>
-      <c r="AA6" s="1" t="str">
+      <c r="AA6" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>6</v>
       </c>
-      <c r="AB6" s="1" t="str">
+      <c r="AB6" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>6</v>
       </c>
-      <c r="AC6" s="1" t="str">
+      <c r="AC6" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v>6</v>
       </c>
       <c r="AD6" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for the ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v/>
+        <v>Pick a winner (V or H) for the Colts at Bills (Game 1).</v>
       </c>
     </row>
     <row r="7" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="35" t="str">
+      <c r="B7" s="35">
         <f ca="1">IF(ISTEXT($C7),ROW($B7)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B7)-ROW($B$4),0)),"")</f>
-        <v/>
+        <v>4</v>
       </c>
-      <c r="C7" s="30"/>
+      <c r="C7" s="30" t="s">
+        <v>14</v>
+      </c>
       <c r="D7" s="23" t="str">
         <f t="shared" ref="D7:D9" ca="1" si="6">IF(B7="","","at")</f>
-        <v/>
+        <v>at</v>
       </c>
-      <c r="E7" s="31"/>
+      <c r="E7" s="31" t="s">
+        <v>20</v>
+      </c>
       <c r="F7" s="22"/>
       <c r="G7" s="23" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v>by</v>
       </c>
       <c r="H7" s="24"/>
       <c r="I7" s="3"/>
       <c r="J7" s="5"/>
-      <c r="AA7" s="1" t="str">
+      <c r="AA7" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>7</v>
       </c>
-      <c r="AB7" s="1" t="str">
+      <c r="AB7" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>7</v>
       </c>
-      <c r="AC7" s="1" t="str">
+      <c r="AC7" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v>7</v>
       </c>
       <c r="AD7" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for the ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v/>
+        <v>Pick a winner (V or H) for the Colts at Bills (Game 1).</v>
       </c>
     </row>
     <row r="8" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="35" t="str">
+      <c r="B8" s="35">
         <f ca="1">IF(ISTEXT($C8),ROW($B8)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B8)-ROW($B$4),0)),"")</f>
-        <v/>
+        <v>5</v>
       </c>
-      <c r="C8" s="30"/>
+      <c r="C8" s="30" t="s">
+        <v>15</v>
+      </c>
       <c r="D8" s="23" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v/>
+        <v>at</v>
       </c>
-      <c r="E8" s="31"/>
+      <c r="E8" s="31" t="s">
+        <v>21</v>
+      </c>
       <c r="F8" s="22"/>
       <c r="G8" s="23" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v>by</v>
       </c>
       <c r="H8" s="24"/>
       <c r="I8" s="6"/>
       <c r="J8" s="7"/>
-      <c r="AA8" s="1" t="str">
+      <c r="AA8" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>8</v>
       </c>
-      <c r="AB8" s="1" t="str">
+      <c r="AB8" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>8</v>
       </c>
-      <c r="AC8" s="1" t="str">
+      <c r="AC8" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v>8</v>
       </c>
       <c r="AD8" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE("Enter the predicted margin of victory for the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v/>
+        <v>Enter the predicted margin of victory for the Bills (Game 1).</v>
       </c>
     </row>
     <row r="9" spans="2:51" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="36" t="str">
+      <c r="B9" s="36">
         <f ca="1">IF(ISTEXT($C9),ROW($B9)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B9)-ROW($B$4),0)),"")</f>
-        <v/>
+        <v>6</v>
       </c>
-      <c r="C9" s="32"/>
+      <c r="C9" s="32" t="s">
+        <v>16</v>
+      </c>
       <c r="D9" s="26" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v/>
+        <v>at</v>
       </c>
-      <c r="E9" s="33"/>
+      <c r="E9" s="33" t="s">
+        <v>22</v>
+      </c>
       <c r="F9" s="25"/>
       <c r="G9" s="26" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v>by</v>
       </c>
       <c r="H9" s="27"/>
       <c r="I9" s="6"/>
       <c r="J9" s="7"/>
-      <c r="AA9" s="1" t="str">
+      <c r="AA9" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>9</v>
       </c>
-      <c r="AB9" s="1" t="str">
+      <c r="AB9" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>9</v>
       </c>
       <c r="AC9" s="1">
         <f ca="1">IF($AD9&lt;&gt;"",ROW(),"")</f>
@@ -1389,7 +1449,7 @@
       </c>
       <c r="AD9" s="2" t="str">
         <f ca="1">IF($H$10="",CONCATENATE("Enter your Total Points Prediction for ",OFFSET($C$4,MAX($B4:$B9)-1,0)," at ",OFFSET($E$4,MAX($B4:$B9)-1,0)," (Game ",OFFSET($B$4,MAX($B4:$B9)-1,0),") in cell H10"),"")</f>
-        <v>Enter your Total Points Prediction for Visitor at Home (Game Game) in cell H10</v>
+        <v>Enter your Total Points Prediction for Browns at Steelers (Game 6) in cell H10</v>
       </c>
     </row>
     <row r="10" spans="2:51" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1398,7 +1458,7 @@
       <c r="D10" s="17"/>
       <c r="E10" s="18" t="str">
         <f ca="1">CONCATENATE("                   Game ",MAX(B4:B9)," Total")</f>
-        <v xml:space="preserve">                   Game 0 Total</v>
+        <v xml:space="preserve">                   Game 6 Total</v>
       </c>
       <c r="F10" s="17"/>
       <c r="G10" s="37" t="s">

</xml_diff>

<commit_message>
2020 Post Season Week 1 Final update.
</commit_message>
<xml_diff>
--- a/post_season_inputs.xlsx
+++ b/post_season_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2020 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88CFCDAD-B16F-4A7C-A47D-D633C97D1F78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EAC6D5D-E551-464D-B56B-AAD52DAF63A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="267" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>H</t>
   </si>
@@ -61,12 +61,6 @@
     <t xml:space="preserve">Name:  </t>
   </si>
   <si>
-    <t>Post Season Week 1 Input Form</t>
-  </si>
-  <si>
-    <t>Colts</t>
-  </si>
-  <si>
     <t>Rams</t>
   </si>
   <si>
@@ -76,28 +70,22 @@
     <t>Ravens</t>
   </si>
   <si>
-    <t>Bears</t>
-  </si>
-  <si>
     <t>Browns</t>
   </si>
   <si>
     <t>Bills</t>
   </si>
   <si>
-    <t>Seahawks</t>
-  </si>
-  <si>
-    <t>Football Team</t>
-  </si>
-  <si>
-    <t>Titans</t>
-  </si>
-  <si>
     <t>Saints</t>
   </si>
   <si>
-    <t>Steelers</t>
+    <t>Packers</t>
+  </si>
+  <si>
+    <t>Chiefs</t>
+  </si>
+  <si>
+    <t>Post Season Week 2 Input Form</t>
   </si>
 </sst>
 </file>
@@ -1103,7 +1091,7 @@
   <sheetData>
     <row r="1" spans="2:51" s="52" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="53" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C1" s="53"/>
       <c r="D1" s="53"/>
@@ -1218,14 +1206,14 @@
         <v>1</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" s="20" t="str">
         <f ca="1">IF(B4="","","at")</f>
         <v>at</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F4" s="19"/>
       <c r="G4" s="20" t="str">
@@ -1265,7 +1253,7 @@
         <v>at</v>
       </c>
       <c r="E5" s="31" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F5" s="22"/>
       <c r="G5" s="23" t="str">
@@ -1289,7 +1277,7 @@
       </c>
       <c r="AD5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for the ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for the Colts at Bills (Game 1).</v>
+        <v>Pick a winner (V or H) for the Rams at Packers (Game 1).</v>
       </c>
     </row>
     <row r="6" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -1305,7 +1293,7 @@
         <v>at</v>
       </c>
       <c r="E6" s="31" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F6" s="22"/>
       <c r="G6" s="23" t="str">
@@ -1329,7 +1317,7 @@
       </c>
       <c r="AD6" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for the ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for the Colts at Bills (Game 1).</v>
+        <v>Pick a winner (V or H) for the Rams at Packers (Game 1).</v>
       </c>
     </row>
     <row r="7" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -1338,14 +1326,14 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D7" s="23" t="str">
         <f t="shared" ref="D7:D9" ca="1" si="6">IF(B7="","","at")</f>
         <v>at</v>
       </c>
       <c r="E7" s="31" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F7" s="22"/>
       <c r="G7" s="23" t="str">
@@ -1369,39 +1357,35 @@
       </c>
       <c r="AD7" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for the ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for the Colts at Bills (Game 1).</v>
+        <v>Pick a winner (V or H) for the Rams at Packers (Game 1).</v>
       </c>
     </row>
     <row r="8" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="35">
+      <c r="B8" s="35" t="str">
         <f ca="1">IF(ISTEXT($C8),ROW($B8)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B8)-ROW($B$4),0)),"")</f>
-        <v>5</v>
+        <v/>
       </c>
-      <c r="C8" s="30" t="s">
-        <v>15</v>
-      </c>
+      <c r="C8" s="30"/>
       <c r="D8" s="23" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>at</v>
+        <v/>
       </c>
-      <c r="E8" s="31" t="s">
-        <v>21</v>
-      </c>
+      <c r="E8" s="31"/>
       <c r="F8" s="22"/>
       <c r="G8" s="23" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>by</v>
+        <v/>
       </c>
       <c r="H8" s="24"/>
       <c r="I8" s="6"/>
       <c r="J8" s="7"/>
-      <c r="AA8" s="1">
+      <c r="AA8" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v/>
       </c>
-      <c r="AB8" s="1">
+      <c r="AB8" s="1" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v/>
       </c>
       <c r="AC8" s="1">
         <f t="shared" ca="1" si="4"/>
@@ -1409,39 +1393,35 @@
       </c>
       <c r="AD8" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE("Enter the predicted margin of victory for the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Enter the predicted margin of victory for the Bills (Game 1).</v>
+        <v>Enter the predicted margin of victory for the Packers (Game 1).</v>
       </c>
     </row>
     <row r="9" spans="2:51" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="36">
+      <c r="B9" s="36" t="str">
         <f ca="1">IF(ISTEXT($C9),ROW($B9)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B9)-ROW($B$4),0)),"")</f>
-        <v>6</v>
+        <v/>
       </c>
-      <c r="C9" s="32" t="s">
-        <v>16</v>
-      </c>
+      <c r="C9" s="32"/>
       <c r="D9" s="26" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>at</v>
+        <v/>
       </c>
-      <c r="E9" s="33" t="s">
-        <v>22</v>
-      </c>
+      <c r="E9" s="33"/>
       <c r="F9" s="25"/>
       <c r="G9" s="26" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>by</v>
+        <v/>
       </c>
       <c r="H9" s="27"/>
       <c r="I9" s="6"/>
       <c r="J9" s="7"/>
-      <c r="AA9" s="1">
+      <c r="AA9" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v/>
       </c>
-      <c r="AB9" s="1">
+      <c r="AB9" s="1" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v/>
       </c>
       <c r="AC9" s="1">
         <f ca="1">IF($AD9&lt;&gt;"",ROW(),"")</f>
@@ -1449,7 +1429,7 @@
       </c>
       <c r="AD9" s="2" t="str">
         <f ca="1">IF($H$10="",CONCATENATE("Enter your Total Points Prediction for ",OFFSET($C$4,MAX($B4:$B9)-1,0)," at ",OFFSET($E$4,MAX($B4:$B9)-1,0)," (Game ",OFFSET($B$4,MAX($B4:$B9)-1,0),") in cell H10"),"")</f>
-        <v>Enter your Total Points Prediction for Browns at Steelers (Game 6) in cell H10</v>
+        <v>Enter your Total Points Prediction for Buccaneers at Saints (Game 4) in cell H10</v>
       </c>
     </row>
     <row r="10" spans="2:51" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1458,7 +1438,7 @@
       <c r="D10" s="17"/>
       <c r="E10" s="18" t="str">
         <f ca="1">CONCATENATE("                   Game ",MAX(B4:B9)," Total")</f>
-        <v xml:space="preserve">                   Game 6 Total</v>
+        <v xml:space="preserve">                   Game 4 Total</v>
       </c>
       <c r="F10" s="17"/>
       <c r="G10" s="37" t="s">

</xml_diff>

<commit_message>
2020 Post Season Week 2 Final update.
</commit_message>
<xml_diff>
--- a/post_season_inputs.xlsx
+++ b/post_season_inputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2020 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EAC6D5D-E551-464D-B56B-AAD52DAF63A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3BB21F1-7D64-4CC8-B20E-C8C74EA187D6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="267" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" tabRatio="267" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Post Season Input Form" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>H</t>
   </si>
@@ -61,22 +61,10 @@
     <t xml:space="preserve">Name:  </t>
   </si>
   <si>
-    <t>Rams</t>
-  </si>
-  <si>
     <t>Buccaneers</t>
   </si>
   <si>
-    <t>Ravens</t>
-  </si>
-  <si>
-    <t>Browns</t>
-  </si>
-  <si>
     <t>Bills</t>
-  </si>
-  <si>
-    <t>Saints</t>
   </si>
   <si>
     <t>Packers</t>
@@ -85,7 +73,7 @@
     <t>Chiefs</t>
   </si>
   <si>
-    <t>Post Season Week 2 Input Form</t>
+    <t>Post Season Week 3 Input Form</t>
   </si>
 </sst>
 </file>
@@ -1091,7 +1079,7 @@
   <sheetData>
     <row r="1" spans="2:51" s="52" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="53" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C1" s="53"/>
       <c r="D1" s="53"/>
@@ -1213,7 +1201,7 @@
         <v>at</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F4" s="19"/>
       <c r="G4" s="20" t="str">
@@ -1246,14 +1234,14 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" s="23" t="str">
         <f t="shared" ref="D5" ca="1" si="3">IF(B5="","","at")</f>
         <v>at</v>
       </c>
       <c r="E5" s="31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F5" s="22"/>
       <c r="G5" s="23" t="str">
@@ -1277,39 +1265,35 @@
       </c>
       <c r="AD5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for the ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for the Rams at Packers (Game 1).</v>
+        <v>Pick a winner (V or H) for the Buccaneers at Packers (Game 1).</v>
       </c>
     </row>
     <row r="6" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="35">
+      <c r="B6" s="35" t="str">
         <f ca="1">IF(ISTEXT($C6),ROW($B6)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B6)-ROW($B$4),0)),"")</f>
-        <v>3</v>
+        <v/>
       </c>
-      <c r="C6" s="30" t="s">
-        <v>13</v>
-      </c>
+      <c r="C6" s="30"/>
       <c r="D6" s="23" t="str">
         <f t="shared" ref="D6" ca="1" si="5">IF(B6="","","at")</f>
-        <v>at</v>
+        <v/>
       </c>
-      <c r="E6" s="31" t="s">
-        <v>17</v>
-      </c>
+      <c r="E6" s="31"/>
       <c r="F6" s="22"/>
       <c r="G6" s="23" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>by</v>
+        <v/>
       </c>
       <c r="H6" s="24"/>
       <c r="I6" s="3"/>
       <c r="J6" s="5"/>
-      <c r="AA6" s="1">
+      <c r="AA6" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v/>
       </c>
-      <c r="AB6" s="1">
+      <c r="AB6" s="1" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v/>
       </c>
       <c r="AC6" s="1">
         <f t="shared" ca="1" si="4"/>
@@ -1317,39 +1301,35 @@
       </c>
       <c r="AD6" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for the ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for the Rams at Packers (Game 1).</v>
+        <v>Pick a winner (V or H) for the Buccaneers at Packers (Game 1).</v>
       </c>
     </row>
     <row r="7" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="35">
+      <c r="B7" s="35" t="str">
         <f ca="1">IF(ISTEXT($C7),ROW($B7)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B7)-ROW($B$4),0)),"")</f>
-        <v>4</v>
+        <v/>
       </c>
-      <c r="C7" s="30" t="s">
-        <v>11</v>
-      </c>
+      <c r="C7" s="30"/>
       <c r="D7" s="23" t="str">
         <f t="shared" ref="D7:D9" ca="1" si="6">IF(B7="","","at")</f>
-        <v>at</v>
+        <v/>
       </c>
-      <c r="E7" s="31" t="s">
-        <v>15</v>
-      </c>
+      <c r="E7" s="31"/>
       <c r="F7" s="22"/>
       <c r="G7" s="23" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>by</v>
+        <v/>
       </c>
       <c r="H7" s="24"/>
       <c r="I7" s="3"/>
       <c r="J7" s="5"/>
-      <c r="AA7" s="1">
+      <c r="AA7" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v/>
       </c>
-      <c r="AB7" s="1">
+      <c r="AB7" s="1" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>7</v>
+        <v/>
       </c>
       <c r="AC7" s="1">
         <f t="shared" ca="1" si="4"/>
@@ -1357,7 +1337,7 @@
       </c>
       <c r="AD7" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for the ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for the Rams at Packers (Game 1).</v>
+        <v>Pick a winner (V or H) for the Buccaneers at Packers (Game 1).</v>
       </c>
     </row>
     <row r="8" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -1429,7 +1409,7 @@
       </c>
       <c r="AD9" s="2" t="str">
         <f ca="1">IF($H$10="",CONCATENATE("Enter your Total Points Prediction for ",OFFSET($C$4,MAX($B4:$B9)-1,0)," at ",OFFSET($E$4,MAX($B4:$B9)-1,0)," (Game ",OFFSET($B$4,MAX($B4:$B9)-1,0),") in cell H10"),"")</f>
-        <v>Enter your Total Points Prediction for Buccaneers at Saints (Game 4) in cell H10</v>
+        <v>Enter your Total Points Prediction for Bills at Chiefs (Game 2) in cell H10</v>
       </c>
     </row>
     <row r="10" spans="2:51" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1438,7 +1418,7 @@
       <c r="D10" s="17"/>
       <c r="E10" s="18" t="str">
         <f ca="1">CONCATENATE("                   Game ",MAX(B4:B9)," Total")</f>
-        <v xml:space="preserve">                   Game 4 Total</v>
+        <v xml:space="preserve">                   Game 2 Total</v>
       </c>
       <c r="F10" s="17"/>
       <c r="G10" s="37" t="s">

</xml_diff>

<commit_message>
2020 Post Season Week 3 Final update.
</commit_message>
<xml_diff>
--- a/post_season_inputs.xlsx
+++ b/post_season_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2020 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3BB21F1-7D64-4CC8-B20E-C8C74EA187D6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB1AF6C-2FEA-488C-812D-A9FB425AD7A2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" tabRatio="267" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>H</t>
   </si>
@@ -64,16 +64,10 @@
     <t>Buccaneers</t>
   </si>
   <si>
-    <t>Bills</t>
-  </si>
-  <si>
-    <t>Packers</t>
-  </si>
-  <si>
     <t>Chiefs</t>
   </si>
   <si>
-    <t>Post Season Week 3 Input Form</t>
+    <t>Post Season Week 4 Input Form</t>
   </si>
 </sst>
 </file>
@@ -1079,7 +1073,7 @@
   <sheetData>
     <row r="1" spans="2:51" s="52" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="53" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C1" s="53"/>
       <c r="D1" s="53"/>
@@ -1194,14 +1188,14 @@
         <v>1</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D4" s="20" t="str">
         <f ca="1">IF(B4="","","at")</f>
         <v>at</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F4" s="19"/>
       <c r="G4" s="20" t="str">
@@ -1229,35 +1223,31 @@
       </c>
     </row>
     <row r="5" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="35">
+      <c r="B5" s="35" t="str">
         <f ca="1">IF(ISTEXT($C5),ROW($B5)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B5)-ROW($B$4),0)),"")</f>
-        <v>2</v>
+        <v/>
       </c>
-      <c r="C5" s="30" t="s">
-        <v>11</v>
-      </c>
+      <c r="C5" s="30"/>
       <c r="D5" s="23" t="str">
         <f t="shared" ref="D5" ca="1" si="3">IF(B5="","","at")</f>
-        <v>at</v>
+        <v/>
       </c>
-      <c r="E5" s="31" t="s">
-        <v>13</v>
-      </c>
+      <c r="E5" s="31"/>
       <c r="F5" s="22"/>
       <c r="G5" s="23" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>by</v>
+        <v/>
       </c>
       <c r="H5" s="24"/>
       <c r="I5" s="3"/>
       <c r="J5" s="5"/>
-      <c r="AA5" s="1">
+      <c r="AA5" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v/>
       </c>
-      <c r="AB5" s="1">
+      <c r="AB5" s="1" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v/>
       </c>
       <c r="AC5" s="1">
         <f t="shared" ref="AC5:AC15" ca="1" si="4">IF($AD5&lt;&gt;"",ROW(),"")</f>
@@ -1265,7 +1255,7 @@
       </c>
       <c r="AD5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for the ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for the Buccaneers at Packers (Game 1).</v>
+        <v>Pick a winner (V or H) for the Chiefs at Buccaneers (Game 1).</v>
       </c>
     </row>
     <row r="6" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -1301,7 +1291,7 @@
       </c>
       <c r="AD6" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for the ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for the Buccaneers at Packers (Game 1).</v>
+        <v>Pick a winner (V or H) for the Chiefs at Buccaneers (Game 1).</v>
       </c>
     </row>
     <row r="7" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -1337,7 +1327,7 @@
       </c>
       <c r="AD7" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for the ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for the Buccaneers at Packers (Game 1).</v>
+        <v>Pick a winner (V or H) for the Chiefs at Buccaneers (Game 1).</v>
       </c>
     </row>
     <row r="8" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -1373,7 +1363,7 @@
       </c>
       <c r="AD8" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE("Enter the predicted margin of victory for the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Enter the predicted margin of victory for the Packers (Game 1).</v>
+        <v>Enter the predicted margin of victory for the Buccaneers (Game 1).</v>
       </c>
     </row>
     <row r="9" spans="2:51" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1409,7 +1399,7 @@
       </c>
       <c r="AD9" s="2" t="str">
         <f ca="1">IF($H$10="",CONCATENATE("Enter your Total Points Prediction for ",OFFSET($C$4,MAX($B4:$B9)-1,0)," at ",OFFSET($E$4,MAX($B4:$B9)-1,0)," (Game ",OFFSET($B$4,MAX($B4:$B9)-1,0),") in cell H10"),"")</f>
-        <v>Enter your Total Points Prediction for Bills at Chiefs (Game 2) in cell H10</v>
+        <v>Enter your Total Points Prediction for Chiefs at Buccaneers (Game 1) in cell H10</v>
       </c>
     </row>
     <row r="10" spans="2:51" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1418,7 +1408,7 @@
       <c r="D10" s="17"/>
       <c r="E10" s="18" t="str">
         <f ca="1">CONCATENATE("                   Game ",MAX(B4:B9)," Total")</f>
-        <v xml:space="preserve">                   Game 2 Total</v>
+        <v xml:space="preserve">                   Game 1 Total</v>
       </c>
       <c r="F10" s="17"/>
       <c r="G10" s="37" t="s">

</xml_diff>

<commit_message>
Change references to Monday Night Total Points to Total Points.
</commit_message>
<xml_diff>
--- a/post_season_inputs.xlsx
+++ b/post_season_inputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2020 Football Pool Page\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jerry\Desktop\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB1AF6C-2FEA-488C-812D-A9FB425AD7A2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1591AC62-7664-4D00-965F-886E762A0D59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" tabRatio="267" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="267" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Post Season Input Form" sheetId="1" r:id="rId1"/>
@@ -18,10 +18,10 @@
   <definedNames>
     <definedName name="home_teams_column">'Post Season Input Form'!$E$4</definedName>
     <definedName name="input_form">'Post Season Input Form'!$B$1,'Post Season Input Form'!$D$2,'Post Season Input Form'!$C$4:$C$9,'Post Season Input Form'!$E$4:$E$9,'Post Season Input Form'!$F$4:$F$9,'Post Season Input Form'!$H$4:$H$9,'Post Season Input Form'!$H$10</definedName>
-    <definedName name="name">'Post Season Input Form'!$D$2</definedName>
+    <definedName name="player_name">'Post Season Input Form'!$D$2</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Post Season Input Form'!$B$1:$H$9</definedName>
-    <definedName name="Season_total_points">'Post Season Input Form'!#REF!</definedName>
     <definedName name="title">'Post Season Input Form'!$B$1</definedName>
+    <definedName name="total_points">'Post Season Input Form'!$H$10</definedName>
     <definedName name="visiting_teams_column">'Post Season Input Form'!$C$4</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>H</t>
   </si>
@@ -38,9 +38,6 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Points:</t>
   </si>
   <si>
     <t>Game</t>
@@ -1073,7 +1070,7 @@
   <sheetData>
     <row r="1" spans="2:51" s="52" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="53" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C1" s="53"/>
       <c r="D1" s="53"/>
@@ -1128,7 +1125,7 @@
     <row r="2" spans="2:51" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="39"/>
       <c r="C2" s="40" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" s="41"/>
       <c r="E2" s="42"/>
@@ -1148,20 +1145,20 @@
     </row>
     <row r="3" spans="2:51" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="46" t="s">
+      <c r="D3" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="47" t="s">
+      <c r="E3" s="48" t="s">
         <v>6</v>
-      </c>
-      <c r="E3" s="48" t="s">
-        <v>7</v>
       </c>
       <c r="F3" s="46"/>
       <c r="G3" s="47" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H3" s="49"/>
       <c r="I3" s="3"/>
@@ -1188,14 +1185,14 @@
         <v>1</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" s="20" t="str">
         <f ca="1">IF(B4="","","at")</f>
         <v>at</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4" s="19"/>
       <c r="G4" s="20" t="str">
@@ -1218,7 +1215,7 @@
         <v>4</v>
       </c>
       <c r="AD4" s="2" t="str">
-        <f>IF($D$2="",CONCATENATE("Enter your name in cell ",ADDRESS(ROW($D$2),COLUMN($D$2),4),"."),IF(LEN($D$2)&lt;2,"Include at least 2 non-blank characters in your name.",""))</f>
+        <f>IF(player_name="",CONCATENATE("Enter your name in cell ",ADDRESS(ROW(player_name),COLUMN(player_name),4),"."),"")</f>
         <v>Enter your name in cell D2.</v>
       </c>
     </row>
@@ -1398,21 +1395,19 @@
         <v>9</v>
       </c>
       <c r="AD9" s="2" t="str">
-        <f ca="1">IF($H$10="",CONCATENATE("Enter your Total Points Prediction for ",OFFSET($C$4,MAX($B4:$B9)-1,0)," at ",OFFSET($E$4,MAX($B4:$B9)-1,0)," (Game ",OFFSET($B$4,MAX($B4:$B9)-1,0),") in cell H10"),"")</f>
-        <v>Enter your Total Points Prediction for Chiefs at Buccaneers (Game 1) in cell H10</v>
+        <f ca="1">IF(total_points="",CONCATENATE("Enter your Total Points Prediction for ",OFFSET($C$4,MAX($B4:$B9)-1,0)," at ",OFFSET($E$4,MAX($B4:$B9)-1,0)," (Game ",OFFSET($B$4,MAX($B4:$B9)-1,0),") in cell ",ADDRESS(ROW(total_points),COLUMN(total_points),4),"."),"")</f>
+        <v>Enter your Total Points Prediction for Chiefs at Buccaneers (Game 1) in cell H10.</v>
       </c>
     </row>
     <row r="10" spans="2:51" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="16"/>
       <c r="C10" s="17"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="18" t="str">
-        <f ca="1">CONCATENATE("                   Game ",MAX(B4:B9)," Total")</f>
-        <v xml:space="preserve">                   Game 1 Total</v>
-      </c>
+      <c r="E10" s="18"/>
       <c r="F10" s="17"/>
-      <c r="G10" s="37" t="s">
-        <v>3</v>
+      <c r="G10" s="37" t="str">
+        <f ca="1">IF(J2="","Points:",CONCATENATE("Game ",MAX(B4:B9)," Total Points:  "))</f>
+        <v xml:space="preserve">Game 1 Total Points:  </v>
       </c>
       <c r="H10" s="38"/>
       <c r="I10" s="6"/>

</xml_diff>

<commit_message>
2021 Week 18 Final update.
</commit_message>
<xml_diff>
--- a/post_season_inputs.xlsx
+++ b/post_season_inputs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jerry\Desktop\Test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2021 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1591AC62-7664-4D00-965F-886E762A0D59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDE3F79D-08B3-4429-9E70-C74EB15FD094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="267" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,11 +25,20 @@
     <definedName name="visiting_teams_column">'Post Season Input Form'!$C$4</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>H</t>
   </si>
@@ -64,7 +73,37 @@
     <t>Chiefs</t>
   </si>
   <si>
-    <t>Post Season Week 4 Input Form</t>
+    <t>Raiders</t>
+  </si>
+  <si>
+    <t>Patriots</t>
+  </si>
+  <si>
+    <t>Eagles</t>
+  </si>
+  <si>
+    <t>49ers</t>
+  </si>
+  <si>
+    <t>Steelers</t>
+  </si>
+  <si>
+    <t>Cardinals</t>
+  </si>
+  <si>
+    <t>Bengals</t>
+  </si>
+  <si>
+    <t>Bills</t>
+  </si>
+  <si>
+    <t>Cowboys</t>
+  </si>
+  <si>
+    <t>Rams</t>
+  </si>
+  <si>
+    <t>Post Season Week 1 Input Form</t>
   </si>
 </sst>
 </file>
@@ -1070,7 +1109,7 @@
   <sheetData>
     <row r="1" spans="2:51" s="52" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="53" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C1" s="53"/>
       <c r="D1" s="53"/>
@@ -1185,14 +1224,14 @@
         <v>1</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D4" s="20" t="str">
         <f ca="1">IF(B4="","","at")</f>
         <v>at</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F4" s="19"/>
       <c r="G4" s="20" t="str">
@@ -1220,31 +1259,35 @@
       </c>
     </row>
     <row r="5" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="35" t="str">
+      <c r="B5" s="35">
         <f ca="1">IF(ISTEXT($C5),ROW($B5)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B5)-ROW($B$4),0)),"")</f>
-        <v/>
+        <v>2</v>
       </c>
-      <c r="C5" s="30"/>
+      <c r="C5" s="30" t="s">
+        <v>12</v>
+      </c>
       <c r="D5" s="23" t="str">
         <f t="shared" ref="D5" ca="1" si="3">IF(B5="","","at")</f>
-        <v/>
+        <v>at</v>
       </c>
-      <c r="E5" s="31"/>
+      <c r="E5" s="31" t="s">
+        <v>18</v>
+      </c>
       <c r="F5" s="22"/>
       <c r="G5" s="23" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v>by</v>
       </c>
       <c r="H5" s="24"/>
       <c r="I5" s="3"/>
       <c r="J5" s="5"/>
-      <c r="AA5" s="1" t="str">
+      <c r="AA5" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>5</v>
       </c>
-      <c r="AB5" s="1" t="str">
+      <c r="AB5" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>5</v>
       </c>
       <c r="AC5" s="1">
         <f t="shared" ref="AC5:AC15" ca="1" si="4">IF($AD5&lt;&gt;"",ROW(),"")</f>
@@ -1252,35 +1295,39 @@
       </c>
       <c r="AD5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for the ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for the Chiefs at Buccaneers (Game 1).</v>
+        <v>Pick a winner (V or H) for the Raiders at Bengals (Game 1).</v>
       </c>
     </row>
     <row r="6" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="35" t="str">
+      <c r="B6" s="35">
         <f ca="1">IF(ISTEXT($C6),ROW($B6)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B6)-ROW($B$4),0)),"")</f>
-        <v/>
+        <v>3</v>
       </c>
-      <c r="C6" s="30"/>
+      <c r="C6" s="30" t="s">
+        <v>13</v>
+      </c>
       <c r="D6" s="23" t="str">
         <f t="shared" ref="D6" ca="1" si="5">IF(B6="","","at")</f>
-        <v/>
+        <v>at</v>
       </c>
-      <c r="E6" s="31"/>
+      <c r="E6" s="31" t="s">
+        <v>9</v>
+      </c>
       <c r="F6" s="22"/>
       <c r="G6" s="23" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v>by</v>
       </c>
       <c r="H6" s="24"/>
       <c r="I6" s="3"/>
       <c r="J6" s="5"/>
-      <c r="AA6" s="1" t="str">
+      <c r="AA6" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>6</v>
       </c>
-      <c r="AB6" s="1" t="str">
+      <c r="AB6" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>6</v>
       </c>
       <c r="AC6" s="1">
         <f t="shared" ca="1" si="4"/>
@@ -1288,35 +1335,39 @@
       </c>
       <c r="AD6" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for the ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for the Chiefs at Buccaneers (Game 1).</v>
+        <v>Pick a winner (V or H) for the Raiders at Bengals (Game 1).</v>
       </c>
     </row>
     <row r="7" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="35" t="str">
+      <c r="B7" s="35">
         <f ca="1">IF(ISTEXT($C7),ROW($B7)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B7)-ROW($B$4),0)),"")</f>
-        <v/>
+        <v>4</v>
       </c>
-      <c r="C7" s="30"/>
+      <c r="C7" s="30" t="s">
+        <v>14</v>
+      </c>
       <c r="D7" s="23" t="str">
         <f t="shared" ref="D7:D9" ca="1" si="6">IF(B7="","","at")</f>
-        <v/>
+        <v>at</v>
       </c>
-      <c r="E7" s="31"/>
+      <c r="E7" s="31" t="s">
+        <v>19</v>
+      </c>
       <c r="F7" s="22"/>
       <c r="G7" s="23" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v>by</v>
       </c>
       <c r="H7" s="24"/>
       <c r="I7" s="3"/>
       <c r="J7" s="5"/>
-      <c r="AA7" s="1" t="str">
+      <c r="AA7" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>7</v>
       </c>
-      <c r="AB7" s="1" t="str">
+      <c r="AB7" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>7</v>
       </c>
       <c r="AC7" s="1">
         <f t="shared" ca="1" si="4"/>
@@ -1324,35 +1375,39 @@
       </c>
       <c r="AD7" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for the ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for the Chiefs at Buccaneers (Game 1).</v>
+        <v>Pick a winner (V or H) for the Raiders at Bengals (Game 1).</v>
       </c>
     </row>
     <row r="8" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="35" t="str">
+      <c r="B8" s="35">
         <f ca="1">IF(ISTEXT($C8),ROW($B8)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B8)-ROW($B$4),0)),"")</f>
-        <v/>
+        <v>5</v>
       </c>
-      <c r="C8" s="30"/>
+      <c r="C8" s="30" t="s">
+        <v>15</v>
+      </c>
       <c r="D8" s="23" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v/>
+        <v>at</v>
       </c>
-      <c r="E8" s="31"/>
+      <c r="E8" s="31" t="s">
+        <v>10</v>
+      </c>
       <c r="F8" s="22"/>
       <c r="G8" s="23" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v>by</v>
       </c>
       <c r="H8" s="24"/>
       <c r="I8" s="6"/>
       <c r="J8" s="7"/>
-      <c r="AA8" s="1" t="str">
+      <c r="AA8" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>8</v>
       </c>
-      <c r="AB8" s="1" t="str">
+      <c r="AB8" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>8</v>
       </c>
       <c r="AC8" s="1">
         <f t="shared" ca="1" si="4"/>
@@ -1360,35 +1415,39 @@
       </c>
       <c r="AD8" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE("Enter the predicted margin of victory for the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Enter the predicted margin of victory for the Buccaneers (Game 1).</v>
+        <v>Enter the predicted margin of victory for the Bengals (Game 1).</v>
       </c>
     </row>
     <row r="9" spans="2:51" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="36" t="str">
+      <c r="B9" s="36">
         <f ca="1">IF(ISTEXT($C9),ROW($B9)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B9)-ROW($B$4),0)),"")</f>
-        <v/>
+        <v>6</v>
       </c>
-      <c r="C9" s="32"/>
+      <c r="C9" s="32" t="s">
+        <v>16</v>
+      </c>
       <c r="D9" s="26" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v/>
+        <v>at</v>
       </c>
-      <c r="E9" s="33"/>
+      <c r="E9" s="33" t="s">
+        <v>20</v>
+      </c>
       <c r="F9" s="25"/>
       <c r="G9" s="26" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v>by</v>
       </c>
       <c r="H9" s="27"/>
       <c r="I9" s="6"/>
       <c r="J9" s="7"/>
-      <c r="AA9" s="1" t="str">
+      <c r="AA9" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>9</v>
       </c>
-      <c r="AB9" s="1" t="str">
+      <c r="AB9" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>9</v>
       </c>
       <c r="AC9" s="1">
         <f ca="1">IF($AD9&lt;&gt;"",ROW(),"")</f>
@@ -1396,7 +1455,7 @@
       </c>
       <c r="AD9" s="2" t="str">
         <f ca="1">IF(total_points="",CONCATENATE("Enter your Total Points Prediction for ",OFFSET($C$4,MAX($B4:$B9)-1,0)," at ",OFFSET($E$4,MAX($B4:$B9)-1,0)," (Game ",OFFSET($B$4,MAX($B4:$B9)-1,0),") in cell ",ADDRESS(ROW(total_points),COLUMN(total_points),4),"."),"")</f>
-        <v>Enter your Total Points Prediction for Chiefs at Buccaneers (Game 1) in cell H10.</v>
+        <v>Enter your Total Points Prediction for Cardinals at Rams (Game 6) in cell H10.</v>
       </c>
     </row>
     <row r="10" spans="2:51" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1407,7 +1466,7 @@
       <c r="F10" s="17"/>
       <c r="G10" s="37" t="str">
         <f ca="1">IF(J2="","Points:",CONCATENATE("Game ",MAX(B4:B9)," Total Points:  "))</f>
-        <v xml:space="preserve">Game 1 Total Points:  </v>
+        <v xml:space="preserve">Game 6 Total Points:  </v>
       </c>
       <c r="H10" s="38"/>
       <c r="I10" s="6"/>

</xml_diff>

<commit_message>
2021 Post Season Week 1 Final update.
</commit_message>
<xml_diff>
--- a/post_season_inputs.xlsx
+++ b/post_season_inputs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2021 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDE3F79D-08B3-4429-9E70-C74EB15FD094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E0B012-905A-42C8-BF6F-05672580F3C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="267" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>H</t>
   </si>
@@ -73,22 +73,7 @@
     <t>Chiefs</t>
   </si>
   <si>
-    <t>Raiders</t>
-  </si>
-  <si>
-    <t>Patriots</t>
-  </si>
-  <si>
-    <t>Eagles</t>
-  </si>
-  <si>
     <t>49ers</t>
-  </si>
-  <si>
-    <t>Steelers</t>
-  </si>
-  <si>
-    <t>Cardinals</t>
   </si>
   <si>
     <t>Bengals</t>
@@ -97,13 +82,16 @@
     <t>Bills</t>
   </si>
   <si>
-    <t>Cowboys</t>
-  </si>
-  <si>
     <t>Rams</t>
   </si>
   <si>
-    <t>Post Season Week 1 Input Form</t>
+    <t>Titans</t>
+  </si>
+  <si>
+    <t>Packers</t>
+  </si>
+  <si>
+    <t>Post Season Week 2 Input Form</t>
   </si>
 </sst>
 </file>
@@ -1109,7 +1097,7 @@
   <sheetData>
     <row r="1" spans="2:51" s="52" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="53" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C1" s="53"/>
       <c r="D1" s="53"/>
@@ -1224,14 +1212,14 @@
         <v>1</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" s="20" t="str">
         <f ca="1">IF(B4="","","at")</f>
         <v>at</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F4" s="19"/>
       <c r="G4" s="20" t="str">
@@ -1264,14 +1252,14 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" s="23" t="str">
         <f t="shared" ref="D5" ca="1" si="3">IF(B5="","","at")</f>
         <v>at</v>
       </c>
       <c r="E5" s="31" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F5" s="22"/>
       <c r="G5" s="23" t="str">
@@ -1295,7 +1283,7 @@
       </c>
       <c r="AD5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for the ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for the Raiders at Bengals (Game 1).</v>
+        <v>Pick a winner (V or H) for the Bengals at Titans (Game 1).</v>
       </c>
     </row>
     <row r="6" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -1304,7 +1292,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D6" s="23" t="str">
         <f t="shared" ref="D6" ca="1" si="5">IF(B6="","","at")</f>
@@ -1335,7 +1323,7 @@
       </c>
       <c r="AD6" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for the ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for the Raiders at Bengals (Game 1).</v>
+        <v>Pick a winner (V or H) for the Bengals at Titans (Game 1).</v>
       </c>
     </row>
     <row r="7" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -1344,14 +1332,14 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D7" s="23" t="str">
         <f t="shared" ref="D7:D9" ca="1" si="6">IF(B7="","","at")</f>
         <v>at</v>
       </c>
       <c r="E7" s="31" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="F7" s="22"/>
       <c r="G7" s="23" t="str">
@@ -1375,39 +1363,35 @@
       </c>
       <c r="AD7" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for the ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for the Raiders at Bengals (Game 1).</v>
+        <v>Pick a winner (V or H) for the Bengals at Titans (Game 1).</v>
       </c>
     </row>
     <row r="8" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="35">
+      <c r="B8" s="35" t="str">
         <f ca="1">IF(ISTEXT($C8),ROW($B8)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B8)-ROW($B$4),0)),"")</f>
-        <v>5</v>
+        <v/>
       </c>
-      <c r="C8" s="30" t="s">
-        <v>15</v>
-      </c>
+      <c r="C8" s="30"/>
       <c r="D8" s="23" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>at</v>
+        <v/>
       </c>
-      <c r="E8" s="31" t="s">
-        <v>10</v>
-      </c>
+      <c r="E8" s="31"/>
       <c r="F8" s="22"/>
       <c r="G8" s="23" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>by</v>
+        <v/>
       </c>
       <c r="H8" s="24"/>
       <c r="I8" s="6"/>
       <c r="J8" s="7"/>
-      <c r="AA8" s="1">
+      <c r="AA8" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v/>
       </c>
-      <c r="AB8" s="1">
+      <c r="AB8" s="1" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v/>
       </c>
       <c r="AC8" s="1">
         <f t="shared" ca="1" si="4"/>
@@ -1415,39 +1399,35 @@
       </c>
       <c r="AD8" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE("Enter the predicted margin of victory for the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Enter the predicted margin of victory for the Bengals (Game 1).</v>
+        <v>Enter the predicted margin of victory for the Titans (Game 1).</v>
       </c>
     </row>
     <row r="9" spans="2:51" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="36">
+      <c r="B9" s="36" t="str">
         <f ca="1">IF(ISTEXT($C9),ROW($B9)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B9)-ROW($B$4),0)),"")</f>
-        <v>6</v>
+        <v/>
       </c>
-      <c r="C9" s="32" t="s">
-        <v>16</v>
-      </c>
+      <c r="C9" s="32"/>
       <c r="D9" s="26" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>at</v>
+        <v/>
       </c>
-      <c r="E9" s="33" t="s">
-        <v>20</v>
-      </c>
+      <c r="E9" s="33"/>
       <c r="F9" s="25"/>
       <c r="G9" s="26" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>by</v>
+        <v/>
       </c>
       <c r="H9" s="27"/>
       <c r="I9" s="6"/>
       <c r="J9" s="7"/>
-      <c r="AA9" s="1">
+      <c r="AA9" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v/>
       </c>
-      <c r="AB9" s="1">
+      <c r="AB9" s="1" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v/>
       </c>
       <c r="AC9" s="1">
         <f ca="1">IF($AD9&lt;&gt;"",ROW(),"")</f>
@@ -1455,7 +1435,7 @@
       </c>
       <c r="AD9" s="2" t="str">
         <f ca="1">IF(total_points="",CONCATENATE("Enter your Total Points Prediction for ",OFFSET($C$4,MAX($B4:$B9)-1,0)," at ",OFFSET($E$4,MAX($B4:$B9)-1,0)," (Game ",OFFSET($B$4,MAX($B4:$B9)-1,0),") in cell ",ADDRESS(ROW(total_points),COLUMN(total_points),4),"."),"")</f>
-        <v>Enter your Total Points Prediction for Cardinals at Rams (Game 6) in cell H10.</v>
+        <v>Enter your Total Points Prediction for Bills at Chiefs (Game 4) in cell H10.</v>
       </c>
     </row>
     <row r="10" spans="2:51" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1466,7 +1446,7 @@
       <c r="F10" s="17"/>
       <c r="G10" s="37" t="str">
         <f ca="1">IF(J2="","Points:",CONCATENATE("Game ",MAX(B4:B9)," Total Points:  "))</f>
-        <v xml:space="preserve">Game 6 Total Points:  </v>
+        <v xml:space="preserve">Game 4 Total Points:  </v>
       </c>
       <c r="H10" s="38"/>
       <c r="I10" s="6"/>

</xml_diff>

<commit_message>
2021 Post Season Week 2 Final update.
</commit_message>
<xml_diff>
--- a/post_season_inputs.xlsx
+++ b/post_season_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2021 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E0B012-905A-42C8-BF6F-05672580F3C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70324EC1-1753-4015-9F4D-69127E711482}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="267" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" tabRatio="267" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Post Season Input Form" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>H</t>
   </si>
@@ -67,9 +67,6 @@
     <t xml:space="preserve">Name:  </t>
   </si>
   <si>
-    <t>Buccaneers</t>
-  </si>
-  <si>
     <t>Chiefs</t>
   </si>
   <si>
@@ -79,19 +76,10 @@
     <t>Bengals</t>
   </si>
   <si>
-    <t>Bills</t>
-  </si>
-  <si>
     <t>Rams</t>
   </si>
   <si>
-    <t>Titans</t>
-  </si>
-  <si>
-    <t>Packers</t>
-  </si>
-  <si>
-    <t>Post Season Week 2 Input Form</t>
+    <t>Post Season Week 3 Input Form</t>
   </si>
 </sst>
 </file>
@@ -1097,7 +1085,7 @@
   <sheetData>
     <row r="1" spans="2:51" s="52" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="53" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C1" s="53"/>
       <c r="D1" s="53"/>
@@ -1212,14 +1200,14 @@
         <v>1</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" s="20" t="str">
         <f ca="1">IF(B4="","","at")</f>
         <v>at</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F4" s="19"/>
       <c r="G4" s="20" t="str">
@@ -1252,14 +1240,14 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" s="23" t="str">
         <f t="shared" ref="D5" ca="1" si="3">IF(B5="","","at")</f>
         <v>at</v>
       </c>
       <c r="E5" s="31" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F5" s="22"/>
       <c r="G5" s="23" t="str">
@@ -1283,39 +1271,35 @@
       </c>
       <c r="AD5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for the ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for the Bengals at Titans (Game 1).</v>
+        <v>Pick a winner (V or H) for the Bengals at Chiefs (Game 1).</v>
       </c>
     </row>
     <row r="6" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="35">
+      <c r="B6" s="35" t="str">
         <f ca="1">IF(ISTEXT($C6),ROW($B6)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B6)-ROW($B$4),0)),"")</f>
-        <v>3</v>
+        <v/>
       </c>
-      <c r="C6" s="30" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="30"/>
       <c r="D6" s="23" t="str">
         <f t="shared" ref="D6" ca="1" si="5">IF(B6="","","at")</f>
-        <v>at</v>
+        <v/>
       </c>
-      <c r="E6" s="31" t="s">
-        <v>9</v>
-      </c>
+      <c r="E6" s="31"/>
       <c r="F6" s="22"/>
       <c r="G6" s="23" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>by</v>
+        <v/>
       </c>
       <c r="H6" s="24"/>
       <c r="I6" s="3"/>
       <c r="J6" s="5"/>
-      <c r="AA6" s="1">
+      <c r="AA6" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v/>
       </c>
-      <c r="AB6" s="1">
+      <c r="AB6" s="1" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v/>
       </c>
       <c r="AC6" s="1">
         <f t="shared" ca="1" si="4"/>
@@ -1323,39 +1307,35 @@
       </c>
       <c r="AD6" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for the ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for the Bengals at Titans (Game 1).</v>
+        <v>Pick a winner (V or H) for the Bengals at Chiefs (Game 1).</v>
       </c>
     </row>
     <row r="7" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="35">
+      <c r="B7" s="35" t="str">
         <f ca="1">IF(ISTEXT($C7),ROW($B7)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B7)-ROW($B$4),0)),"")</f>
-        <v>4</v>
+        <v/>
       </c>
-      <c r="C7" s="30" t="s">
-        <v>13</v>
-      </c>
+      <c r="C7" s="30"/>
       <c r="D7" s="23" t="str">
         <f t="shared" ref="D7:D9" ca="1" si="6">IF(B7="","","at")</f>
-        <v>at</v>
+        <v/>
       </c>
-      <c r="E7" s="31" t="s">
-        <v>10</v>
-      </c>
+      <c r="E7" s="31"/>
       <c r="F7" s="22"/>
       <c r="G7" s="23" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>by</v>
+        <v/>
       </c>
       <c r="H7" s="24"/>
       <c r="I7" s="3"/>
       <c r="J7" s="5"/>
-      <c r="AA7" s="1">
+      <c r="AA7" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v/>
       </c>
-      <c r="AB7" s="1">
+      <c r="AB7" s="1" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>7</v>
+        <v/>
       </c>
       <c r="AC7" s="1">
         <f t="shared" ca="1" si="4"/>
@@ -1363,7 +1343,7 @@
       </c>
       <c r="AD7" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for the ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for the Bengals at Titans (Game 1).</v>
+        <v>Pick a winner (V or H) for the Bengals at Chiefs (Game 1).</v>
       </c>
     </row>
     <row r="8" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -1399,7 +1379,7 @@
       </c>
       <c r="AD8" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE("Enter the predicted margin of victory for the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Enter the predicted margin of victory for the Titans (Game 1).</v>
+        <v>Enter the predicted margin of victory for the Chiefs (Game 1).</v>
       </c>
     </row>
     <row r="9" spans="2:51" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1435,7 +1415,7 @@
       </c>
       <c r="AD9" s="2" t="str">
         <f ca="1">IF(total_points="",CONCATENATE("Enter your Total Points Prediction for ",OFFSET($C$4,MAX($B4:$B9)-1,0)," at ",OFFSET($E$4,MAX($B4:$B9)-1,0)," (Game ",OFFSET($B$4,MAX($B4:$B9)-1,0),") in cell ",ADDRESS(ROW(total_points),COLUMN(total_points),4),"."),"")</f>
-        <v>Enter your Total Points Prediction for Bills at Chiefs (Game 4) in cell H10.</v>
+        <v>Enter your Total Points Prediction for 49ers at Rams (Game 2) in cell H10.</v>
       </c>
     </row>
     <row r="10" spans="2:51" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1446,7 +1426,7 @@
       <c r="F10" s="17"/>
       <c r="G10" s="37" t="str">
         <f ca="1">IF(J2="","Points:",CONCATENATE("Game ",MAX(B4:B9)," Total Points:  "))</f>
-        <v xml:space="preserve">Game 4 Total Points:  </v>
+        <v xml:space="preserve">Game 2 Total Points:  </v>
       </c>
       <c r="H10" s="38"/>
       <c r="I10" s="6"/>

</xml_diff>

<commit_message>
2021 Post Season Week 3 Final update.
</commit_message>
<xml_diff>
--- a/post_season_inputs.xlsx
+++ b/post_season_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2021 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70324EC1-1753-4015-9F4D-69127E711482}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63ABA758-DAE3-4B22-BE4E-2D3F2B3FDAE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" tabRatio="267" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="267" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Post Season Input Form" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>H</t>
   </si>
@@ -67,19 +67,13 @@
     <t xml:space="preserve">Name:  </t>
   </si>
   <si>
-    <t>Chiefs</t>
-  </si>
-  <si>
-    <t>49ers</t>
-  </si>
-  <si>
     <t>Bengals</t>
   </si>
   <si>
     <t>Rams</t>
   </si>
   <si>
-    <t>Post Season Week 3 Input Form</t>
+    <t>Post Season Week 4 Input Form</t>
   </si>
 </sst>
 </file>
@@ -1085,7 +1079,7 @@
   <sheetData>
     <row r="1" spans="2:51" s="52" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="53" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C1" s="53"/>
       <c r="D1" s="53"/>
@@ -1200,7 +1194,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" s="20" t="str">
         <f ca="1">IF(B4="","","at")</f>
@@ -1235,35 +1229,31 @@
       </c>
     </row>
     <row r="5" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="35">
+      <c r="B5" s="35" t="str">
         <f ca="1">IF(ISTEXT($C5),ROW($B5)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B5)-ROW($B$4),0)),"")</f>
-        <v>2</v>
+        <v/>
       </c>
-      <c r="C5" s="30" t="s">
-        <v>10</v>
-      </c>
+      <c r="C5" s="30"/>
       <c r="D5" s="23" t="str">
         <f t="shared" ref="D5" ca="1" si="3">IF(B5="","","at")</f>
-        <v>at</v>
+        <v/>
       </c>
-      <c r="E5" s="31" t="s">
-        <v>12</v>
-      </c>
+      <c r="E5" s="31"/>
       <c r="F5" s="22"/>
       <c r="G5" s="23" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>by</v>
+        <v/>
       </c>
       <c r="H5" s="24"/>
       <c r="I5" s="3"/>
       <c r="J5" s="5"/>
-      <c r="AA5" s="1">
+      <c r="AA5" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v/>
       </c>
-      <c r="AB5" s="1">
+      <c r="AB5" s="1" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v/>
       </c>
       <c r="AC5" s="1">
         <f t="shared" ref="AC5:AC15" ca="1" si="4">IF($AD5&lt;&gt;"",ROW(),"")</f>
@@ -1271,7 +1261,7 @@
       </c>
       <c r="AD5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for the ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for the Bengals at Chiefs (Game 1).</v>
+        <v>Pick a winner (V or H) for the Rams at Bengals (Game 1).</v>
       </c>
     </row>
     <row r="6" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -1307,7 +1297,7 @@
       </c>
       <c r="AD6" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for the ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for the Bengals at Chiefs (Game 1).</v>
+        <v>Pick a winner (V or H) for the Rams at Bengals (Game 1).</v>
       </c>
     </row>
     <row r="7" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -1343,7 +1333,7 @@
       </c>
       <c r="AD7" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for the ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for the Bengals at Chiefs (Game 1).</v>
+        <v>Pick a winner (V or H) for the Rams at Bengals (Game 1).</v>
       </c>
     </row>
     <row r="8" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -1379,7 +1369,7 @@
       </c>
       <c r="AD8" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE("Enter the predicted margin of victory for the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Enter the predicted margin of victory for the Chiefs (Game 1).</v>
+        <v>Enter the predicted margin of victory for the Bengals (Game 1).</v>
       </c>
     </row>
     <row r="9" spans="2:51" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1415,7 +1405,7 @@
       </c>
       <c r="AD9" s="2" t="str">
         <f ca="1">IF(total_points="",CONCATENATE("Enter your Total Points Prediction for ",OFFSET($C$4,MAX($B4:$B9)-1,0)," at ",OFFSET($E$4,MAX($B4:$B9)-1,0)," (Game ",OFFSET($B$4,MAX($B4:$B9)-1,0),") in cell ",ADDRESS(ROW(total_points),COLUMN(total_points),4),"."),"")</f>
-        <v>Enter your Total Points Prediction for 49ers at Rams (Game 2) in cell H10.</v>
+        <v>Enter your Total Points Prediction for Rams at Bengals (Game 1) in cell H10.</v>
       </c>
     </row>
     <row r="10" spans="2:51" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1426,7 +1416,7 @@
       <c r="F10" s="17"/>
       <c r="G10" s="37" t="str">
         <f ca="1">IF(J2="","Points:",CONCATENATE("Game ",MAX(B4:B9)," Total Points:  "))</f>
-        <v xml:space="preserve">Game 2 Total Points:  </v>
+        <v xml:space="preserve">Game 1 Total Points:  </v>
       </c>
       <c r="H10" s="38"/>
       <c r="I10" s="6"/>

</xml_diff>

<commit_message>
2022 Post Season Week 1 Final update.
</commit_message>
<xml_diff>
--- a/post_season_inputs.xlsx
+++ b/post_season_inputs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2022 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC153DC1-D52E-4E01-862B-7F73E41DDF20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE7395D5-DFF5-4AA9-91BD-7FA05CE65507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="267" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,20 +25,11 @@
     <definedName name="visiting_teams_column">'Post Season Input Form'!$C$4</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>H</t>
   </si>
@@ -70,19 +61,7 @@
     <t>Bengals</t>
   </si>
   <si>
-    <t>Seahawks</t>
-  </si>
-  <si>
-    <t>Chargers</t>
-  </si>
-  <si>
-    <t>Dolphins</t>
-  </si>
-  <si>
     <t>Giants</t>
-  </si>
-  <si>
-    <t>Ravens</t>
   </si>
   <si>
     <t>Cowboys</t>
@@ -97,13 +76,13 @@
     <t>Bills</t>
   </si>
   <si>
-    <t>Vikings</t>
+    <t>Chiefs</t>
   </si>
   <si>
-    <t>Buccaneers</t>
+    <t>Eagles</t>
   </si>
   <si>
-    <t>Post Season Week 1 Input Form</t>
+    <t>Post Season Week 2 Input Form</t>
   </si>
 </sst>
 </file>
@@ -1100,7 +1079,7 @@
   <sheetData>
     <row r="1" spans="2:51" s="49" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="50" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C1" s="50"/>
       <c r="D1" s="50"/>
@@ -1215,14 +1194,14 @@
         <v>1</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D4" s="17" t="str">
         <f ca="1">IF(B4="","","at")</f>
         <v>at</v>
       </c>
       <c r="E4" s="26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F4" s="16"/>
       <c r="G4" s="17" t="str">
@@ -1255,14 +1234,14 @@
         <v>2</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" s="20" t="str">
         <f t="shared" ref="D5" ca="1" si="3">IF(B5="","","at")</f>
         <v>at</v>
       </c>
       <c r="E5" s="28" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F5" s="19"/>
       <c r="G5" s="20" t="str">
@@ -1286,7 +1265,7 @@
       </c>
       <c r="AD5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for the ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for the Seahawks at 49ers (Game 1).</v>
+        <v>Pick a winner (V or H) for the Jaguars at Chiefs (Game 1).</v>
       </c>
     </row>
     <row r="6" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -1295,14 +1274,14 @@
         <v>3</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D6" s="20" t="str">
         <f t="shared" ref="D6" ca="1" si="5">IF(B6="","","at")</f>
         <v>at</v>
       </c>
       <c r="E6" s="28" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F6" s="19"/>
       <c r="G6" s="20" t="str">
@@ -1326,7 +1305,7 @@
       </c>
       <c r="AD6" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for the ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for the Seahawks at 49ers (Game 1).</v>
+        <v>Pick a winner (V or H) for the Jaguars at Chiefs (Game 1).</v>
       </c>
     </row>
     <row r="7" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -1335,14 +1314,14 @@
         <v>4</v>
       </c>
       <c r="C7" s="27" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D7" s="20" t="str">
         <f t="shared" ref="D7:D9" ca="1" si="6">IF(B7="","","at")</f>
         <v>at</v>
       </c>
       <c r="E7" s="28" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F7" s="19"/>
       <c r="G7" s="20" t="str">
@@ -1366,39 +1345,35 @@
       </c>
       <c r="AD7" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for the ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for the Seahawks at 49ers (Game 1).</v>
+        <v>Pick a winner (V or H) for the Jaguars at Chiefs (Game 1).</v>
       </c>
     </row>
     <row r="8" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="32">
+      <c r="B8" s="32" t="str">
         <f ca="1">IF(ISTEXT($C8),ROW($B8)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B8)-ROW($B$4),0)),"")</f>
-        <v>5</v>
-      </c>
-      <c r="C8" s="27" t="s">
-        <v>14</v>
-      </c>
+        <v/>
+      </c>
+      <c r="C8" s="27"/>
       <c r="D8" s="20" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>at</v>
-      </c>
-      <c r="E8" s="28" t="s">
-        <v>9</v>
-      </c>
+        <v/>
+      </c>
+      <c r="E8" s="28"/>
       <c r="F8" s="19"/>
       <c r="G8" s="20" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>by</v>
+        <v/>
       </c>
       <c r="H8" s="21"/>
       <c r="I8" s="5"/>
       <c r="J8" s="6"/>
-      <c r="AA8" s="1">
+      <c r="AA8" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="AB8" s="1">
+        <v/>
+      </c>
+      <c r="AB8" s="1" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v/>
       </c>
       <c r="AC8" s="1">
         <f t="shared" ca="1" si="4"/>
@@ -1406,39 +1381,35 @@
       </c>
       <c r="AD8" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE("Enter the predicted margin of victory for the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Enter the predicted margin of victory for the 49ers (Game 1).</v>
+        <v>Enter the predicted margin of victory for the Chiefs (Game 1).</v>
       </c>
     </row>
     <row r="9" spans="2:51" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="33">
+      <c r="B9" s="33" t="str">
         <f ca="1">IF(ISTEXT($C9),ROW($B9)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B9)-ROW($B$4),0)),"")</f>
-        <v>6</v>
-      </c>
-      <c r="C9" s="29" t="s">
-        <v>15</v>
-      </c>
+        <v/>
+      </c>
+      <c r="C9" s="29"/>
       <c r="D9" s="23" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>at</v>
-      </c>
-      <c r="E9" s="30" t="s">
-        <v>20</v>
-      </c>
+        <v/>
+      </c>
+      <c r="E9" s="30"/>
       <c r="F9" s="22"/>
       <c r="G9" s="23" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>by</v>
+        <v/>
       </c>
       <c r="H9" s="24"/>
       <c r="I9" s="5"/>
       <c r="J9" s="6"/>
-      <c r="AA9" s="1">
+      <c r="AA9" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="AB9" s="1">
+        <v/>
+      </c>
+      <c r="AB9" s="1" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v/>
       </c>
       <c r="AC9" s="1">
         <f ca="1">IF($AD9&lt;&gt;"",ROW(),"")</f>
@@ -1446,7 +1417,7 @@
       </c>
       <c r="AD9" s="2" t="str">
         <f ca="1">IF(total_points="",CONCATENATE("Enter your Total Points Prediction for ",OFFSET($C$4,MAX($B4:$B9)-1,0)," at ",OFFSET($E$4,MAX($B4:$B9)-1,0)," (Game ",OFFSET($B$4,MAX($B4:$B9)-1,0),") in cell ",ADDRESS(ROW(total_points),COLUMN(total_points),4),"."),"")</f>
-        <v>Enter your Total Points Prediction for Cowboys at Buccaneers (Game 6) in cell H10.</v>
+        <v>Enter your Total Points Prediction for Cowboys at 49ers (Game 4) in cell H10.</v>
       </c>
     </row>
     <row r="10" spans="2:51" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1457,7 +1428,7 @@
       <c r="F10" s="14"/>
       <c r="G10" s="34" t="str">
         <f ca="1">IF(J2="","Points:",CONCATENATE("Game ",MAX(B4:B9)," Total Points:  "))</f>
-        <v xml:space="preserve">Game 6 Total Points:  </v>
+        <v xml:space="preserve">Game 4 Total Points:  </v>
       </c>
       <c r="H10" s="35"/>
       <c r="I10" s="5"/>

</xml_diff>

<commit_message>
2022 Post Season Week 2 Final update.
</commit_message>
<xml_diff>
--- a/post_season_inputs.xlsx
+++ b/post_season_inputs.xlsx
@@ -8,14 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2022 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE7395D5-DFF5-4AA9-91BD-7FA05CE65507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6733E69C-3520-4162-96A4-76D6C62C2B94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="267" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" tabRatio="267" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Post Season Input Form" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="all_games">'Post Season Input Form'!$4:$9</definedName>
+    <definedName name="game_1">'Post Season Input Form'!$4:$4</definedName>
+    <definedName name="game_2">'Post Season Input Form'!$5:$5</definedName>
+    <definedName name="game_3">'Post Season Input Form'!$6:$6</definedName>
+    <definedName name="game_4">'Post Season Input Form'!$7:$7</definedName>
+    <definedName name="game_5">'Post Season Input Form'!$8:$8</definedName>
+    <definedName name="game_6">'Post Season Input Form'!$9:$9</definedName>
     <definedName name="home_teams_column">'Post Season Input Form'!$E$4</definedName>
     <definedName name="input_form">'Post Season Input Form'!$B$1,'Post Season Input Form'!$D$2,'Post Season Input Form'!$C$4:$C$9,'Post Season Input Form'!$E$4:$E$9,'Post Season Input Form'!$F$4:$F$9,'Post Season Input Form'!$H$4:$H$9,'Post Season Input Form'!$H$10</definedName>
     <definedName name="player_name">'Post Season Input Form'!$D$2</definedName>
@@ -29,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>H</t>
   </si>
@@ -61,19 +68,7 @@
     <t>Bengals</t>
   </si>
   <si>
-    <t>Giants</t>
-  </si>
-  <si>
-    <t>Cowboys</t>
-  </si>
-  <si>
     <t>49ers</t>
-  </si>
-  <si>
-    <t>Jaguars</t>
-  </si>
-  <si>
-    <t>Bills</t>
   </si>
   <si>
     <t>Chiefs</t>
@@ -82,7 +77,7 @@
     <t>Eagles</t>
   </si>
   <si>
-    <t>Post Season Week 2 Input Form</t>
+    <t>Post Season Week 3 Input Form</t>
   </si>
 </sst>
 </file>
@@ -207,7 +202,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -253,30 +248,8 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom style="medium">
         <color indexed="64"/>
@@ -377,14 +350,29 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color rgb="FFD3D3D3"/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFD3D3D3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
       </right>
       <top style="thin">
         <color rgb="FFD3D3D3"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
+      <bottom style="thin">
+        <color rgb="FFD3D3D3"/>
       </bottom>
       <diagonal/>
     </border>
@@ -392,26 +380,11 @@
       <left style="thin">
         <color rgb="FFD3D3D3"/>
       </left>
-      <right style="thin">
-        <color rgb="FFD3D3D3"/>
+      <right style="medium">
+        <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color rgb="FFD3D3D3"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFD3D3D3"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFD3D3D3"/>
+      <top style="medium">
+        <color indexed="64"/>
       </top>
       <bottom style="medium">
         <color indexed="64"/>
@@ -425,57 +398,49 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
+      <top style="thin">
+        <color rgb="FFD3D3D3"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFD3D3D3"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
+      <right style="thin">
+        <color rgb="FFD3D3D3"/>
       </right>
       <top style="thin">
         <color rgb="FFD3D3D3"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFD3D3D3"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFD3D3D3"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FFD3D3D3"/>
       </left>
+      <right style="thin">
+        <color rgb="FFD3D3D3"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFD3D3D3"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFD3D3D3"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
+      <top style="thin">
+        <color rgb="FFD3D3D3"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -518,79 +483,47 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -637,7 +570,39 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1077,9 +1042,9 @@
     <col min="53" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:51" s="49" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:51" s="39" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="50" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C1" s="50"/>
       <c r="D1" s="50"/>
@@ -1087,60 +1052,60 @@
       <c r="F1" s="50"/>
       <c r="G1" s="50"/>
       <c r="H1" s="50"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
-      <c r="N1" s="47"/>
-      <c r="O1" s="47"/>
-      <c r="P1" s="47"/>
-      <c r="Q1" s="47"/>
-      <c r="R1" s="47"/>
-      <c r="S1" s="47"/>
-      <c r="T1" s="47"/>
-      <c r="U1" s="47"/>
-      <c r="V1" s="47"/>
-      <c r="W1" s="47"/>
-      <c r="X1" s="47"/>
-      <c r="Y1" s="47"/>
-      <c r="Z1" s="47"/>
-      <c r="AA1" s="47"/>
-      <c r="AB1" s="47"/>
-      <c r="AC1" s="47"/>
-      <c r="AD1" s="48"/>
-      <c r="AE1" s="47"/>
-      <c r="AF1" s="47"/>
-      <c r="AG1" s="47"/>
-      <c r="AH1" s="47"/>
-      <c r="AI1" s="47"/>
-      <c r="AJ1" s="47"/>
-      <c r="AK1" s="47"/>
-      <c r="AL1" s="47"/>
-      <c r="AM1" s="47"/>
-      <c r="AN1" s="47"/>
-      <c r="AO1" s="48"/>
-      <c r="AP1" s="47"/>
-      <c r="AQ1" s="47"/>
-      <c r="AR1" s="47"/>
-      <c r="AS1" s="47"/>
-      <c r="AT1" s="47"/>
-      <c r="AU1" s="47"/>
-      <c r="AV1" s="47"/>
-      <c r="AW1" s="47"/>
-      <c r="AX1" s="47"/>
-      <c r="AY1" s="47"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
+      <c r="Q1" s="37"/>
+      <c r="R1" s="37"/>
+      <c r="S1" s="37"/>
+      <c r="T1" s="37"/>
+      <c r="U1" s="37"/>
+      <c r="V1" s="37"/>
+      <c r="W1" s="37"/>
+      <c r="X1" s="37"/>
+      <c r="Y1" s="37"/>
+      <c r="Z1" s="37"/>
+      <c r="AA1" s="37"/>
+      <c r="AB1" s="37"/>
+      <c r="AC1" s="37"/>
+      <c r="AD1" s="38"/>
+      <c r="AE1" s="37"/>
+      <c r="AF1" s="37"/>
+      <c r="AG1" s="37"/>
+      <c r="AH1" s="37"/>
+      <c r="AI1" s="37"/>
+      <c r="AJ1" s="37"/>
+      <c r="AK1" s="37"/>
+      <c r="AL1" s="37"/>
+      <c r="AM1" s="37"/>
+      <c r="AN1" s="37"/>
+      <c r="AO1" s="38"/>
+      <c r="AP1" s="37"/>
+      <c r="AQ1" s="37"/>
+      <c r="AR1" s="37"/>
+      <c r="AS1" s="37"/>
+      <c r="AT1" s="37"/>
+      <c r="AU1" s="37"/>
+      <c r="AV1" s="37"/>
+      <c r="AW1" s="37"/>
+      <c r="AX1" s="37"/>
+      <c r="AY1" s="37"/>
     </row>
     <row r="2" spans="2:51" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="36"/>
-      <c r="C2" s="37" t="s">
+      <c r="B2" s="26"/>
+      <c r="C2" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="38"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="41"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="31"/>
       <c r="J2" s="11" t="str">
         <f ca="1">IF(COUNTIF($AA$3:$AC$3,"&gt;0"),"Input Form Error:","")</f>
         <v>Input Form Error:</v>
@@ -1153,23 +1118,23 @@
       </c>
     </row>
     <row r="3" spans="2:51" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="43" t="s">
+      <c r="C3" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="44" t="s">
+      <c r="D3" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="45" t="s">
+      <c r="E3" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="43"/>
-      <c r="G3" s="44" t="s">
+      <c r="F3" s="33"/>
+      <c r="G3" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="46"/>
+      <c r="H3" s="36"/>
       <c r="I3" s="3"/>
       <c r="J3" s="12" t="str">
         <f ca="1">IF($AC$3&gt;0,OFFSET($AD$4,$AC$3-ROW($B$4),0),"")</f>
@@ -1189,26 +1154,26 @@
       </c>
     </row>
     <row r="4" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="31">
+      <c r="B4" s="23">
         <f ca="1">IF(ISTEXT($C4),ROW($B4)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B4)-ROW($B$4),0)),"")</f>
         <v>1</v>
       </c>
-      <c r="C4" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="17" t="str">
+      <c r="C4" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="14" t="str">
         <f ca="1">IF(B4="","","at")</f>
         <v>at</v>
       </c>
-      <c r="E4" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="16"/>
-      <c r="G4" s="17" t="str">
+      <c r="E4" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="13"/>
+      <c r="G4" s="14" t="str">
         <f t="shared" ref="G4:G9" ca="1" si="0">IF(B4="","","by")</f>
         <v>by</v>
       </c>
-      <c r="H4" s="18"/>
+      <c r="H4" s="15"/>
       <c r="I4" s="3"/>
       <c r="J4" s="4"/>
       <c r="AA4" s="1">
@@ -1228,27 +1193,27 @@
         <v>Enter your name in cell D2.</v>
       </c>
     </row>
-    <row r="5" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="32">
+    <row r="5" spans="2:51" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="24">
         <f ca="1">IF(ISTEXT($C5),ROW($B5)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B5)-ROW($B$4),0)),"")</f>
         <v>2</v>
       </c>
-      <c r="C5" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="20" t="str">
+      <c r="C5" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="17" t="str">
         <f t="shared" ref="D5" ca="1" si="3">IF(B5="","","at")</f>
         <v>at</v>
       </c>
-      <c r="E5" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="19"/>
-      <c r="G5" s="20" t="str">
+      <c r="E5" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="16"/>
+      <c r="G5" s="17" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>by</v>
       </c>
-      <c r="H5" s="21"/>
+      <c r="H5" s="18"/>
       <c r="I5" s="3"/>
       <c r="J5" s="2"/>
       <c r="AA5" s="1">
@@ -1265,39 +1230,35 @@
       </c>
       <c r="AD5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for the ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for the Jaguars at Chiefs (Game 1).</v>
-      </c>
-    </row>
-    <row r="6" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="32">
+        <v>Pick a winner (V or H) for the 49ers at Eagles (Game 1).</v>
+      </c>
+    </row>
+    <row r="6" spans="2:51" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="24" t="str">
         <f ca="1">IF(ISTEXT($C6),ROW($B6)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B6)-ROW($B$4),0)),"")</f>
-        <v>3</v>
-      </c>
-      <c r="C6" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="20" t="str">
+        <v/>
+      </c>
+      <c r="C6" s="21"/>
+      <c r="D6" s="17" t="str">
         <f t="shared" ref="D6" ca="1" si="5">IF(B6="","","at")</f>
-        <v>at</v>
-      </c>
-      <c r="E6" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="19"/>
-      <c r="G6" s="20" t="str">
+        <v/>
+      </c>
+      <c r="E6" s="22"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="17" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>by</v>
-      </c>
-      <c r="H6" s="21"/>
+        <v/>
+      </c>
+      <c r="H6" s="18"/>
       <c r="I6" s="3"/>
       <c r="J6" s="2"/>
-      <c r="AA6" s="1">
+      <c r="AA6" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="AB6" s="1">
+        <v/>
+      </c>
+      <c r="AB6" s="1" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v/>
       </c>
       <c r="AC6" s="1">
         <f t="shared" ca="1" si="4"/>
@@ -1305,39 +1266,35 @@
       </c>
       <c r="AD6" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for the ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for the Jaguars at Chiefs (Game 1).</v>
-      </c>
-    </row>
-    <row r="7" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="32">
+        <v>Pick a winner (V or H) for the 49ers at Eagles (Game 1).</v>
+      </c>
+    </row>
+    <row r="7" spans="2:51" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="24" t="str">
         <f ca="1">IF(ISTEXT($C7),ROW($B7)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B7)-ROW($B$4),0)),"")</f>
-        <v>4</v>
-      </c>
-      <c r="C7" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="20" t="str">
+        <v/>
+      </c>
+      <c r="C7" s="21"/>
+      <c r="D7" s="17" t="str">
         <f t="shared" ref="D7:D9" ca="1" si="6">IF(B7="","","at")</f>
-        <v>at</v>
-      </c>
-      <c r="E7" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="19"/>
-      <c r="G7" s="20" t="str">
+        <v/>
+      </c>
+      <c r="E7" s="22"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="17" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>by</v>
-      </c>
-      <c r="H7" s="21"/>
+        <v/>
+      </c>
+      <c r="H7" s="18"/>
       <c r="I7" s="3"/>
       <c r="J7" s="2"/>
-      <c r="AA7" s="1">
+      <c r="AA7" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="AB7" s="1">
+        <v/>
+      </c>
+      <c r="AB7" s="1" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>7</v>
+        <v/>
       </c>
       <c r="AC7" s="1">
         <f t="shared" ca="1" si="4"/>
@@ -1345,26 +1302,26 @@
       </c>
       <c r="AD7" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for the ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for the Jaguars at Chiefs (Game 1).</v>
-      </c>
-    </row>
-    <row r="8" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="32" t="str">
+        <v>Pick a winner (V or H) for the 49ers at Eagles (Game 1).</v>
+      </c>
+    </row>
+    <row r="8" spans="2:51" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="24" t="str">
         <f ca="1">IF(ISTEXT($C8),ROW($B8)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B8)-ROW($B$4),0)),"")</f>
         <v/>
       </c>
-      <c r="C8" s="27"/>
-      <c r="D8" s="20" t="str">
+      <c r="C8" s="21"/>
+      <c r="D8" s="17" t="str">
         <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
-      <c r="E8" s="28"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="20" t="str">
+      <c r="E8" s="22"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="17" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
-      <c r="H8" s="21"/>
+      <c r="H8" s="18"/>
       <c r="I8" s="5"/>
       <c r="J8" s="6"/>
       <c r="AA8" s="1" t="str">
@@ -1381,26 +1338,26 @@
       </c>
       <c r="AD8" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE("Enter the predicted margin of victory for the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Enter the predicted margin of victory for the Chiefs (Game 1).</v>
-      </c>
-    </row>
-    <row r="9" spans="2:51" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="33" t="str">
+        <v>Enter the predicted margin of victory for the Eagles (Game 1).</v>
+      </c>
+    </row>
+    <row r="9" spans="2:51" ht="20.100000000000001" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="40" t="str">
         <f ca="1">IF(ISTEXT($C9),ROW($B9)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B9)-ROW($B$4),0)),"")</f>
         <v/>
       </c>
-      <c r="C9" s="29"/>
-      <c r="D9" s="23" t="str">
+      <c r="C9" s="41"/>
+      <c r="D9" s="42" t="str">
         <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
-      <c r="E9" s="30"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="23" t="str">
+      <c r="E9" s="43"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="42" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
-      <c r="H9" s="24"/>
+      <c r="H9" s="45"/>
       <c r="I9" s="5"/>
       <c r="J9" s="6"/>
       <c r="AA9" s="1" t="str">
@@ -1417,20 +1374,20 @@
       </c>
       <c r="AD9" s="2" t="str">
         <f ca="1">IF(total_points="",CONCATENATE("Enter your Total Points Prediction for ",OFFSET($C$4,MAX($B4:$B9)-1,0)," at ",OFFSET($E$4,MAX($B4:$B9)-1,0)," (Game ",OFFSET($B$4,MAX($B4:$B9)-1,0),") in cell ",ADDRESS(ROW(total_points),COLUMN(total_points),4),"."),"")</f>
-        <v>Enter your Total Points Prediction for Cowboys at 49ers (Game 4) in cell H10.</v>
+        <v>Enter your Total Points Prediction for Bengals at Chiefs (Game 2) in cell H10.</v>
       </c>
     </row>
     <row r="10" spans="2:51" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="13"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="34" t="str">
+      <c r="B10" s="46"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="49" t="str">
         <f ca="1">IF(J2="","Points:",CONCATENATE("Game ",MAX(B4:B9)," Total Points:  "))</f>
-        <v xml:space="preserve">Game 4 Total Points:  </v>
-      </c>
-      <c r="H10" s="35"/>
+        <v xml:space="preserve">Game 2 Total Points:  </v>
+      </c>
+      <c r="H10" s="25"/>
       <c r="I10" s="5"/>
       <c r="J10" s="6"/>
     </row>

</xml_diff>

<commit_message>
2022 Post Season Week 3 Final update.
</commit_message>
<xml_diff>
--- a/post_season_inputs.xlsx
+++ b/post_season_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2022 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6733E69C-3520-4162-96A4-76D6C62C2B94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1A1978F-9C4E-4E8A-B5EC-B4F70A941047}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" tabRatio="267" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>H</t>
   </si>
@@ -65,19 +65,13 @@
     <t xml:space="preserve">Name:  </t>
   </si>
   <si>
-    <t>Bengals</t>
-  </si>
-  <si>
-    <t>49ers</t>
-  </si>
-  <si>
     <t>Chiefs</t>
   </si>
   <si>
     <t>Eagles</t>
   </si>
   <si>
-    <t>Post Season Week 3 Input Form</t>
+    <t>Post Season Week 4 Input Form</t>
   </si>
 </sst>
 </file>
@@ -1044,7 +1038,7 @@
   <sheetData>
     <row r="1" spans="2:51" s="39" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="50" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C1" s="50"/>
       <c r="D1" s="50"/>
@@ -1153,20 +1147,20 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:51" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="23">
         <f ca="1">IF(ISTEXT($C4),ROW($B4)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B4)-ROW($B$4),0)),"")</f>
         <v>1</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4" s="14" t="str">
         <f ca="1">IF(B4="","","at")</f>
         <v>at</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F4" s="13"/>
       <c r="G4" s="14" t="str">
@@ -1193,36 +1187,32 @@
         <v>Enter your name in cell D2.</v>
       </c>
     </row>
-    <row r="5" spans="2:51" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="24">
+    <row r="5" spans="2:51" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="24" t="str">
         <f ca="1">IF(ISTEXT($C5),ROW($B5)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B5)-ROW($B$4),0)),"")</f>
-        <v>2</v>
-      </c>
-      <c r="C5" s="21" t="s">
-        <v>9</v>
-      </c>
+        <v/>
+      </c>
+      <c r="C5" s="21"/>
       <c r="D5" s="17" t="str">
         <f t="shared" ref="D5" ca="1" si="3">IF(B5="","","at")</f>
-        <v>at</v>
-      </c>
-      <c r="E5" s="22" t="s">
-        <v>11</v>
-      </c>
+        <v/>
+      </c>
+      <c r="E5" s="22"/>
       <c r="F5" s="16"/>
       <c r="G5" s="17" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>by</v>
+        <v/>
       </c>
       <c r="H5" s="18"/>
       <c r="I5" s="3"/>
       <c r="J5" s="2"/>
-      <c r="AA5" s="1">
+      <c r="AA5" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="AB5" s="1">
+        <v/>
+      </c>
+      <c r="AB5" s="1" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v/>
       </c>
       <c r="AC5" s="1">
         <f t="shared" ref="AC5:AC15" ca="1" si="4">IF($AD5&lt;&gt;"",ROW(),"")</f>
@@ -1230,7 +1220,7 @@
       </c>
       <c r="AD5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for the ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for the 49ers at Eagles (Game 1).</v>
+        <v>Pick a winner (V or H) for the Chiefs at Eagles (Game 1).</v>
       </c>
     </row>
     <row r="6" spans="2:51" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -1266,7 +1256,7 @@
       </c>
       <c r="AD6" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for the ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for the 49ers at Eagles (Game 1).</v>
+        <v>Pick a winner (V or H) for the Chiefs at Eagles (Game 1).</v>
       </c>
     </row>
     <row r="7" spans="2:51" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -1302,7 +1292,7 @@
       </c>
       <c r="AD7" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for the ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for the 49ers at Eagles (Game 1).</v>
+        <v>Pick a winner (V or H) for the Chiefs at Eagles (Game 1).</v>
       </c>
     </row>
     <row r="8" spans="2:51" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -1374,7 +1364,7 @@
       </c>
       <c r="AD9" s="2" t="str">
         <f ca="1">IF(total_points="",CONCATENATE("Enter your Total Points Prediction for ",OFFSET($C$4,MAX($B4:$B9)-1,0)," at ",OFFSET($E$4,MAX($B4:$B9)-1,0)," (Game ",OFFSET($B$4,MAX($B4:$B9)-1,0),") in cell ",ADDRESS(ROW(total_points),COLUMN(total_points),4),"."),"")</f>
-        <v>Enter your Total Points Prediction for Bengals at Chiefs (Game 2) in cell H10.</v>
+        <v>Enter your Total Points Prediction for Chiefs at Eagles (Game 1) in cell H10.</v>
       </c>
     </row>
     <row r="10" spans="2:51" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1385,7 +1375,7 @@
       <c r="F10" s="47"/>
       <c r="G10" s="49" t="str">
         <f ca="1">IF(J2="","Points:",CONCATENATE("Game ",MAX(B4:B9)," Total Points:  "))</f>
-        <v xml:space="preserve">Game 2 Total Points:  </v>
+        <v xml:space="preserve">Game 1 Total Points:  </v>
       </c>
       <c r="H10" s="25"/>
       <c r="I10" s="5"/>

</xml_diff>